<commit_message>
Data Entry in Habitat data. Modify habitat data and create summary CSV, write code to merge this into metadata.
</commit_message>
<xml_diff>
--- a/raw_data/arabuko_sokoke_11.xlsx
+++ b/raw_data/arabuko_sokoke_11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesseborden/Dropbox/Research/research_projects/arabuko_sokoke/ASF/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DC61AB-FCB7-DB4F-B5D9-4578F49D2289}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D2A4F9-90B3-744E-8004-F944F9DDFD1E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="460" windowWidth="26380" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="780" windowWidth="27800" windowHeight="16600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Herps" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17789" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17679" uniqueCount="885">
   <si>
     <t>ind_numb</t>
   </si>
@@ -41962,8 +41962,8 @@
   <dimension ref="A1:AA649"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C146" sqref="C146"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -49968,17 +49968,17 @@
       <c r="B146" t="s">
         <v>774</v>
       </c>
-      <c r="C146" t="s">
-        <v>30</v>
-      </c>
-      <c r="D146" t="s">
-        <v>30</v>
-      </c>
-      <c r="E146" t="s">
-        <v>30</v>
-      </c>
-      <c r="F146" t="s">
-        <v>30</v>
+      <c r="C146">
+        <v>10</v>
+      </c>
+      <c r="D146">
+        <v>11</v>
+      </c>
+      <c r="E146">
+        <v>17</v>
+      </c>
+      <c r="F146">
+        <v>11</v>
       </c>
       <c r="G146">
         <v>2</v>
@@ -50013,27 +50013,27 @@
       </c>
       <c r="Q146">
         <f t="shared" ref="Q146" si="137">((SUM(C146:F146))/4)*1.04</f>
-        <v>0</v>
+        <v>12.74</v>
       </c>
       <c r="R146">
         <f t="shared" ref="R146" si="138">((SUM(C148:F148))/4)*1.04</f>
-        <v>0</v>
+        <v>13.26</v>
       </c>
       <c r="S146">
         <f t="shared" ref="S146" si="139">((SUM(C150:F150))/4)*1.04</f>
-        <v>0</v>
+        <v>23.400000000000002</v>
       </c>
       <c r="T146">
         <f t="shared" ref="T146" si="140">((SUM(C152:F152))/4)*1.04</f>
-        <v>0</v>
+        <v>20.54</v>
       </c>
       <c r="U146">
         <f t="shared" ref="U146" si="141">((SUM(C154:F154))/4)*1.04</f>
-        <v>0</v>
+        <v>15.08</v>
       </c>
       <c r="V146">
         <f t="shared" ref="V146" si="142">((SUM(C146:F154))/20)*1.04</f>
-        <v>0</v>
+        <v>17.004000000000001</v>
       </c>
       <c r="W146">
         <f t="shared" ref="W146" si="143">(SUM(G146:H154))/10</f>
@@ -50112,17 +50112,17 @@
       <c r="B148" t="s">
         <v>777</v>
       </c>
-      <c r="C148" t="s">
-        <v>30</v>
-      </c>
-      <c r="D148" t="s">
-        <v>30</v>
-      </c>
-      <c r="E148" t="s">
-        <v>30</v>
-      </c>
-      <c r="F148" t="s">
-        <v>30</v>
+      <c r="C148">
+        <v>8</v>
+      </c>
+      <c r="D148">
+        <v>11</v>
+      </c>
+      <c r="E148">
+        <v>26</v>
+      </c>
+      <c r="F148">
+        <v>6</v>
       </c>
       <c r="G148">
         <v>1</v>
@@ -50212,17 +50212,17 @@
       <c r="B150" t="s">
         <v>779</v>
       </c>
-      <c r="C150" t="s">
-        <v>30</v>
-      </c>
-      <c r="D150" t="s">
-        <v>30</v>
-      </c>
-      <c r="E150" t="s">
-        <v>30</v>
-      </c>
-      <c r="F150" t="s">
-        <v>30</v>
+      <c r="C150">
+        <v>23</v>
+      </c>
+      <c r="D150">
+        <v>19</v>
+      </c>
+      <c r="E150">
+        <v>22</v>
+      </c>
+      <c r="F150">
+        <v>26</v>
       </c>
       <c r="G150">
         <v>5</v>
@@ -50312,17 +50312,17 @@
       <c r="B152" t="s">
         <v>781</v>
       </c>
-      <c r="C152" t="s">
-        <v>30</v>
-      </c>
-      <c r="D152" t="s">
-        <v>30</v>
-      </c>
-      <c r="E152" t="s">
-        <v>30</v>
-      </c>
-      <c r="F152" t="s">
-        <v>30</v>
+      <c r="C152">
+        <v>19</v>
+      </c>
+      <c r="D152">
+        <v>13</v>
+      </c>
+      <c r="E152">
+        <v>20</v>
+      </c>
+      <c r="F152">
+        <v>27</v>
       </c>
       <c r="G152">
         <v>5</v>
@@ -50412,17 +50412,17 @@
       <c r="B154" t="s">
         <v>783</v>
       </c>
-      <c r="C154" t="s">
-        <v>30</v>
-      </c>
-      <c r="D154" t="s">
-        <v>30</v>
-      </c>
-      <c r="E154" t="s">
-        <v>30</v>
-      </c>
-      <c r="F154" t="s">
-        <v>30</v>
+      <c r="C154">
+        <v>28</v>
+      </c>
+      <c r="D154">
+        <v>18</v>
+      </c>
+      <c r="E154">
+        <v>9</v>
+      </c>
+      <c r="F154">
+        <v>3</v>
       </c>
       <c r="G154">
         <v>1</v>
@@ -50462,17 +50462,17 @@
       <c r="B155" t="s">
         <v>774</v>
       </c>
-      <c r="C155" t="s">
-        <v>30</v>
-      </c>
-      <c r="D155" t="s">
-        <v>30</v>
-      </c>
-      <c r="E155" t="s">
-        <v>30</v>
-      </c>
-      <c r="F155" t="s">
-        <v>30</v>
+      <c r="C155">
+        <v>15</v>
+      </c>
+      <c r="D155">
+        <v>12</v>
+      </c>
+      <c r="E155">
+        <v>15</v>
+      </c>
+      <c r="F155">
+        <v>13</v>
       </c>
       <c r="G155">
         <v>5</v>
@@ -50502,47 +50502,46 @@
         <v>29</v>
       </c>
       <c r="P155">
-        <f t="shared" ref="P155" si="147">M155*10</f>
+        <f>M155*10</f>
         <v>120</v>
       </c>
       <c r="Q155">
-        <f t="shared" ref="Q155" si="148">((SUM(C155:F155))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="Q155" si="147">((SUM(C155:F155))/4)*1.04</f>
+        <v>14.3</v>
       </c>
       <c r="R155">
-        <f t="shared" ref="R155" si="149">((SUM(C157:F157))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="R155" si="148">((SUM(C157:F157))/4)*1.04</f>
+        <v>14.040000000000001</v>
       </c>
       <c r="S155">
-        <f t="shared" ref="S155" si="150">((SUM(C159:F159))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="S155" si="149">((SUM(C159:F159))/4)*1.04</f>
+        <v>8.84</v>
       </c>
       <c r="T155">
-        <f t="shared" ref="T155" si="151">((SUM(C161:F161))/4)*1.04</f>
-        <v>0</v>
-      </c>
-      <c r="U155">
-        <f t="shared" ref="U155" si="152">((SUM(C163:F163))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="T155" si="150">((SUM(C161:F161))/4)*1.04</f>
+        <v>15.08</v>
+      </c>
+      <c r="U155" t="s">
+        <v>30</v>
       </c>
       <c r="V155">
-        <f t="shared" ref="V155" si="153">((SUM(C155:F163))/20)*1.04</f>
-        <v>0</v>
+        <f>((SUM(C155:F163))/16)*1.04</f>
+        <v>13.065000000000001</v>
       </c>
       <c r="W155">
-        <f t="shared" ref="W155" si="154">(SUM(G155:H163))/10</f>
+        <f t="shared" ref="W155" si="151">(SUM(G155:H163))/10</f>
         <v>3.05</v>
       </c>
       <c r="X155">
-        <f t="shared" ref="X155" si="155">(SUM(I155:I163))/5</f>
+        <f t="shared" ref="X155" si="152">(SUM(I155:I163))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y155">
-        <f t="shared" ref="Y155" si="156">SUM(K155:K163)-Z155</f>
+        <f t="shared" ref="Y155" si="153">SUM(K155:K163)-Z155</f>
         <v>6</v>
       </c>
       <c r="Z155">
-        <f t="shared" ref="Z155" si="157">SUM(L155:L163)</f>
+        <f t="shared" ref="Z155" si="154">SUM(L155:L163)</f>
         <v>7</v>
       </c>
       <c r="AA155" t="s">
@@ -50606,17 +50605,17 @@
       <c r="B157" t="s">
         <v>777</v>
       </c>
-      <c r="C157" t="s">
-        <v>30</v>
-      </c>
-      <c r="D157" t="s">
-        <v>30</v>
-      </c>
-      <c r="E157" t="s">
-        <v>30</v>
-      </c>
-      <c r="F157" t="s">
-        <v>30</v>
+      <c r="C157">
+        <v>16</v>
+      </c>
+      <c r="D157">
+        <v>7</v>
+      </c>
+      <c r="E157">
+        <v>12</v>
+      </c>
+      <c r="F157">
+        <v>19</v>
       </c>
       <c r="G157">
         <v>1</v>
@@ -50706,17 +50705,17 @@
       <c r="B159" t="s">
         <v>779</v>
       </c>
-      <c r="C159" t="s">
-        <v>30</v>
-      </c>
-      <c r="D159" t="s">
-        <v>30</v>
-      </c>
-      <c r="E159" t="s">
-        <v>30</v>
-      </c>
-      <c r="F159" t="s">
-        <v>30</v>
+      <c r="C159">
+        <v>2</v>
+      </c>
+      <c r="D159">
+        <v>4</v>
+      </c>
+      <c r="E159">
+        <v>25</v>
+      </c>
+      <c r="F159">
+        <v>3</v>
       </c>
       <c r="G159">
         <v>1</v>
@@ -50806,17 +50805,17 @@
       <c r="B161" t="s">
         <v>781</v>
       </c>
-      <c r="C161" t="s">
-        <v>30</v>
-      </c>
-      <c r="D161" t="s">
-        <v>30</v>
-      </c>
-      <c r="E161" t="s">
-        <v>30</v>
-      </c>
-      <c r="F161" t="s">
-        <v>30</v>
+      <c r="C161">
+        <v>16</v>
+      </c>
+      <c r="D161">
+        <v>17</v>
+      </c>
+      <c r="E161">
+        <v>20</v>
+      </c>
+      <c r="F161">
+        <v>5</v>
       </c>
       <c r="G161">
         <v>1</v>
@@ -50956,17 +50955,17 @@
       <c r="B164" t="s">
         <v>774</v>
       </c>
-      <c r="C164" t="s">
-        <v>30</v>
-      </c>
-      <c r="D164" t="s">
-        <v>30</v>
-      </c>
-      <c r="E164" t="s">
-        <v>30</v>
-      </c>
-      <c r="F164" t="s">
-        <v>30</v>
+      <c r="C164">
+        <v>23</v>
+      </c>
+      <c r="D164">
+        <v>17</v>
+      </c>
+      <c r="E164">
+        <v>25</v>
+      </c>
+      <c r="F164">
+        <v>29</v>
       </c>
       <c r="G164">
         <v>20</v>
@@ -50996,47 +50995,46 @@
         <v>29</v>
       </c>
       <c r="P164">
-        <f t="shared" ref="P164" si="158">M164*10</f>
+        <f t="shared" ref="P164" si="155">M164*10</f>
         <v>130</v>
       </c>
       <c r="Q164">
-        <f t="shared" ref="Q164" si="159">((SUM(C164:F164))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="Q164" si="156">((SUM(C164:F164))/4)*1.04</f>
+        <v>24.44</v>
       </c>
       <c r="R164">
-        <f t="shared" ref="R164" si="160">((SUM(C166:F166))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="R164" si="157">((SUM(C166:F166))/4)*1.04</f>
+        <v>14.82</v>
       </c>
       <c r="S164">
-        <f t="shared" ref="S164" si="161">((SUM(C168:F168))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="S164" si="158">((SUM(C168:F168))/4)*1.04</f>
+        <v>8.32</v>
       </c>
       <c r="T164">
-        <f t="shared" ref="T164" si="162">((SUM(C170:F170))/4)*1.04</f>
-        <v>0</v>
-      </c>
-      <c r="U164">
-        <f t="shared" ref="U164" si="163">((SUM(C172:F172))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="T164" si="159">((SUM(C170:F170))/4)*1.04</f>
+        <v>13.26</v>
+      </c>
+      <c r="U164" t="s">
+        <v>30</v>
       </c>
       <c r="V164">
-        <f t="shared" ref="V164" si="164">((SUM(C164:F172))/20)*1.04</f>
-        <v>0</v>
+        <f>((SUM(C164:F172))/16)*1.04</f>
+        <v>15.21</v>
       </c>
       <c r="W164">
-        <f t="shared" ref="W164" si="165">(SUM(G164:H172))/10</f>
+        <f t="shared" ref="W164" si="160">(SUM(G164:H172))/10</f>
         <v>7.8</v>
       </c>
       <c r="X164">
-        <f t="shared" ref="X164" si="166">(SUM(I164:I172))/5</f>
+        <f t="shared" ref="X164" si="161">(SUM(I164:I172))/5</f>
         <v>1</v>
       </c>
       <c r="Y164">
-        <f t="shared" ref="Y164" si="167">SUM(K164:K172)-Z164</f>
+        <f t="shared" ref="Y164" si="162">SUM(K164:K172)-Z164</f>
         <v>14</v>
       </c>
       <c r="Z164">
-        <f t="shared" ref="Z164" si="168">SUM(L164:L172)</f>
+        <f t="shared" ref="Z164" si="163">SUM(L164:L172)</f>
         <v>11</v>
       </c>
       <c r="AA164" t="s">
@@ -51100,17 +51098,17 @@
       <c r="B166" t="s">
         <v>777</v>
       </c>
-      <c r="C166" t="s">
-        <v>30</v>
-      </c>
-      <c r="D166" t="s">
-        <v>30</v>
-      </c>
-      <c r="E166" t="s">
-        <v>30</v>
-      </c>
-      <c r="F166" t="s">
-        <v>30</v>
+      <c r="C166">
+        <v>12</v>
+      </c>
+      <c r="D166">
+        <v>14</v>
+      </c>
+      <c r="E166">
+        <v>7</v>
+      </c>
+      <c r="F166">
+        <v>24</v>
       </c>
       <c r="G166">
         <v>1</v>
@@ -51200,17 +51198,17 @@
       <c r="B168" t="s">
         <v>779</v>
       </c>
-      <c r="C168" t="s">
-        <v>30</v>
-      </c>
-      <c r="D168" t="s">
-        <v>30</v>
-      </c>
-      <c r="E168" t="s">
-        <v>30</v>
-      </c>
-      <c r="F168" t="s">
-        <v>30</v>
+      <c r="C168">
+        <v>18</v>
+      </c>
+      <c r="D168">
+        <v>7</v>
+      </c>
+      <c r="E168">
+        <v>5</v>
+      </c>
+      <c r="F168">
+        <v>2</v>
       </c>
       <c r="G168">
         <v>0</v>
@@ -51300,17 +51298,17 @@
       <c r="B170" t="s">
         <v>781</v>
       </c>
-      <c r="C170" t="s">
-        <v>30</v>
-      </c>
-      <c r="D170" t="s">
-        <v>30</v>
-      </c>
-      <c r="E170" t="s">
-        <v>30</v>
-      </c>
-      <c r="F170" t="s">
-        <v>30</v>
+      <c r="C170">
+        <v>2</v>
+      </c>
+      <c r="D170">
+        <v>4</v>
+      </c>
+      <c r="E170">
+        <v>5</v>
+      </c>
+      <c r="F170">
+        <v>40</v>
       </c>
       <c r="G170">
         <v>1</v>
@@ -51450,17 +51448,17 @@
       <c r="B173" t="s">
         <v>774</v>
       </c>
-      <c r="C173" t="s">
-        <v>30</v>
-      </c>
-      <c r="D173" t="s">
-        <v>30</v>
-      </c>
-      <c r="E173" t="s">
-        <v>30</v>
-      </c>
-      <c r="F173" t="s">
-        <v>30</v>
+      <c r="C173">
+        <v>26</v>
+      </c>
+      <c r="D173">
+        <v>19</v>
+      </c>
+      <c r="E173">
+        <v>28</v>
+      </c>
+      <c r="F173">
+        <v>5</v>
       </c>
       <c r="G173">
         <v>80</v>
@@ -51490,47 +51488,47 @@
         <v>29</v>
       </c>
       <c r="P173">
-        <f t="shared" ref="P173" si="169">M173*10</f>
+        <f t="shared" ref="P173" si="164">M173*10</f>
         <v>50</v>
       </c>
       <c r="Q173">
-        <f t="shared" ref="Q173" si="170">((SUM(C173:F173))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="Q173" si="165">((SUM(C173:F173))/4)*1.04</f>
+        <v>20.28</v>
       </c>
       <c r="R173">
-        <f t="shared" ref="R173" si="171">((SUM(C175:F175))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="R173" si="166">((SUM(C175:F175))/4)*1.04</f>
+        <v>19.760000000000002</v>
       </c>
       <c r="S173">
-        <f t="shared" ref="S173" si="172">((SUM(C177:F177))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="S173" si="167">((SUM(C177:F177))/4)*1.04</f>
+        <v>24.96</v>
       </c>
       <c r="T173">
-        <f t="shared" ref="T173" si="173">((SUM(C179:F179))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="T173" si="168">((SUM(C179:F179))/4)*1.04</f>
+        <v>24.96</v>
       </c>
       <c r="U173">
-        <f t="shared" ref="U173" si="174">((SUM(C181:F181))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="U173" si="169">((SUM(C181:F181))/4)*1.04</f>
+        <v>28.6</v>
       </c>
       <c r="V173">
-        <f t="shared" ref="V173" si="175">((SUM(C173:F181))/20)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="V173" si="170">((SUM(C173:F181))/20)*1.04</f>
+        <v>23.712000000000003</v>
       </c>
       <c r="W173">
-        <f t="shared" ref="W173" si="176">(SUM(G173:H181))/10</f>
+        <f t="shared" ref="W173" si="171">(SUM(G173:H181))/10</f>
         <v>62.9</v>
       </c>
       <c r="X173">
-        <f t="shared" ref="X173" si="177">(SUM(I173:I181))/5</f>
+        <f t="shared" ref="X173" si="172">(SUM(I173:I181))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y173">
-        <f t="shared" ref="Y173" si="178">SUM(K173:K181)-Z173</f>
+        <f t="shared" ref="Y173" si="173">SUM(K173:K181)-Z173</f>
         <v>56</v>
       </c>
       <c r="Z173">
-        <f t="shared" ref="Z173" si="179">SUM(L173:L181)</f>
+        <f t="shared" ref="Z173" si="174">SUM(L173:L181)</f>
         <v>1</v>
       </c>
       <c r="AA173" t="s">
@@ -51594,17 +51592,17 @@
       <c r="B175" t="s">
         <v>777</v>
       </c>
-      <c r="C175" t="s">
-        <v>30</v>
-      </c>
-      <c r="D175" t="s">
-        <v>30</v>
-      </c>
-      <c r="E175" t="s">
-        <v>30</v>
-      </c>
-      <c r="F175" t="s">
-        <v>30</v>
+      <c r="C175">
+        <v>4</v>
+      </c>
+      <c r="D175">
+        <v>24</v>
+      </c>
+      <c r="E175">
+        <v>17</v>
+      </c>
+      <c r="F175">
+        <v>31</v>
       </c>
       <c r="G175">
         <v>20</v>
@@ -51694,17 +51692,17 @@
       <c r="B177" t="s">
         <v>779</v>
       </c>
-      <c r="C177" t="s">
-        <v>30</v>
-      </c>
-      <c r="D177" t="s">
-        <v>30</v>
-      </c>
-      <c r="E177" t="s">
-        <v>30</v>
-      </c>
-      <c r="F177" t="s">
-        <v>30</v>
+      <c r="C177">
+        <v>27</v>
+      </c>
+      <c r="D177">
+        <v>28</v>
+      </c>
+      <c r="E177">
+        <v>15</v>
+      </c>
+      <c r="F177">
+        <v>26</v>
       </c>
       <c r="G177">
         <v>20</v>
@@ -51794,17 +51792,17 @@
       <c r="B179" t="s">
         <v>781</v>
       </c>
-      <c r="C179" t="s">
-        <v>30</v>
-      </c>
-      <c r="D179" t="s">
-        <v>30</v>
-      </c>
-      <c r="E179" t="s">
-        <v>30</v>
-      </c>
-      <c r="F179" t="s">
-        <v>30</v>
+      <c r="C179">
+        <v>20</v>
+      </c>
+      <c r="D179">
+        <v>25</v>
+      </c>
+      <c r="E179">
+        <v>33</v>
+      </c>
+      <c r="F179">
+        <v>18</v>
       </c>
       <c r="G179">
         <v>80</v>
@@ -51894,17 +51892,17 @@
       <c r="B181" t="s">
         <v>783</v>
       </c>
-      <c r="C181" t="s">
-        <v>30</v>
-      </c>
-      <c r="D181" t="s">
-        <v>30</v>
-      </c>
-      <c r="E181" t="s">
-        <v>30</v>
-      </c>
-      <c r="F181" t="s">
-        <v>30</v>
+      <c r="C181">
+        <v>24</v>
+      </c>
+      <c r="D181">
+        <v>30</v>
+      </c>
+      <c r="E181">
+        <v>30</v>
+      </c>
+      <c r="F181">
+        <v>26</v>
       </c>
       <c r="G181">
         <v>95</v>
@@ -51944,17 +51942,17 @@
       <c r="B182" t="s">
         <v>774</v>
       </c>
-      <c r="C182" t="s">
-        <v>30</v>
-      </c>
-      <c r="D182" t="s">
-        <v>30</v>
-      </c>
-      <c r="E182" t="s">
-        <v>30</v>
-      </c>
-      <c r="F182" t="s">
-        <v>30</v>
+      <c r="C182">
+        <v>20</v>
+      </c>
+      <c r="D182">
+        <v>22</v>
+      </c>
+      <c r="E182">
+        <v>18</v>
+      </c>
+      <c r="F182">
+        <v>14</v>
       </c>
       <c r="G182">
         <v>45</v>
@@ -51984,47 +51982,47 @@
         <v>29</v>
       </c>
       <c r="P182">
-        <f t="shared" ref="P182" si="180">M182*10</f>
+        <f t="shared" ref="P182" si="175">M182*10</f>
         <v>50</v>
       </c>
       <c r="Q182">
-        <f t="shared" ref="Q182" si="181">((SUM(C182:F182))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="Q182" si="176">((SUM(C182:F182))/4)*1.04</f>
+        <v>19.240000000000002</v>
       </c>
       <c r="R182">
-        <f t="shared" ref="R182" si="182">((SUM(C184:F184))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="R182" si="177">((SUM(C184:F184))/4)*1.04</f>
+        <v>18.72</v>
       </c>
       <c r="S182">
-        <f t="shared" ref="S182" si="183">((SUM(C186:F186))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="S182" si="178">((SUM(C186:F186))/4)*1.04</f>
+        <v>11.96</v>
       </c>
       <c r="T182">
-        <f t="shared" ref="T182" si="184">((SUM(C188:F188))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="T182" si="179">((SUM(C188:F188))/4)*1.04</f>
+        <v>24.18</v>
       </c>
       <c r="U182">
-        <f t="shared" ref="U182" si="185">((SUM(C190:F190))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="U182" si="180">((SUM(C190:F190))/4)*1.04</f>
+        <v>44.2</v>
       </c>
       <c r="V182">
-        <f t="shared" ref="V182" si="186">((SUM(C182:F190))/20)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="V182" si="181">((SUM(C182:F190))/20)*1.04</f>
+        <v>23.66</v>
       </c>
       <c r="W182">
-        <f t="shared" ref="W182" si="187">(SUM(G182:H190))/10</f>
+        <f t="shared" ref="W182" si="182">(SUM(G182:H190))/10</f>
         <v>51</v>
       </c>
       <c r="X182">
-        <f t="shared" ref="X182" si="188">(SUM(I182:I190))/5</f>
+        <f t="shared" ref="X182" si="183">(SUM(I182:I190))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y182">
-        <f t="shared" ref="Y182" si="189">SUM(K182:K190)-Z182</f>
+        <f t="shared" ref="Y182" si="184">SUM(K182:K190)-Z182</f>
         <v>64</v>
       </c>
       <c r="Z182">
-        <f t="shared" ref="Z182" si="190">SUM(L182:L190)</f>
+        <f t="shared" ref="Z182" si="185">SUM(L182:L190)</f>
         <v>5</v>
       </c>
       <c r="AA182" t="s">
@@ -52088,17 +52086,17 @@
       <c r="B184" t="s">
         <v>777</v>
       </c>
-      <c r="C184" t="s">
-        <v>30</v>
-      </c>
-      <c r="D184" t="s">
-        <v>30</v>
-      </c>
-      <c r="E184" t="s">
-        <v>30</v>
-      </c>
-      <c r="F184" t="s">
-        <v>30</v>
+      <c r="C184">
+        <v>20</v>
+      </c>
+      <c r="D184">
+        <v>20</v>
+      </c>
+      <c r="E184">
+        <v>15</v>
+      </c>
+      <c r="F184">
+        <v>17</v>
       </c>
       <c r="G184">
         <v>50</v>
@@ -52188,17 +52186,17 @@
       <c r="B186" t="s">
         <v>779</v>
       </c>
-      <c r="C186" t="s">
-        <v>30</v>
-      </c>
-      <c r="D186" t="s">
-        <v>30</v>
-      </c>
-      <c r="E186" t="s">
-        <v>30</v>
-      </c>
-      <c r="F186" t="s">
-        <v>30</v>
+      <c r="C186">
+        <v>17</v>
+      </c>
+      <c r="D186">
+        <v>4</v>
+      </c>
+      <c r="E186">
+        <v>3</v>
+      </c>
+      <c r="F186">
+        <v>22</v>
       </c>
       <c r="G186">
         <v>25</v>
@@ -52288,17 +52286,17 @@
       <c r="B188" t="s">
         <v>781</v>
       </c>
-      <c r="C188" t="s">
-        <v>30</v>
-      </c>
-      <c r="D188" t="s">
-        <v>30</v>
-      </c>
-      <c r="E188" t="s">
-        <v>30</v>
-      </c>
-      <c r="F188" t="s">
-        <v>30</v>
+      <c r="C188">
+        <v>27</v>
+      </c>
+      <c r="D188">
+        <v>21</v>
+      </c>
+      <c r="E188">
+        <v>18</v>
+      </c>
+      <c r="F188">
+        <v>27</v>
       </c>
       <c r="G188">
         <v>50</v>
@@ -52388,17 +52386,17 @@
       <c r="B190" t="s">
         <v>783</v>
       </c>
-      <c r="C190" t="s">
-        <v>30</v>
-      </c>
-      <c r="D190" t="s">
-        <v>30</v>
-      </c>
-      <c r="E190" t="s">
-        <v>30</v>
-      </c>
-      <c r="F190" t="s">
-        <v>30</v>
+      <c r="C190">
+        <v>78</v>
+      </c>
+      <c r="D190">
+        <v>30</v>
+      </c>
+      <c r="E190">
+        <v>33</v>
+      </c>
+      <c r="F190">
+        <v>29</v>
       </c>
       <c r="G190">
         <v>55</v>
@@ -52438,17 +52436,17 @@
       <c r="B191" t="s">
         <v>774</v>
       </c>
-      <c r="C191" t="s">
-        <v>30</v>
-      </c>
-      <c r="D191" t="s">
-        <v>30</v>
-      </c>
-      <c r="E191" t="s">
-        <v>30</v>
-      </c>
-      <c r="F191" t="s">
-        <v>30</v>
+      <c r="C191">
+        <v>15</v>
+      </c>
+      <c r="D191">
+        <v>7</v>
+      </c>
+      <c r="E191">
+        <v>14</v>
+      </c>
+      <c r="F191">
+        <v>12</v>
       </c>
       <c r="G191">
         <v>30</v>
@@ -52478,47 +52476,47 @@
         <v>43</v>
       </c>
       <c r="P191">
-        <f t="shared" ref="P191" si="191">M191*10</f>
+        <f t="shared" ref="P191" si="186">M191*10</f>
         <v>70</v>
       </c>
       <c r="Q191">
-        <f t="shared" ref="Q191" si="192">((SUM(C191:F191))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="Q191" si="187">((SUM(C191:F191))/4)*1.04</f>
+        <v>12.48</v>
       </c>
       <c r="R191">
-        <f t="shared" ref="R191" si="193">((SUM(C193:F193))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="R191" si="188">((SUM(C193:F193))/4)*1.04</f>
+        <v>11.440000000000001</v>
       </c>
       <c r="S191">
-        <f t="shared" ref="S191" si="194">((SUM(C195:F195))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="S191" si="189">((SUM(C195:F195))/4)*1.04</f>
+        <v>13.52</v>
       </c>
       <c r="T191">
-        <f t="shared" ref="T191" si="195">((SUM(C197:F197))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="T191" si="190">((SUM(C197:F197))/4)*1.04</f>
+        <v>12.74</v>
       </c>
       <c r="U191">
-        <f t="shared" ref="U191" si="196">((SUM(C199:F199))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="U191" si="191">((SUM(C199:F199))/4)*1.04</f>
+        <v>22.62</v>
       </c>
       <c r="V191">
-        <f t="shared" ref="V191" si="197">((SUM(C191:F199))/20)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="V191" si="192">((SUM(C191:F199))/20)*1.04</f>
+        <v>14.56</v>
       </c>
       <c r="W191">
-        <f t="shared" ref="W191" si="198">(SUM(G191:H199))/10</f>
+        <f t="shared" ref="W191" si="193">(SUM(G191:H199))/10</f>
         <v>24.4</v>
       </c>
       <c r="X191">
-        <f t="shared" ref="X191" si="199">(SUM(I191:I199))/5</f>
+        <f t="shared" ref="X191" si="194">(SUM(I191:I199))/5</f>
         <v>3</v>
       </c>
       <c r="Y191">
-        <f t="shared" ref="Y191" si="200">SUM(K191:K199)-Z191</f>
+        <f t="shared" ref="Y191" si="195">SUM(K191:K199)-Z191</f>
         <v>35</v>
       </c>
       <c r="Z191">
-        <f t="shared" ref="Z191" si="201">SUM(L191:L199)</f>
+        <f t="shared" ref="Z191" si="196">SUM(L191:L199)</f>
         <v>5</v>
       </c>
       <c r="AA191" t="s">
@@ -52582,17 +52580,17 @@
       <c r="B193" t="s">
         <v>777</v>
       </c>
-      <c r="C193" t="s">
-        <v>30</v>
-      </c>
-      <c r="D193" t="s">
-        <v>30</v>
-      </c>
-      <c r="E193" t="s">
-        <v>30</v>
-      </c>
-      <c r="F193" t="s">
-        <v>30</v>
+      <c r="C193">
+        <v>13</v>
+      </c>
+      <c r="D193">
+        <v>9</v>
+      </c>
+      <c r="E193">
+        <v>12</v>
+      </c>
+      <c r="F193">
+        <v>10</v>
       </c>
       <c r="G193">
         <v>25</v>
@@ -52682,17 +52680,17 @@
       <c r="B195" t="s">
         <v>779</v>
       </c>
-      <c r="C195" t="s">
-        <v>30</v>
-      </c>
-      <c r="D195" t="s">
-        <v>30</v>
-      </c>
-      <c r="E195" t="s">
-        <v>30</v>
-      </c>
-      <c r="F195" t="s">
-        <v>30</v>
+      <c r="C195">
+        <v>23</v>
+      </c>
+      <c r="D195">
+        <v>7</v>
+      </c>
+      <c r="E195">
+        <v>18</v>
+      </c>
+      <c r="F195">
+        <v>4</v>
       </c>
       <c r="G195">
         <v>10</v>
@@ -52782,17 +52780,17 @@
       <c r="B197" t="s">
         <v>781</v>
       </c>
-      <c r="C197" t="s">
-        <v>30</v>
-      </c>
-      <c r="D197" t="s">
-        <v>30</v>
-      </c>
-      <c r="E197" t="s">
-        <v>30</v>
-      </c>
-      <c r="F197" t="s">
-        <v>30</v>
+      <c r="C197">
+        <v>9</v>
+      </c>
+      <c r="D197">
+        <v>8</v>
+      </c>
+      <c r="E197">
+        <v>12</v>
+      </c>
+      <c r="F197">
+        <v>20</v>
       </c>
       <c r="G197">
         <v>50</v>
@@ -52882,17 +52880,17 @@
       <c r="B199" t="s">
         <v>783</v>
       </c>
-      <c r="C199" t="s">
-        <v>30</v>
-      </c>
-      <c r="D199" t="s">
-        <v>30</v>
-      </c>
-      <c r="E199" t="s">
-        <v>30</v>
-      </c>
-      <c r="F199" t="s">
-        <v>30</v>
+      <c r="C199">
+        <v>15</v>
+      </c>
+      <c r="D199">
+        <v>26</v>
+      </c>
+      <c r="E199">
+        <v>20</v>
+      </c>
+      <c r="F199">
+        <v>26</v>
       </c>
       <c r="G199">
         <v>2</v>
@@ -52972,47 +52970,47 @@
         <v>29</v>
       </c>
       <c r="P200">
-        <f t="shared" ref="P200" si="202">M200*10</f>
+        <f t="shared" ref="P200" si="197">M200*10</f>
         <v>70</v>
       </c>
       <c r="Q200">
-        <f t="shared" ref="Q200" si="203">((SUM(C200:F200))/4)*1.04</f>
+        <f t="shared" ref="Q200" si="198">((SUM(C200:F200))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R200">
-        <f t="shared" ref="R200" si="204">((SUM(C202:F202))/4)*1.04</f>
+        <f t="shared" ref="R200" si="199">((SUM(C202:F202))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S200">
-        <f t="shared" ref="S200" si="205">((SUM(C204:F204))/4)*1.04</f>
+        <f t="shared" ref="S200" si="200">((SUM(C204:F204))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T200">
-        <f t="shared" ref="T200" si="206">((SUM(C206:F206))/4)*1.04</f>
+        <f t="shared" ref="T200" si="201">((SUM(C206:F206))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U200">
-        <f t="shared" ref="U200" si="207">((SUM(C208:F208))/4)*1.04</f>
+        <f t="shared" ref="U200" si="202">((SUM(C208:F208))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V200">
-        <f t="shared" ref="V200" si="208">((SUM(C200:F208))/20)*1.04</f>
+        <f t="shared" ref="V200" si="203">((SUM(C200:F208))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W200">
-        <f t="shared" ref="W200" si="209">(SUM(G200:H208))/10</f>
+        <f t="shared" ref="W200" si="204">(SUM(G200:H208))/10</f>
         <v>30</v>
       </c>
       <c r="X200">
-        <f t="shared" ref="X200" si="210">(SUM(I200:I208))/5</f>
+        <f t="shared" ref="X200" si="205">(SUM(I200:I208))/5</f>
         <v>1.4</v>
       </c>
       <c r="Y200">
-        <f t="shared" ref="Y200" si="211">SUM(K200:K208)-Z200</f>
+        <f t="shared" ref="Y200" si="206">SUM(K200:K208)-Z200</f>
         <v>66</v>
       </c>
       <c r="Z200">
-        <f t="shared" ref="Z200" si="212">SUM(L200:L208)</f>
+        <f t="shared" ref="Z200" si="207">SUM(L200:L208)</f>
         <v>2</v>
       </c>
       <c r="AA200" t="s">
@@ -53466,47 +53464,47 @@
         <v>29</v>
       </c>
       <c r="P209">
-        <f t="shared" ref="P209" si="213">M209*10</f>
+        <f t="shared" ref="P209" si="208">M209*10</f>
         <v>110</v>
       </c>
       <c r="Q209">
-        <f t="shared" ref="Q209" si="214">((SUM(C209:F209))/4)*1.04</f>
+        <f t="shared" ref="Q209" si="209">((SUM(C209:F209))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R209">
-        <f t="shared" ref="R209" si="215">((SUM(C211:F211))/4)*1.04</f>
+        <f t="shared" ref="R209" si="210">((SUM(C211:F211))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S209">
-        <f t="shared" ref="S209" si="216">((SUM(C213:F213))/4)*1.04</f>
+        <f t="shared" ref="S209" si="211">((SUM(C213:F213))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T209">
-        <f t="shared" ref="T209" si="217">((SUM(C215:F215))/4)*1.04</f>
+        <f t="shared" ref="T209" si="212">((SUM(C215:F215))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U209">
-        <f t="shared" ref="U209" si="218">((SUM(C217:F217))/4)*1.04</f>
+        <f t="shared" ref="U209" si="213">((SUM(C217:F217))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V209">
-        <f t="shared" ref="V209" si="219">((SUM(C209:F217))/20)*1.04</f>
+        <f t="shared" ref="V209" si="214">((SUM(C209:F217))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W209">
-        <f t="shared" ref="W209" si="220">(SUM(G209:H217))/10</f>
+        <f t="shared" ref="W209" si="215">(SUM(G209:H217))/10</f>
         <v>0.3</v>
       </c>
       <c r="X209">
-        <f t="shared" ref="X209" si="221">(SUM(I209:I217))/5</f>
+        <f t="shared" ref="X209" si="216">(SUM(I209:I217))/5</f>
         <v>2.4</v>
       </c>
       <c r="Y209">
-        <f t="shared" ref="Y209" si="222">SUM(K209:K217)-Z209</f>
+        <f t="shared" ref="Y209" si="217">SUM(K209:K217)-Z209</f>
         <v>35</v>
       </c>
       <c r="Z209">
-        <f t="shared" ref="Z209" si="223">SUM(L209:L217)</f>
+        <f t="shared" ref="Z209" si="218">SUM(L209:L217)</f>
         <v>19</v>
       </c>
       <c r="AA209" t="s">
@@ -53960,47 +53958,47 @@
         <v>29</v>
       </c>
       <c r="P218">
-        <f t="shared" ref="P218" si="224">M218*10</f>
+        <f t="shared" ref="P218" si="219">M218*10</f>
         <v>80</v>
       </c>
       <c r="Q218">
-        <f t="shared" ref="Q218" si="225">((SUM(C218:F218))/4)*1.04</f>
+        <f t="shared" ref="Q218" si="220">((SUM(C218:F218))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R218">
-        <f t="shared" ref="R218" si="226">((SUM(C220:F220))/4)*1.04</f>
+        <f t="shared" ref="R218" si="221">((SUM(C220:F220))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S218">
-        <f t="shared" ref="S218" si="227">((SUM(C222:F222))/4)*1.04</f>
+        <f t="shared" ref="S218" si="222">((SUM(C222:F222))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T218">
-        <f t="shared" ref="T218" si="228">((SUM(C224:F224))/4)*1.04</f>
+        <f t="shared" ref="T218" si="223">((SUM(C224:F224))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U218">
-        <f t="shared" ref="U218" si="229">((SUM(C226:F226))/4)*1.04</f>
+        <f t="shared" ref="U218" si="224">((SUM(C226:F226))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V218">
-        <f t="shared" ref="V218" si="230">((SUM(C218:F226))/20)*1.04</f>
+        <f t="shared" ref="V218" si="225">((SUM(C218:F226))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W218">
-        <f t="shared" ref="W218" si="231">(SUM(G218:H226))/10</f>
+        <f t="shared" ref="W218" si="226">(SUM(G218:H226))/10</f>
         <v>0.4</v>
       </c>
       <c r="X218">
-        <f t="shared" ref="X218" si="232">(SUM(I218:I226))/5</f>
+        <f t="shared" ref="X218" si="227">(SUM(I218:I226))/5</f>
         <v>2.4</v>
       </c>
       <c r="Y218">
-        <f t="shared" ref="Y218" si="233">SUM(K218:K226)-Z218</f>
+        <f t="shared" ref="Y218" si="228">SUM(K218:K226)-Z218</f>
         <v>10</v>
       </c>
       <c r="Z218">
-        <f t="shared" ref="Z218" si="234">SUM(L218:L226)</f>
+        <f t="shared" ref="Z218" si="229">SUM(L218:L226)</f>
         <v>7</v>
       </c>
       <c r="AA218" t="s">
@@ -54454,47 +54452,47 @@
         <v>29</v>
       </c>
       <c r="P227">
-        <f t="shared" ref="P227" si="235">M227*10</f>
+        <f t="shared" ref="P227" si="230">M227*10</f>
         <v>40</v>
       </c>
       <c r="Q227">
-        <f t="shared" ref="Q227" si="236">((SUM(C227:F227))/4)*1.04</f>
+        <f t="shared" ref="Q227" si="231">((SUM(C227:F227))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R227">
-        <f t="shared" ref="R227" si="237">((SUM(C229:F229))/4)*1.04</f>
+        <f t="shared" ref="R227" si="232">((SUM(C229:F229))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S227">
-        <f t="shared" ref="S227" si="238">((SUM(C231:F231))/4)*1.04</f>
+        <f t="shared" ref="S227" si="233">((SUM(C231:F231))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T227">
-        <f t="shared" ref="T227" si="239">((SUM(C233:F233))/4)*1.04</f>
+        <f t="shared" ref="T227" si="234">((SUM(C233:F233))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U227">
-        <f t="shared" ref="U227" si="240">((SUM(C235:F235))/4)*1.04</f>
+        <f t="shared" ref="U227" si="235">((SUM(C235:F235))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V227">
-        <f t="shared" ref="V227" si="241">((SUM(C227:F235))/20)*1.04</f>
+        <f t="shared" ref="V227" si="236">((SUM(C227:F235))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W227">
-        <f t="shared" ref="W227" si="242">(SUM(G227:H235))/10</f>
+        <f t="shared" ref="W227" si="237">(SUM(G227:H235))/10</f>
         <v>34</v>
       </c>
       <c r="X227">
-        <f t="shared" ref="X227" si="243">(SUM(I227:I235))/5</f>
+        <f t="shared" ref="X227" si="238">(SUM(I227:I235))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y227">
-        <f t="shared" ref="Y227" si="244">SUM(K227:K235)-Z227</f>
+        <f t="shared" ref="Y227" si="239">SUM(K227:K235)-Z227</f>
         <v>1</v>
       </c>
       <c r="Z227">
-        <f t="shared" ref="Z227" si="245">SUM(L227:L235)</f>
+        <f t="shared" ref="Z227" si="240">SUM(L227:L235)</f>
         <v>6</v>
       </c>
       <c r="AA227" t="s">
@@ -54948,47 +54946,47 @@
         <v>29</v>
       </c>
       <c r="P236">
-        <f t="shared" ref="P236" si="246">M236*10</f>
+        <f t="shared" ref="P236" si="241">M236*10</f>
         <v>70</v>
       </c>
       <c r="Q236">
-        <f t="shared" ref="Q236" si="247">((SUM(C236:F236))/4)*1.04</f>
+        <f t="shared" ref="Q236" si="242">((SUM(C236:F236))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R236">
-        <f t="shared" ref="R236" si="248">((SUM(C238:F238))/4)*1.04</f>
+        <f t="shared" ref="R236" si="243">((SUM(C238:F238))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S236">
-        <f t="shared" ref="S236" si="249">((SUM(C240:F240))/4)*1.04</f>
+        <f t="shared" ref="S236" si="244">((SUM(C240:F240))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T236">
-        <f t="shared" ref="T236" si="250">((SUM(C242:F242))/4)*1.04</f>
+        <f t="shared" ref="T236" si="245">((SUM(C242:F242))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U236">
-        <f t="shared" ref="U236" si="251">((SUM(C244:F244))/4)*1.04</f>
+        <f t="shared" ref="U236" si="246">((SUM(C244:F244))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V236">
-        <f t="shared" ref="V236" si="252">((SUM(C236:F244))/20)*1.04</f>
+        <f t="shared" ref="V236" si="247">((SUM(C236:F244))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W236">
-        <f t="shared" ref="W236" si="253">(SUM(G236:H244))/10</f>
+        <f t="shared" ref="W236" si="248">(SUM(G236:H244))/10</f>
         <v>48.5</v>
       </c>
       <c r="X236">
-        <f t="shared" ref="X236" si="254">(SUM(I236:I244))/5</f>
+        <f t="shared" ref="X236" si="249">(SUM(I236:I244))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y236">
-        <f t="shared" ref="Y236" si="255">SUM(K236:K244)-Z236</f>
+        <f t="shared" ref="Y236" si="250">SUM(K236:K244)-Z236</f>
         <v>6</v>
       </c>
       <c r="Z236">
-        <f t="shared" ref="Z236" si="256">SUM(L236:L244)</f>
+        <f t="shared" ref="Z236" si="251">SUM(L236:L244)</f>
         <v>6</v>
       </c>
       <c r="AA236" t="s">
@@ -55442,47 +55440,47 @@
         <v>29</v>
       </c>
       <c r="P245">
-        <f t="shared" ref="P245" si="257">M245*10</f>
+        <f t="shared" ref="P245" si="252">M245*10</f>
         <v>100</v>
       </c>
       <c r="Q245">
-        <f t="shared" ref="Q245" si="258">((SUM(C245:F245))/4)*1.04</f>
+        <f t="shared" ref="Q245" si="253">((SUM(C245:F245))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R245">
-        <f t="shared" ref="R245" si="259">((SUM(C247:F247))/4)*1.04</f>
+        <f t="shared" ref="R245" si="254">((SUM(C247:F247))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S245">
-        <f t="shared" ref="S245" si="260">((SUM(C249:F249))/4)*1.04</f>
+        <f t="shared" ref="S245" si="255">((SUM(C249:F249))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T245">
-        <f t="shared" ref="T245" si="261">((SUM(C251:F251))/4)*1.04</f>
+        <f t="shared" ref="T245" si="256">((SUM(C251:F251))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U245">
-        <f t="shared" ref="U245" si="262">((SUM(C253:F253))/4)*1.04</f>
+        <f t="shared" ref="U245" si="257">((SUM(C253:F253))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V245">
-        <f t="shared" ref="V245" si="263">((SUM(C245:F253))/20)*1.04</f>
+        <f t="shared" ref="V245" si="258">((SUM(C245:F253))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W245">
-        <f t="shared" ref="W245" si="264">(SUM(G245:H253))/10</f>
+        <f t="shared" ref="W245" si="259">(SUM(G245:H253))/10</f>
         <v>1.7</v>
       </c>
       <c r="X245">
-        <f t="shared" ref="X245" si="265">(SUM(I245:I253))/5</f>
+        <f t="shared" ref="X245" si="260">(SUM(I245:I253))/5</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="Y245">
-        <f t="shared" ref="Y245" si="266">SUM(K245:K253)-Z245</f>
+        <f t="shared" ref="Y245" si="261">SUM(K245:K253)-Z245</f>
         <v>83</v>
       </c>
       <c r="Z245">
-        <f t="shared" ref="Z245" si="267">SUM(L245:L253)</f>
+        <f t="shared" ref="Z245" si="262">SUM(L245:L253)</f>
         <v>3</v>
       </c>
       <c r="AA245" t="s">
@@ -55936,47 +55934,47 @@
         <v>29</v>
       </c>
       <c r="P254">
-        <f t="shared" ref="P254" si="268">M254*10</f>
+        <f t="shared" ref="P254" si="263">M254*10</f>
         <v>120</v>
       </c>
       <c r="Q254">
-        <f t="shared" ref="Q254" si="269">((SUM(C254:F254))/4)*1.04</f>
+        <f t="shared" ref="Q254" si="264">((SUM(C254:F254))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R254">
-        <f t="shared" ref="R254" si="270">((SUM(C256:F256))/4)*1.04</f>
+        <f t="shared" ref="R254" si="265">((SUM(C256:F256))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S254">
-        <f t="shared" ref="S254" si="271">((SUM(C258:F258))/4)*1.04</f>
+        <f t="shared" ref="S254" si="266">((SUM(C258:F258))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T254">
-        <f t="shared" ref="T254" si="272">((SUM(C260:F260))/4)*1.04</f>
+        <f t="shared" ref="T254" si="267">((SUM(C260:F260))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U254">
-        <f t="shared" ref="U254" si="273">((SUM(C262:F262))/4)*1.04</f>
+        <f t="shared" ref="U254" si="268">((SUM(C262:F262))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V254">
-        <f t="shared" ref="V254" si="274">((SUM(C254:F262))/20)*1.04</f>
+        <f t="shared" ref="V254" si="269">((SUM(C254:F262))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W254">
-        <f t="shared" ref="W254" si="275">(SUM(G254:H262))/10</f>
+        <f t="shared" ref="W254" si="270">(SUM(G254:H262))/10</f>
         <v>15.6</v>
       </c>
       <c r="X254">
-        <f t="shared" ref="X254" si="276">(SUM(I254:I262))/5</f>
+        <f t="shared" ref="X254" si="271">(SUM(I254:I262))/5</f>
         <v>2</v>
       </c>
       <c r="Y254">
-        <f t="shared" ref="Y254" si="277">SUM(K254:K262)-Z254</f>
+        <f t="shared" ref="Y254" si="272">SUM(K254:K262)-Z254</f>
         <v>58</v>
       </c>
       <c r="Z254">
-        <f t="shared" ref="Z254" si="278">SUM(L254:L262)</f>
+        <f t="shared" ref="Z254" si="273">SUM(L254:L262)</f>
         <v>12</v>
       </c>
       <c r="AA254" t="s">
@@ -56430,47 +56428,47 @@
         <v>240</v>
       </c>
       <c r="P263">
-        <f t="shared" ref="P263" si="279">M263*10</f>
+        <f t="shared" ref="P263" si="274">M263*10</f>
         <v>60</v>
       </c>
       <c r="Q263">
-        <f t="shared" ref="Q263" si="280">((SUM(C263:F263))/4)*1.04</f>
+        <f t="shared" ref="Q263" si="275">((SUM(C263:F263))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R263">
-        <f t="shared" ref="R263" si="281">((SUM(C265:F265))/4)*1.04</f>
+        <f t="shared" ref="R263" si="276">((SUM(C265:F265))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S263">
-        <f t="shared" ref="S263" si="282">((SUM(C267:F267))/4)*1.04</f>
+        <f t="shared" ref="S263" si="277">((SUM(C267:F267))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T263">
-        <f t="shared" ref="T263" si="283">((SUM(C269:F269))/4)*1.04</f>
+        <f t="shared" ref="T263" si="278">((SUM(C269:F269))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U263">
-        <f t="shared" ref="U263" si="284">((SUM(C271:F271))/4)*1.04</f>
+        <f t="shared" ref="U263" si="279">((SUM(C271:F271))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V263">
-        <f t="shared" ref="V263" si="285">((SUM(C263:F271))/20)*1.04</f>
+        <f t="shared" ref="V263" si="280">((SUM(C263:F271))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W263">
-        <f t="shared" ref="W263" si="286">(SUM(G263:H271))/10</f>
+        <f t="shared" ref="W263" si="281">(SUM(G263:H271))/10</f>
         <v>4.5</v>
       </c>
       <c r="X263">
-        <f t="shared" ref="X263" si="287">(SUM(I263:I271))/5</f>
+        <f t="shared" ref="X263" si="282">(SUM(I263:I271))/5</f>
         <v>4</v>
       </c>
       <c r="Y263">
-        <f t="shared" ref="Y263" si="288">SUM(K263:K271)-Z263</f>
+        <f t="shared" ref="Y263" si="283">SUM(K263:K271)-Z263</f>
         <v>16</v>
       </c>
       <c r="Z263">
-        <f t="shared" ref="Z263" si="289">SUM(L263:L271)</f>
+        <f t="shared" ref="Z263" si="284">SUM(L263:L271)</f>
         <v>3</v>
       </c>
       <c r="AA263" t="s">
@@ -56924,47 +56922,47 @@
         <v>240</v>
       </c>
       <c r="P272">
-        <f t="shared" ref="P272" si="290">M272*10</f>
+        <f t="shared" ref="P272" si="285">M272*10</f>
         <v>30</v>
       </c>
       <c r="Q272">
-        <f t="shared" ref="Q272" si="291">((SUM(C272:F272))/4)*1.04</f>
+        <f t="shared" ref="Q272" si="286">((SUM(C272:F272))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R272">
-        <f t="shared" ref="R272" si="292">((SUM(C274:F274))/4)*1.04</f>
+        <f t="shared" ref="R272" si="287">((SUM(C274:F274))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S272">
-        <f t="shared" ref="S272" si="293">((SUM(C276:F276))/4)*1.04</f>
+        <f t="shared" ref="S272" si="288">((SUM(C276:F276))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T272">
-        <f t="shared" ref="T272" si="294">((SUM(C278:F278))/4)*1.04</f>
+        <f t="shared" ref="T272" si="289">((SUM(C278:F278))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U272">
-        <f t="shared" ref="U272" si="295">((SUM(C280:F280))/4)*1.04</f>
+        <f t="shared" ref="U272" si="290">((SUM(C280:F280))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V272">
-        <f t="shared" ref="V272" si="296">((SUM(C272:F280))/20)*1.04</f>
+        <f t="shared" ref="V272" si="291">((SUM(C272:F280))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W272">
-        <f t="shared" ref="W272" si="297">(SUM(G272:H280))/10</f>
+        <f t="shared" ref="W272" si="292">(SUM(G272:H280))/10</f>
         <v>6</v>
       </c>
       <c r="X272">
-        <f t="shared" ref="X272" si="298">(SUM(I272:I280))/5</f>
+        <f t="shared" ref="X272" si="293">(SUM(I272:I280))/5</f>
         <v>2.6</v>
       </c>
       <c r="Y272">
-        <f t="shared" ref="Y272" si="299">SUM(K272:K280)-Z272</f>
+        <f t="shared" ref="Y272" si="294">SUM(K272:K280)-Z272</f>
         <v>12</v>
       </c>
       <c r="Z272">
-        <f t="shared" ref="Z272" si="300">SUM(L272:L280)</f>
+        <f t="shared" ref="Z272" si="295">SUM(L272:L280)</f>
         <v>3</v>
       </c>
       <c r="AA272" t="s">
@@ -57418,47 +57416,47 @@
         <v>240</v>
       </c>
       <c r="P281">
-        <f t="shared" ref="P281" si="301">M281*10</f>
+        <f t="shared" ref="P281" si="296">M281*10</f>
         <v>50</v>
       </c>
       <c r="Q281">
-        <f t="shared" ref="Q281" si="302">((SUM(C281:F281))/4)*1.04</f>
+        <f t="shared" ref="Q281" si="297">((SUM(C281:F281))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R281">
-        <f t="shared" ref="R281" si="303">((SUM(C283:F283))/4)*1.04</f>
+        <f t="shared" ref="R281" si="298">((SUM(C283:F283))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S281">
-        <f t="shared" ref="S281" si="304">((SUM(C285:F285))/4)*1.04</f>
+        <f t="shared" ref="S281" si="299">((SUM(C285:F285))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T281">
-        <f t="shared" ref="T281" si="305">((SUM(C287:F287))/4)*1.04</f>
+        <f t="shared" ref="T281" si="300">((SUM(C287:F287))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U281">
-        <f t="shared" ref="U281" si="306">((SUM(C289:F289))/4)*1.04</f>
+        <f t="shared" ref="U281" si="301">((SUM(C289:F289))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V281">
-        <f t="shared" ref="V281" si="307">((SUM(C281:F289))/20)*1.04</f>
+        <f t="shared" ref="V281" si="302">((SUM(C281:F289))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W281">
-        <f t="shared" ref="W281" si="308">(SUM(G281:H289))/10</f>
+        <f t="shared" ref="W281" si="303">(SUM(G281:H289))/10</f>
         <v>21</v>
       </c>
       <c r="X281">
-        <f t="shared" ref="X281" si="309">(SUM(I281:I289))/5</f>
+        <f t="shared" ref="X281" si="304">(SUM(I281:I289))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y281">
-        <f t="shared" ref="Y281" si="310">SUM(K281:K289)-Z281</f>
+        <f t="shared" ref="Y281" si="305">SUM(K281:K289)-Z281</f>
         <v>11</v>
       </c>
       <c r="Z281">
-        <f t="shared" ref="Z281" si="311">SUM(L281:L289)</f>
+        <f t="shared" ref="Z281" si="306">SUM(L281:L289)</f>
         <v>4</v>
       </c>
       <c r="AA281" t="s">
@@ -57912,47 +57910,47 @@
         <v>43</v>
       </c>
       <c r="P290">
-        <f t="shared" ref="P290" si="312">M290*10</f>
+        <f t="shared" ref="P290" si="307">M290*10</f>
         <v>90</v>
       </c>
       <c r="Q290">
-        <f t="shared" ref="Q290" si="313">((SUM(C290:F290))/4)*1.04</f>
+        <f t="shared" ref="Q290" si="308">((SUM(C290:F290))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R290">
-        <f t="shared" ref="R290" si="314">((SUM(C292:F292))/4)*1.04</f>
+        <f t="shared" ref="R290" si="309">((SUM(C292:F292))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S290">
-        <f t="shared" ref="S290" si="315">((SUM(C294:F294))/4)*1.04</f>
+        <f t="shared" ref="S290" si="310">((SUM(C294:F294))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T290">
-        <f t="shared" ref="T290" si="316">((SUM(C296:F296))/4)*1.04</f>
+        <f t="shared" ref="T290" si="311">((SUM(C296:F296))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U290">
-        <f t="shared" ref="U290" si="317">((SUM(C298:F298))/4)*1.04</f>
+        <f t="shared" ref="U290" si="312">((SUM(C298:F298))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V290">
-        <f t="shared" ref="V290" si="318">((SUM(C290:F298))/20)*1.04</f>
+        <f t="shared" ref="V290" si="313">((SUM(C290:F298))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W290">
-        <f t="shared" ref="W290" si="319">(SUM(G290:H298))/10</f>
+        <f t="shared" ref="W290" si="314">(SUM(G290:H298))/10</f>
         <v>3.2</v>
       </c>
       <c r="X290">
-        <f t="shared" ref="X290" si="320">(SUM(I290:I298))/5</f>
+        <f t="shared" ref="X290" si="315">(SUM(I290:I298))/5</f>
         <v>2.6</v>
       </c>
       <c r="Y290">
-        <f t="shared" ref="Y290" si="321">SUM(K290:K298)-Z290</f>
+        <f t="shared" ref="Y290" si="316">SUM(K290:K298)-Z290</f>
         <v>65</v>
       </c>
       <c r="Z290">
-        <f t="shared" ref="Z290" si="322">SUM(L290:L298)</f>
+        <f t="shared" ref="Z290" si="317">SUM(L290:L298)</f>
         <v>2</v>
       </c>
       <c r="AA290" t="s">
@@ -58406,47 +58404,47 @@
         <v>29</v>
       </c>
       <c r="P299">
-        <f t="shared" ref="P299" si="323">M299*10</f>
+        <f t="shared" ref="P299" si="318">M299*10</f>
         <v>90</v>
       </c>
       <c r="Q299">
-        <f t="shared" ref="Q299" si="324">((SUM(C299:F299))/4)*1.04</f>
+        <f t="shared" ref="Q299" si="319">((SUM(C299:F299))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R299">
-        <f t="shared" ref="R299" si="325">((SUM(C301:F301))/4)*1.04</f>
+        <f t="shared" ref="R299" si="320">((SUM(C301:F301))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S299">
-        <f t="shared" ref="S299" si="326">((SUM(C303:F303))/4)*1.04</f>
+        <f t="shared" ref="S299" si="321">((SUM(C303:F303))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T299">
-        <f t="shared" ref="T299" si="327">((SUM(C305:F305))/4)*1.04</f>
+        <f t="shared" ref="T299" si="322">((SUM(C305:F305))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U299">
-        <f t="shared" ref="U299" si="328">((SUM(C307:F307))/4)*1.04</f>
+        <f t="shared" ref="U299" si="323">((SUM(C307:F307))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V299">
-        <f t="shared" ref="V299" si="329">((SUM(C299:F307))/20)*1.04</f>
+        <f t="shared" ref="V299" si="324">((SUM(C299:F307))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W299">
-        <f t="shared" ref="W299" si="330">(SUM(G299:H307))/10</f>
+        <f t="shared" ref="W299" si="325">(SUM(G299:H307))/10</f>
         <v>0.4</v>
       </c>
       <c r="X299">
-        <f t="shared" ref="X299" si="331">(SUM(I299:I307))/5</f>
+        <f t="shared" ref="X299" si="326">(SUM(I299:I307))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y299">
-        <f t="shared" ref="Y299" si="332">SUM(K299:K307)-Z299</f>
+        <f t="shared" ref="Y299" si="327">SUM(K299:K307)-Z299</f>
         <v>76</v>
       </c>
       <c r="Z299">
-        <f t="shared" ref="Z299" si="333">SUM(L299:L307)</f>
+        <f t="shared" ref="Z299" si="328">SUM(L299:L307)</f>
         <v>10</v>
       </c>
       <c r="AA299" t="s">
@@ -58900,47 +58898,47 @@
         <v>29</v>
       </c>
       <c r="P308">
-        <f t="shared" ref="P308" si="334">M308*10</f>
+        <f t="shared" ref="P308" si="329">M308*10</f>
         <v>60</v>
       </c>
       <c r="Q308">
-        <f t="shared" ref="Q308" si="335">((SUM(C308:F308))/4)*1.04</f>
+        <f t="shared" ref="Q308" si="330">((SUM(C308:F308))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R308">
-        <f t="shared" ref="R308" si="336">((SUM(C310:F310))/4)*1.04</f>
+        <f t="shared" ref="R308" si="331">((SUM(C310:F310))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S308">
-        <f t="shared" ref="S308" si="337">((SUM(C312:F312))/4)*1.04</f>
+        <f t="shared" ref="S308" si="332">((SUM(C312:F312))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T308">
-        <f t="shared" ref="T308" si="338">((SUM(C314:F314))/4)*1.04</f>
+        <f t="shared" ref="T308" si="333">((SUM(C314:F314))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U308">
-        <f t="shared" ref="U308" si="339">((SUM(C316:F316))/4)*1.04</f>
+        <f t="shared" ref="U308" si="334">((SUM(C316:F316))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V308">
-        <f t="shared" ref="V308" si="340">((SUM(C308:F316))/20)*1.04</f>
+        <f t="shared" ref="V308" si="335">((SUM(C308:F316))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W308">
-        <f t="shared" ref="W308" si="341">(SUM(G308:H316))/10</f>
+        <f t="shared" ref="W308" si="336">(SUM(G308:H316))/10</f>
         <v>42.7</v>
       </c>
       <c r="X308">
-        <f t="shared" ref="X308" si="342">(SUM(I308:I316))/5</f>
+        <f t="shared" ref="X308" si="337">(SUM(I308:I316))/5</f>
         <v>2</v>
       </c>
       <c r="Y308">
-        <f t="shared" ref="Y308" si="343">SUM(K308:K316)-Z308</f>
+        <f t="shared" ref="Y308" si="338">SUM(K308:K316)-Z308</f>
         <v>80</v>
       </c>
       <c r="Z308">
-        <f t="shared" ref="Z308" si="344">SUM(L308:L316)</f>
+        <f t="shared" ref="Z308" si="339">SUM(L308:L316)</f>
         <v>5</v>
       </c>
       <c r="AA308" t="s">
@@ -59394,47 +59392,47 @@
         <v>240</v>
       </c>
       <c r="P317">
-        <f t="shared" ref="P317" si="345">M317*10</f>
+        <f t="shared" ref="P317" si="340">M317*10</f>
         <v>60</v>
       </c>
       <c r="Q317">
-        <f t="shared" ref="Q317" si="346">((SUM(C317:F317))/4)*1.04</f>
+        <f t="shared" ref="Q317" si="341">((SUM(C317:F317))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R317">
-        <f t="shared" ref="R317" si="347">((SUM(C319:F319))/4)*1.04</f>
+        <f t="shared" ref="R317" si="342">((SUM(C319:F319))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S317">
-        <f t="shared" ref="S317" si="348">((SUM(C321:F321))/4)*1.04</f>
+        <f t="shared" ref="S317" si="343">((SUM(C321:F321))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T317">
-        <f t="shared" ref="T317" si="349">((SUM(C323:F323))/4)*1.04</f>
+        <f t="shared" ref="T317" si="344">((SUM(C323:F323))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U317">
-        <f t="shared" ref="U317" si="350">((SUM(C325:F325))/4)*1.04</f>
+        <f t="shared" ref="U317" si="345">((SUM(C325:F325))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V317">
-        <f t="shared" ref="V317" si="351">((SUM(C317:F325))/20)*1.04</f>
+        <f t="shared" ref="V317" si="346">((SUM(C317:F325))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W317">
-        <f t="shared" ref="W317" si="352">(SUM(G317:H325))/10</f>
+        <f t="shared" ref="W317" si="347">(SUM(G317:H325))/10</f>
         <v>16.5</v>
       </c>
       <c r="X317">
-        <f t="shared" ref="X317" si="353">(SUM(I317:I325))/5</f>
+        <f t="shared" ref="X317" si="348">(SUM(I317:I325))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y317">
-        <f t="shared" ref="Y317" si="354">SUM(K317:K325)-Z317</f>
+        <f t="shared" ref="Y317" si="349">SUM(K317:K325)-Z317</f>
         <v>19</v>
       </c>
       <c r="Z317">
-        <f t="shared" ref="Z317" si="355">SUM(L317:L325)</f>
+        <f t="shared" ref="Z317" si="350">SUM(L317:L325)</f>
         <v>2</v>
       </c>
       <c r="AA317" t="s">
@@ -59888,47 +59886,47 @@
         <v>43</v>
       </c>
       <c r="P326" t="e">
-        <f t="shared" ref="P326" si="356">M326*10</f>
+        <f t="shared" ref="P326" si="351">M326*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q326">
-        <f t="shared" ref="Q326" si="357">((SUM(C326:F326))/4)*1.04</f>
+        <f t="shared" ref="Q326" si="352">((SUM(C326:F326))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R326">
-        <f t="shared" ref="R326" si="358">((SUM(C328:F328))/4)*1.04</f>
+        <f t="shared" ref="R326" si="353">((SUM(C328:F328))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S326">
-        <f t="shared" ref="S326" si="359">((SUM(C330:F330))/4)*1.04</f>
+        <f t="shared" ref="S326" si="354">((SUM(C330:F330))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T326">
-        <f t="shared" ref="T326" si="360">((SUM(C332:F332))/4)*1.04</f>
+        <f t="shared" ref="T326" si="355">((SUM(C332:F332))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U326">
-        <f t="shared" ref="U326" si="361">((SUM(C334:F334))/4)*1.04</f>
+        <f t="shared" ref="U326" si="356">((SUM(C334:F334))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V326">
-        <f t="shared" ref="V326" si="362">((SUM(C326:F334))/20)*1.04</f>
+        <f t="shared" ref="V326" si="357">((SUM(C326:F334))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W326">
-        <f t="shared" ref="W326" si="363">(SUM(G326:H334))/10</f>
+        <f t="shared" ref="W326" si="358">(SUM(G326:H334))/10</f>
         <v>50.5</v>
       </c>
       <c r="X326">
-        <f t="shared" ref="X326" si="364">(SUM(I326:I334))/5</f>
+        <f t="shared" ref="X326" si="359">(SUM(I326:I334))/5</f>
         <v>1.6</v>
       </c>
       <c r="Y326">
-        <f t="shared" ref="Y326" si="365">SUM(K326:K334)-Z326</f>
+        <f t="shared" ref="Y326" si="360">SUM(K326:K334)-Z326</f>
         <v>32</v>
       </c>
       <c r="Z326">
-        <f t="shared" ref="Z326" si="366">SUM(L326:L334)</f>
+        <f t="shared" ref="Z326" si="361">SUM(L326:L334)</f>
         <v>2</v>
       </c>
       <c r="AA326" t="s">
@@ -60382,47 +60380,47 @@
         <v>240</v>
       </c>
       <c r="P335" t="e">
-        <f t="shared" ref="P335" si="367">M335*10</f>
+        <f t="shared" ref="P335" si="362">M335*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q335">
-        <f t="shared" ref="Q335" si="368">((SUM(C335:F335))/4)*1.04</f>
+        <f t="shared" ref="Q335" si="363">((SUM(C335:F335))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R335">
-        <f t="shared" ref="R335" si="369">((SUM(C337:F337))/4)*1.04</f>
+        <f t="shared" ref="R335" si="364">((SUM(C337:F337))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S335">
-        <f t="shared" ref="S335" si="370">((SUM(C339:F339))/4)*1.04</f>
+        <f t="shared" ref="S335" si="365">((SUM(C339:F339))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T335">
-        <f t="shared" ref="T335" si="371">((SUM(C341:F341))/4)*1.04</f>
+        <f t="shared" ref="T335" si="366">((SUM(C341:F341))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U335">
-        <f t="shared" ref="U335" si="372">((SUM(C343:F343))/4)*1.04</f>
+        <f t="shared" ref="U335" si="367">((SUM(C343:F343))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V335">
-        <f t="shared" ref="V335" si="373">((SUM(C335:F343))/20)*1.04</f>
+        <f t="shared" ref="V335" si="368">((SUM(C335:F343))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W335">
-        <f t="shared" ref="W335" si="374">(SUM(G335:H343))/10</f>
+        <f t="shared" ref="W335" si="369">(SUM(G335:H343))/10</f>
         <v>47</v>
       </c>
       <c r="X335">
-        <f t="shared" ref="X335" si="375">(SUM(I335:I343))/5</f>
+        <f t="shared" ref="X335" si="370">(SUM(I335:I343))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y335">
-        <f t="shared" ref="Y335" si="376">SUM(K335:K343)-Z335</f>
+        <f t="shared" ref="Y335" si="371">SUM(K335:K343)-Z335</f>
         <v>24</v>
       </c>
       <c r="Z335">
-        <f t="shared" ref="Z335" si="377">SUM(L335:L343)</f>
+        <f t="shared" ref="Z335" si="372">SUM(L335:L343)</f>
         <v>0</v>
       </c>
       <c r="AA335" t="s">
@@ -60876,47 +60874,47 @@
         <v>43</v>
       </c>
       <c r="P344">
-        <f t="shared" ref="P344" si="378">M344*10</f>
+        <f t="shared" ref="P344" si="373">M344*10</f>
         <v>100</v>
       </c>
       <c r="Q344">
-        <f t="shared" ref="Q344" si="379">((SUM(C344:F344))/4)*1.04</f>
+        <f t="shared" ref="Q344" si="374">((SUM(C344:F344))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R344">
-        <f t="shared" ref="R344" si="380">((SUM(C346:F346))/4)*1.04</f>
+        <f t="shared" ref="R344" si="375">((SUM(C346:F346))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S344">
-        <f t="shared" ref="S344" si="381">((SUM(C348:F348))/4)*1.04</f>
+        <f t="shared" ref="S344" si="376">((SUM(C348:F348))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T344">
-        <f t="shared" ref="T344" si="382">((SUM(C350:F350))/4)*1.04</f>
+        <f t="shared" ref="T344" si="377">((SUM(C350:F350))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U344">
-        <f t="shared" ref="U344" si="383">((SUM(C352:F352))/4)*1.04</f>
+        <f t="shared" ref="U344" si="378">((SUM(C352:F352))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V344">
-        <f t="shared" ref="V344" si="384">((SUM(C344:F352))/20)*1.04</f>
+        <f t="shared" ref="V344" si="379">((SUM(C344:F352))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W344">
-        <f t="shared" ref="W344" si="385">(SUM(G344:H352))/10</f>
+        <f t="shared" ref="W344" si="380">(SUM(G344:H352))/10</f>
         <v>1.7</v>
       </c>
       <c r="X344">
-        <f t="shared" ref="X344" si="386">(SUM(I344:I352))/5</f>
+        <f t="shared" ref="X344" si="381">(SUM(I344:I352))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y344">
-        <f t="shared" ref="Y344" si="387">SUM(K344:K352)-Z344</f>
+        <f t="shared" ref="Y344" si="382">SUM(K344:K352)-Z344</f>
         <v>62</v>
       </c>
       <c r="Z344">
-        <f t="shared" ref="Z344" si="388">SUM(L344:L352)</f>
+        <f t="shared" ref="Z344" si="383">SUM(L344:L352)</f>
         <v>7</v>
       </c>
       <c r="AA344" t="s">
@@ -61370,47 +61368,47 @@
         <v>43</v>
       </c>
       <c r="P353">
-        <f t="shared" ref="P353" si="389">M353*10</f>
+        <f t="shared" ref="P353" si="384">M353*10</f>
         <v>90</v>
       </c>
       <c r="Q353">
-        <f t="shared" ref="Q353" si="390">((SUM(C353:F353))/4)*1.04</f>
+        <f t="shared" ref="Q353" si="385">((SUM(C353:F353))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R353">
-        <f t="shared" ref="R353" si="391">((SUM(C355:F355))/4)*1.04</f>
+        <f t="shared" ref="R353" si="386">((SUM(C355:F355))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S353">
-        <f t="shared" ref="S353" si="392">((SUM(C357:F357))/4)*1.04</f>
+        <f t="shared" ref="S353" si="387">((SUM(C357:F357))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T353">
-        <f t="shared" ref="T353" si="393">((SUM(C359:F359))/4)*1.04</f>
+        <f t="shared" ref="T353" si="388">((SUM(C359:F359))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U353">
-        <f t="shared" ref="U353" si="394">((SUM(C361:F361))/4)*1.04</f>
+        <f t="shared" ref="U353" si="389">((SUM(C361:F361))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V353">
-        <f t="shared" ref="V353" si="395">((SUM(C353:F361))/20)*1.04</f>
+        <f t="shared" ref="V353" si="390">((SUM(C353:F361))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W353">
-        <f t="shared" ref="W353" si="396">(SUM(G353:H361))/10</f>
+        <f t="shared" ref="W353" si="391">(SUM(G353:H361))/10</f>
         <v>2.4</v>
       </c>
       <c r="X353">
-        <f t="shared" ref="X353" si="397">(SUM(I353:I361))/5</f>
+        <f t="shared" ref="X353" si="392">(SUM(I353:I361))/5</f>
         <v>3.8</v>
       </c>
       <c r="Y353">
-        <f t="shared" ref="Y353" si="398">SUM(K353:K361)-Z353</f>
+        <f t="shared" ref="Y353" si="393">SUM(K353:K361)-Z353</f>
         <v>54</v>
       </c>
       <c r="Z353">
-        <f t="shared" ref="Z353" si="399">SUM(L353:L361)</f>
+        <f t="shared" ref="Z353" si="394">SUM(L353:L361)</f>
         <v>6</v>
       </c>
       <c r="AA353" t="s">
@@ -61864,47 +61862,47 @@
         <v>29</v>
       </c>
       <c r="P362">
-        <f t="shared" ref="P362" si="400">M362*10</f>
+        <f t="shared" ref="P362" si="395">M362*10</f>
         <v>50</v>
       </c>
       <c r="Q362">
-        <f t="shared" ref="Q362" si="401">((SUM(C362:F362))/4)*1.04</f>
+        <f t="shared" ref="Q362" si="396">((SUM(C362:F362))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R362">
-        <f t="shared" ref="R362" si="402">((SUM(C364:F364))/4)*1.04</f>
+        <f t="shared" ref="R362" si="397">((SUM(C364:F364))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S362">
-        <f t="shared" ref="S362" si="403">((SUM(C366:F366))/4)*1.04</f>
+        <f t="shared" ref="S362" si="398">((SUM(C366:F366))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T362">
-        <f t="shared" ref="T362" si="404">((SUM(C368:F368))/4)*1.04</f>
+        <f t="shared" ref="T362" si="399">((SUM(C368:F368))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U362">
-        <f t="shared" ref="U362" si="405">((SUM(C370:F370))/4)*1.04</f>
+        <f t="shared" ref="U362" si="400">((SUM(C370:F370))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V362">
-        <f t="shared" ref="V362" si="406">((SUM(C362:F370))/20)*1.04</f>
+        <f t="shared" ref="V362" si="401">((SUM(C362:F370))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W362">
-        <f t="shared" ref="W362" si="407">(SUM(G362:H370))/10</f>
+        <f t="shared" ref="W362" si="402">(SUM(G362:H370))/10</f>
         <v>18.100000000000001</v>
       </c>
       <c r="X362">
-        <f t="shared" ref="X362" si="408">(SUM(I362:I370))/5</f>
+        <f t="shared" ref="X362" si="403">(SUM(I362:I370))/5</f>
         <v>2.4</v>
       </c>
       <c r="Y362">
-        <f t="shared" ref="Y362" si="409">SUM(K362:K370)-Z362</f>
+        <f t="shared" ref="Y362" si="404">SUM(K362:K370)-Z362</f>
         <v>60</v>
       </c>
       <c r="Z362">
-        <f t="shared" ref="Z362" si="410">SUM(L362:L370)</f>
+        <f t="shared" ref="Z362" si="405">SUM(L362:L370)</f>
         <v>8</v>
       </c>
       <c r="AA362" t="s">
@@ -62358,47 +62356,47 @@
         <v>29</v>
       </c>
       <c r="P371">
-        <f t="shared" ref="P371" si="411">M371*10</f>
+        <f t="shared" ref="P371" si="406">M371*10</f>
         <v>100</v>
       </c>
       <c r="Q371">
-        <f t="shared" ref="Q371" si="412">((SUM(C371:F371))/4)*1.04</f>
+        <f t="shared" ref="Q371" si="407">((SUM(C371:F371))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R371">
-        <f t="shared" ref="R371" si="413">((SUM(C373:F373))/4)*1.04</f>
+        <f t="shared" ref="R371" si="408">((SUM(C373:F373))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S371">
-        <f t="shared" ref="S371" si="414">((SUM(C375:F375))/4)*1.04</f>
+        <f t="shared" ref="S371" si="409">((SUM(C375:F375))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T371">
-        <f t="shared" ref="T371" si="415">((SUM(C377:F377))/4)*1.04</f>
+        <f t="shared" ref="T371" si="410">((SUM(C377:F377))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U371">
-        <f t="shared" ref="U371" si="416">((SUM(C379:F379))/4)*1.04</f>
+        <f t="shared" ref="U371" si="411">((SUM(C379:F379))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V371">
-        <f t="shared" ref="V371" si="417">((SUM(C371:F379))/20)*1.04</f>
+        <f t="shared" ref="V371" si="412">((SUM(C371:F379))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W371">
-        <f t="shared" ref="W371" si="418">(SUM(G371:H379))/10</f>
+        <f t="shared" ref="W371" si="413">(SUM(G371:H379))/10</f>
         <v>88.7</v>
       </c>
       <c r="X371">
-        <f t="shared" ref="X371" si="419">(SUM(I371:I379))/5</f>
+        <f t="shared" ref="X371" si="414">(SUM(I371:I379))/5</f>
         <v>1</v>
       </c>
       <c r="Y371">
-        <f t="shared" ref="Y371" si="420">SUM(K371:K379)-Z371</f>
+        <f t="shared" ref="Y371" si="415">SUM(K371:K379)-Z371</f>
         <v>33</v>
       </c>
       <c r="Z371">
-        <f t="shared" ref="Z371" si="421">SUM(L371:L379)</f>
+        <f t="shared" ref="Z371" si="416">SUM(L371:L379)</f>
         <v>6</v>
       </c>
       <c r="AA371" t="s">
@@ -62852,47 +62850,47 @@
         <v>67</v>
       </c>
       <c r="P380">
-        <f t="shared" ref="P380" si="422">M380*10</f>
+        <f t="shared" ref="P380" si="417">M380*10</f>
         <v>100</v>
       </c>
       <c r="Q380">
-        <f t="shared" ref="Q380" si="423">((SUM(C380:F380))/4)*1.04</f>
+        <f t="shared" ref="Q380" si="418">((SUM(C380:F380))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R380">
-        <f t="shared" ref="R380" si="424">((SUM(C382:F382))/4)*1.04</f>
+        <f t="shared" ref="R380" si="419">((SUM(C382:F382))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S380">
-        <f t="shared" ref="S380" si="425">((SUM(C384:F384))/4)*1.04</f>
+        <f t="shared" ref="S380" si="420">((SUM(C384:F384))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T380">
-        <f t="shared" ref="T380" si="426">((SUM(C386:F386))/4)*1.04</f>
+        <f t="shared" ref="T380" si="421">((SUM(C386:F386))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U380">
-        <f t="shared" ref="U380" si="427">((SUM(C388:F388))/4)*1.04</f>
+        <f t="shared" ref="U380" si="422">((SUM(C388:F388))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V380">
-        <f t="shared" ref="V380" si="428">((SUM(C380:F388))/20)*1.04</f>
+        <f t="shared" ref="V380" si="423">((SUM(C380:F388))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W380">
-        <f t="shared" ref="W380" si="429">(SUM(G380:H388))/10</f>
+        <f t="shared" ref="W380" si="424">(SUM(G380:H388))/10</f>
         <v>35.1</v>
       </c>
       <c r="X380">
-        <f t="shared" ref="X380" si="430">(SUM(I380:I388))/5</f>
+        <f t="shared" ref="X380" si="425">(SUM(I380:I388))/5</f>
         <v>2</v>
       </c>
       <c r="Y380">
-        <f t="shared" ref="Y380" si="431">SUM(K380:K388)-Z380</f>
+        <f t="shared" ref="Y380" si="426">SUM(K380:K388)-Z380</f>
         <v>57</v>
       </c>
       <c r="Z380">
-        <f t="shared" ref="Z380" si="432">SUM(L380:L388)</f>
+        <f t="shared" ref="Z380" si="427">SUM(L380:L388)</f>
         <v>5</v>
       </c>
       <c r="AA380" t="s">
@@ -63350,43 +63348,43 @@
         <v>#VALUE!</v>
       </c>
       <c r="Q389">
-        <f t="shared" ref="Q389" si="433">((SUM(C389:F389))/4)*1.04</f>
+        <f t="shared" ref="Q389" si="428">((SUM(C389:F389))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R389">
-        <f t="shared" ref="R389" si="434">((SUM(C391:F391))/4)*1.04</f>
+        <f t="shared" ref="R389" si="429">((SUM(C391:F391))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S389">
-        <f t="shared" ref="S389" si="435">((SUM(C393:F393))/4)*1.04</f>
+        <f t="shared" ref="S389" si="430">((SUM(C393:F393))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T389">
-        <f t="shared" ref="T389" si="436">((SUM(C395:F395))/4)*1.04</f>
+        <f t="shared" ref="T389" si="431">((SUM(C395:F395))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U389">
-        <f t="shared" ref="U389" si="437">((SUM(C397:F397))/4)*1.04</f>
+        <f t="shared" ref="U389" si="432">((SUM(C397:F397))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V389">
-        <f t="shared" ref="V389" si="438">((SUM(C389:F397))/20)*1.04</f>
+        <f t="shared" ref="V389" si="433">((SUM(C389:F397))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W389">
-        <f t="shared" ref="W389" si="439">(SUM(G389:H397))/10</f>
+        <f t="shared" ref="W389" si="434">(SUM(G389:H397))/10</f>
         <v>1.7</v>
       </c>
       <c r="X389">
-        <f t="shared" ref="X389" si="440">(SUM(I389:I397))/5</f>
+        <f t="shared" ref="X389" si="435">(SUM(I389:I397))/5</f>
         <v>2.4</v>
       </c>
       <c r="Y389">
-        <f t="shared" ref="Y389" si="441">SUM(K389:K397)-Z389</f>
+        <f t="shared" ref="Y389" si="436">SUM(K389:K397)-Z389</f>
         <v>84</v>
       </c>
       <c r="Z389">
-        <f t="shared" ref="Z389" si="442">SUM(L389:L397)</f>
+        <f t="shared" ref="Z389" si="437">SUM(L389:L397)</f>
         <v>11</v>
       </c>
       <c r="AA389" t="s">
@@ -63840,47 +63838,47 @@
         <v>43</v>
       </c>
       <c r="P398">
-        <f t="shared" ref="P398" si="443">M398*10</f>
+        <f t="shared" ref="P398" si="438">M398*10</f>
         <v>40</v>
       </c>
       <c r="Q398">
-        <f t="shared" ref="Q398" si="444">((SUM(C398:F398))/4)*1.04</f>
+        <f t="shared" ref="Q398" si="439">((SUM(C398:F398))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R398">
-        <f t="shared" ref="R398" si="445">((SUM(C400:F400))/4)*1.04</f>
+        <f t="shared" ref="R398" si="440">((SUM(C400:F400))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S398">
-        <f t="shared" ref="S398" si="446">((SUM(C402:F402))/4)*1.04</f>
+        <f t="shared" ref="S398" si="441">((SUM(C402:F402))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T398">
-        <f t="shared" ref="T398" si="447">((SUM(C404:F404))/4)*1.04</f>
+        <f t="shared" ref="T398" si="442">((SUM(C404:F404))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U398">
-        <f t="shared" ref="U398" si="448">((SUM(C406:F406))/4)*1.04</f>
+        <f t="shared" ref="U398" si="443">((SUM(C406:F406))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V398">
-        <f t="shared" ref="V398" si="449">((SUM(C398:F406))/20)*1.04</f>
+        <f t="shared" ref="V398" si="444">((SUM(C398:F406))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W398">
-        <f t="shared" ref="W398" si="450">(SUM(G398:H406))/10</f>
+        <f t="shared" ref="W398" si="445">(SUM(G398:H406))/10</f>
         <v>19.7</v>
       </c>
       <c r="X398">
-        <f t="shared" ref="X398" si="451">(SUM(I398:I406))/5</f>
+        <f t="shared" ref="X398" si="446">(SUM(I398:I406))/5</f>
         <v>3.6</v>
       </c>
       <c r="Y398">
-        <f t="shared" ref="Y398" si="452">SUM(K398:K406)-Z398</f>
+        <f t="shared" ref="Y398" si="447">SUM(K398:K406)-Z398</f>
         <v>68</v>
       </c>
       <c r="Z398">
-        <f t="shared" ref="Z398" si="453">SUM(L398:L406)</f>
+        <f t="shared" ref="Z398" si="448">SUM(L398:L406)</f>
         <v>2</v>
       </c>
       <c r="AA398" t="s">
@@ -64334,47 +64332,47 @@
         <v>67</v>
       </c>
       <c r="P407">
-        <f t="shared" ref="P407" si="454">M407*10</f>
+        <f t="shared" ref="P407" si="449">M407*10</f>
         <v>40</v>
       </c>
       <c r="Q407">
-        <f t="shared" ref="Q407" si="455">((SUM(C407:F407))/4)*1.04</f>
+        <f t="shared" ref="Q407" si="450">((SUM(C407:F407))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R407">
-        <f t="shared" ref="R407" si="456">((SUM(C409:F409))/4)*1.04</f>
+        <f t="shared" ref="R407" si="451">((SUM(C409:F409))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S407">
-        <f t="shared" ref="S407" si="457">((SUM(C411:F411))/4)*1.04</f>
+        <f t="shared" ref="S407" si="452">((SUM(C411:F411))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T407">
-        <f t="shared" ref="T407" si="458">((SUM(C413:F413))/4)*1.04</f>
+        <f t="shared" ref="T407" si="453">((SUM(C413:F413))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U407">
-        <f t="shared" ref="U407" si="459">((SUM(C415:F415))/4)*1.04</f>
+        <f t="shared" ref="U407" si="454">((SUM(C415:F415))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V407">
-        <f t="shared" ref="V407" si="460">((SUM(C407:F415))/20)*1.04</f>
+        <f t="shared" ref="V407" si="455">((SUM(C407:F415))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W407">
-        <f t="shared" ref="W407" si="461">(SUM(G407:H415))/10</f>
+        <f t="shared" ref="W407" si="456">(SUM(G407:H415))/10</f>
         <v>41.3</v>
       </c>
       <c r="X407">
-        <f t="shared" ref="X407" si="462">(SUM(I407:I415))/5</f>
+        <f t="shared" ref="X407" si="457">(SUM(I407:I415))/5</f>
         <v>2.4</v>
       </c>
       <c r="Y407">
-        <f t="shared" ref="Y407" si="463">SUM(K407:K415)-Z407</f>
+        <f t="shared" ref="Y407" si="458">SUM(K407:K415)-Z407</f>
         <v>81</v>
       </c>
       <c r="Z407">
-        <f t="shared" ref="Z407" si="464">SUM(L407:L415)</f>
+        <f t="shared" ref="Z407" si="459">SUM(L407:L415)</f>
         <v>12</v>
       </c>
       <c r="AA407" t="s">
@@ -64828,47 +64826,47 @@
         <v>560</v>
       </c>
       <c r="P416" t="e">
-        <f t="shared" ref="P416" si="465">M416*10</f>
+        <f t="shared" ref="P416" si="460">M416*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q416">
-        <f t="shared" ref="Q416" si="466">((SUM(C416:F416))/4)*1.04</f>
+        <f t="shared" ref="Q416" si="461">((SUM(C416:F416))/4)*1.04</f>
         <v>37.700000000000003</v>
       </c>
       <c r="R416">
-        <f t="shared" ref="R416" si="467">((SUM(C418:F418))/4)*1.04</f>
+        <f t="shared" ref="R416" si="462">((SUM(C418:F418))/4)*1.04</f>
         <v>18.46</v>
       </c>
       <c r="S416">
-        <f t="shared" ref="S416" si="468">((SUM(C420:F420))/4)*1.04</f>
+        <f t="shared" ref="S416" si="463">((SUM(C420:F420))/4)*1.04</f>
         <v>5.2</v>
       </c>
       <c r="T416">
-        <f t="shared" ref="T416" si="469">((SUM(C422:F422))/4)*1.04</f>
+        <f t="shared" ref="T416" si="464">((SUM(C422:F422))/4)*1.04</f>
         <v>7.8000000000000007</v>
       </c>
       <c r="U416">
-        <f t="shared" ref="U416" si="470">((SUM(C424:F424))/4)*1.04</f>
+        <f t="shared" ref="U416" si="465">((SUM(C424:F424))/4)*1.04</f>
         <v>11.96</v>
       </c>
       <c r="V416">
-        <f t="shared" ref="V416" si="471">((SUM(C416:F424))/20)*1.04</f>
+        <f t="shared" ref="V416" si="466">((SUM(C416:F424))/20)*1.04</f>
         <v>16.224</v>
       </c>
       <c r="W416">
-        <f t="shared" ref="W416" si="472">(SUM(G416:H424))/10</f>
+        <f t="shared" ref="W416" si="467">(SUM(G416:H424))/10</f>
         <v>19.5</v>
       </c>
       <c r="X416">
-        <f t="shared" ref="X416" si="473">(SUM(I416:I424))/5</f>
+        <f t="shared" ref="X416" si="468">(SUM(I416:I424))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y416">
-        <f t="shared" ref="Y416" si="474">SUM(K416:K424)-Z416</f>
+        <f t="shared" ref="Y416" si="469">SUM(K416:K424)-Z416</f>
         <v>36</v>
       </c>
       <c r="Z416">
-        <f t="shared" ref="Z416" si="475">SUM(L416:L424)</f>
+        <f t="shared" ref="Z416" si="470">SUM(L416:L424)</f>
         <v>3</v>
       </c>
       <c r="AA416" t="s">
@@ -65322,47 +65320,47 @@
         <v>560</v>
       </c>
       <c r="P425" t="e">
-        <f t="shared" ref="P425" si="476">M425*10</f>
+        <f t="shared" ref="P425" si="471">M425*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q425">
-        <f t="shared" ref="Q425" si="477">((SUM(C425:F425))/4)*1.04</f>
+        <f t="shared" ref="Q425" si="472">((SUM(C425:F425))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R425">
-        <f t="shared" ref="R425" si="478">((SUM(C427:F427))/4)*1.04</f>
+        <f t="shared" ref="R425" si="473">((SUM(C427:F427))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S425">
-        <f t="shared" ref="S425" si="479">((SUM(C429:F429))/4)*1.04</f>
+        <f t="shared" ref="S425" si="474">((SUM(C429:F429))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T425">
-        <f t="shared" ref="T425" si="480">((SUM(C431:F431))/4)*1.04</f>
+        <f t="shared" ref="T425" si="475">((SUM(C431:F431))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U425">
-        <f t="shared" ref="U425" si="481">((SUM(C433:F433))/4)*1.04</f>
+        <f t="shared" ref="U425" si="476">((SUM(C433:F433))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V425">
-        <f t="shared" ref="V425" si="482">((SUM(C425:F433))/20)*1.04</f>
+        <f t="shared" ref="V425" si="477">((SUM(C425:F433))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W425">
-        <f t="shared" ref="W425" si="483">(SUM(G425:H433))/10</f>
+        <f t="shared" ref="W425" si="478">(SUM(G425:H433))/10</f>
         <v>26.2</v>
       </c>
       <c r="X425">
-        <f t="shared" ref="X425" si="484">(SUM(I425:I433))/5</f>
+        <f t="shared" ref="X425" si="479">(SUM(I425:I433))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y425">
-        <f t="shared" ref="Y425" si="485">SUM(K425:K433)-Z425</f>
+        <f t="shared" ref="Y425" si="480">SUM(K425:K433)-Z425</f>
         <v>32</v>
       </c>
       <c r="Z425">
-        <f t="shared" ref="Z425" si="486">SUM(L425:L433)</f>
+        <f t="shared" ref="Z425" si="481">SUM(L425:L433)</f>
         <v>1</v>
       </c>
       <c r="AA425" t="s">
@@ -65816,47 +65814,47 @@
         <v>240</v>
       </c>
       <c r="P434">
-        <f t="shared" ref="P434" si="487">M434*10</f>
+        <f t="shared" ref="P434" si="482">M434*10</f>
         <v>20</v>
       </c>
       <c r="Q434">
-        <f t="shared" ref="Q434" si="488">((SUM(C434:F434))/4)*1.04</f>
+        <f t="shared" ref="Q434" si="483">((SUM(C434:F434))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R434">
-        <f t="shared" ref="R434" si="489">((SUM(C436:F436))/4)*1.04</f>
+        <f t="shared" ref="R434" si="484">((SUM(C436:F436))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S434">
-        <f t="shared" ref="S434" si="490">((SUM(C438:F438))/4)*1.04</f>
+        <f t="shared" ref="S434" si="485">((SUM(C438:F438))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T434">
-        <f t="shared" ref="T434" si="491">((SUM(C440:F440))/4)*1.04</f>
+        <f t="shared" ref="T434" si="486">((SUM(C440:F440))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U434">
-        <f t="shared" ref="U434" si="492">((SUM(C442:F442))/4)*1.04</f>
+        <f t="shared" ref="U434" si="487">((SUM(C442:F442))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V434">
-        <f t="shared" ref="V434" si="493">((SUM(C434:F442))/20)*1.04</f>
+        <f t="shared" ref="V434" si="488">((SUM(C434:F442))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W434">
-        <f t="shared" ref="W434" si="494">(SUM(G434:H442))/10</f>
+        <f t="shared" ref="W434" si="489">(SUM(G434:H442))/10</f>
         <v>10.5</v>
       </c>
       <c r="X434">
-        <f t="shared" ref="X434" si="495">(SUM(I434:I442))/5</f>
+        <f t="shared" ref="X434" si="490">(SUM(I434:I442))/5</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="Y434">
-        <f t="shared" ref="Y434" si="496">SUM(K434:K442)-Z434</f>
+        <f t="shared" ref="Y434" si="491">SUM(K434:K442)-Z434</f>
         <v>15</v>
       </c>
       <c r="Z434">
-        <f t="shared" ref="Z434" si="497">SUM(L434:L442)</f>
+        <f t="shared" ref="Z434" si="492">SUM(L434:L442)</f>
         <v>3</v>
       </c>
       <c r="AA434" t="s">
@@ -66310,47 +66308,47 @@
         <v>240</v>
       </c>
       <c r="P443">
-        <f t="shared" ref="P443" si="498">M443*10</f>
+        <f t="shared" ref="P443" si="493">M443*10</f>
         <v>40</v>
       </c>
       <c r="Q443">
-        <f t="shared" ref="Q443" si="499">((SUM(C443:F443))/4)*1.04</f>
+        <f t="shared" ref="Q443" si="494">((SUM(C443:F443))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R443">
-        <f t="shared" ref="R443" si="500">((SUM(C445:F445))/4)*1.04</f>
+        <f t="shared" ref="R443" si="495">((SUM(C445:F445))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S443">
-        <f t="shared" ref="S443" si="501">((SUM(C447:F447))/4)*1.04</f>
+        <f t="shared" ref="S443" si="496">((SUM(C447:F447))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T443">
-        <f t="shared" ref="T443" si="502">((SUM(C449:F449))/4)*1.04</f>
+        <f t="shared" ref="T443" si="497">((SUM(C449:F449))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U443">
-        <f t="shared" ref="U443" si="503">((SUM(C451:F451))/4)*1.04</f>
+        <f t="shared" ref="U443" si="498">((SUM(C451:F451))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V443">
-        <f t="shared" ref="V443" si="504">((SUM(C443:F451))/20)*1.04</f>
+        <f t="shared" ref="V443" si="499">((SUM(C443:F451))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W443">
-        <f t="shared" ref="W443" si="505">(SUM(G443:H451))/10</f>
+        <f t="shared" ref="W443" si="500">(SUM(G443:H451))/10</f>
         <v>37.5</v>
       </c>
       <c r="X443">
-        <f t="shared" ref="X443" si="506">(SUM(I443:I451))/5</f>
+        <f t="shared" ref="X443" si="501">(SUM(I443:I451))/5</f>
         <v>1.6</v>
       </c>
       <c r="Y443">
-        <f t="shared" ref="Y443" si="507">SUM(K443:K451)-Z443</f>
+        <f t="shared" ref="Y443" si="502">SUM(K443:K451)-Z443</f>
         <v>19</v>
       </c>
       <c r="Z443">
-        <f t="shared" ref="Z443" si="508">SUM(L443:L451)</f>
+        <f t="shared" ref="Z443" si="503">SUM(L443:L451)</f>
         <v>1</v>
       </c>
       <c r="AA443" t="s">
@@ -66804,47 +66802,47 @@
         <v>240</v>
       </c>
       <c r="P452">
-        <f t="shared" ref="P452" si="509">M452*10</f>
+        <f t="shared" ref="P452" si="504">M452*10</f>
         <v>40</v>
       </c>
       <c r="Q452">
-        <f t="shared" ref="Q452" si="510">((SUM(C452:F452))/4)*1.04</f>
+        <f t="shared" ref="Q452" si="505">((SUM(C452:F452))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R452">
-        <f t="shared" ref="R452" si="511">((SUM(C454:F454))/4)*1.04</f>
+        <f t="shared" ref="R452" si="506">((SUM(C454:F454))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S452">
-        <f t="shared" ref="S452" si="512">((SUM(C456:F456))/4)*1.04</f>
+        <f t="shared" ref="S452" si="507">((SUM(C456:F456))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T452">
-        <f t="shared" ref="T452" si="513">((SUM(C458:F458))/4)*1.04</f>
+        <f t="shared" ref="T452" si="508">((SUM(C458:F458))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U452">
-        <f t="shared" ref="U452" si="514">((SUM(C460:F460))/4)*1.04</f>
+        <f t="shared" ref="U452" si="509">((SUM(C460:F460))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V452">
-        <f t="shared" ref="V452" si="515">((SUM(C452:F460))/20)*1.04</f>
+        <f t="shared" ref="V452" si="510">((SUM(C452:F460))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W452">
-        <f t="shared" ref="W452" si="516">(SUM(G452:H460))/10</f>
+        <f t="shared" ref="W452" si="511">(SUM(G452:H460))/10</f>
         <v>14</v>
       </c>
       <c r="X452">
-        <f t="shared" ref="X452" si="517">(SUM(I452:I460))/5</f>
+        <f t="shared" ref="X452" si="512">(SUM(I452:I460))/5</f>
         <v>3.2</v>
       </c>
       <c r="Y452">
-        <f t="shared" ref="Y452" si="518">SUM(K452:K460)-Z452</f>
+        <f t="shared" ref="Y452" si="513">SUM(K452:K460)-Z452</f>
         <v>16</v>
       </c>
       <c r="Z452">
-        <f t="shared" ref="Z452" si="519">SUM(L452:L460)</f>
+        <f t="shared" ref="Z452" si="514">SUM(L452:L460)</f>
         <v>4</v>
       </c>
       <c r="AA452" t="s">
@@ -67298,47 +67296,47 @@
         <v>240</v>
       </c>
       <c r="P461" t="e">
-        <f t="shared" ref="P461" si="520">M461*10</f>
+        <f t="shared" ref="P461" si="515">M461*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q461">
-        <f t="shared" ref="Q461" si="521">((SUM(C461:F461))/4)*1.04</f>
+        <f t="shared" ref="Q461" si="516">((SUM(C461:F461))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R461">
-        <f t="shared" ref="R461" si="522">((SUM(C463:F463))/4)*1.04</f>
+        <f t="shared" ref="R461" si="517">((SUM(C463:F463))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S461">
-        <f t="shared" ref="S461" si="523">((SUM(C465:F465))/4)*1.04</f>
+        <f t="shared" ref="S461" si="518">((SUM(C465:F465))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T461">
-        <f t="shared" ref="T461" si="524">((SUM(C467:F467))/4)*1.04</f>
+        <f t="shared" ref="T461" si="519">((SUM(C467:F467))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U461">
-        <f t="shared" ref="U461" si="525">((SUM(C469:F469))/4)*1.04</f>
+        <f t="shared" ref="U461" si="520">((SUM(C469:F469))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V461">
-        <f t="shared" ref="V461" si="526">((SUM(C461:F469))/20)*1.04</f>
+        <f t="shared" ref="V461" si="521">((SUM(C461:F469))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W461">
-        <f t="shared" ref="W461" si="527">(SUM(G461:H469))/10</f>
+        <f t="shared" ref="W461" si="522">(SUM(G461:H469))/10</f>
         <v>19</v>
       </c>
       <c r="X461">
-        <f t="shared" ref="X461" si="528">(SUM(I461:I469))/5</f>
+        <f t="shared" ref="X461" si="523">(SUM(I461:I469))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y461">
-        <f t="shared" ref="Y461" si="529">SUM(K461:K469)-Z461</f>
+        <f t="shared" ref="Y461" si="524">SUM(K461:K469)-Z461</f>
         <v>33</v>
       </c>
       <c r="Z461">
-        <f t="shared" ref="Z461" si="530">SUM(L461:L469)</f>
+        <f t="shared" ref="Z461" si="525">SUM(L461:L469)</f>
         <v>3</v>
       </c>
       <c r="AA461" t="s">
@@ -67792,47 +67790,47 @@
         <v>240</v>
       </c>
       <c r="P470" t="e">
-        <f t="shared" ref="P470" si="531">M470*10</f>
+        <f t="shared" ref="P470" si="526">M470*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q470">
-        <f t="shared" ref="Q470" si="532">((SUM(C470:F470))/4)*1.04</f>
+        <f t="shared" ref="Q470" si="527">((SUM(C470:F470))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R470">
-        <f t="shared" ref="R470" si="533">((SUM(C472:F472))/4)*1.04</f>
+        <f t="shared" ref="R470" si="528">((SUM(C472:F472))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S470">
-        <f t="shared" ref="S470" si="534">((SUM(C474:F474))/4)*1.04</f>
+        <f t="shared" ref="S470" si="529">((SUM(C474:F474))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T470">
-        <f t="shared" ref="T470" si="535">((SUM(C476:F476))/4)*1.04</f>
+        <f t="shared" ref="T470" si="530">((SUM(C476:F476))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U470">
-        <f t="shared" ref="U470" si="536">((SUM(C478:F478))/4)*1.04</f>
+        <f t="shared" ref="U470" si="531">((SUM(C478:F478))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V470">
-        <f t="shared" ref="V470" si="537">((SUM(C470:F478))/20)*1.04</f>
+        <f t="shared" ref="V470" si="532">((SUM(C470:F478))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W470">
-        <f t="shared" ref="W470" si="538">(SUM(G470:H478))/10</f>
+        <f t="shared" ref="W470" si="533">(SUM(G470:H478))/10</f>
         <v>31</v>
       </c>
       <c r="X470">
-        <f t="shared" ref="X470" si="539">(SUM(I470:I478))/5</f>
+        <f t="shared" ref="X470" si="534">(SUM(I470:I478))/5</f>
         <v>3.4</v>
       </c>
       <c r="Y470">
-        <f t="shared" ref="Y470" si="540">SUM(K470:K478)-Z470</f>
+        <f t="shared" ref="Y470" si="535">SUM(K470:K478)-Z470</f>
         <v>42</v>
       </c>
       <c r="Z470">
-        <f t="shared" ref="Z470" si="541">SUM(L470:L478)</f>
+        <f t="shared" ref="Z470" si="536">SUM(L470:L478)</f>
         <v>4</v>
       </c>
       <c r="AA470" t="s">
@@ -68286,47 +68284,47 @@
         <v>240</v>
       </c>
       <c r="P479" t="e">
-        <f t="shared" ref="P479" si="542">M479*10</f>
+        <f t="shared" ref="P479" si="537">M479*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q479">
-        <f t="shared" ref="Q479" si="543">((SUM(C479:F479))/4)*1.04</f>
+        <f t="shared" ref="Q479" si="538">((SUM(C479:F479))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R479">
-        <f t="shared" ref="R479" si="544">((SUM(C481:F481))/4)*1.04</f>
+        <f t="shared" ref="R479" si="539">((SUM(C481:F481))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S479">
-        <f t="shared" ref="S479" si="545">((SUM(C483:F483))/4)*1.04</f>
+        <f t="shared" ref="S479" si="540">((SUM(C483:F483))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T479">
-        <f t="shared" ref="T479" si="546">((SUM(C485:F485))/4)*1.04</f>
+        <f t="shared" ref="T479" si="541">((SUM(C485:F485))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U479">
-        <f t="shared" ref="U479" si="547">((SUM(C487:F487))/4)*1.04</f>
+        <f t="shared" ref="U479" si="542">((SUM(C487:F487))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V479">
-        <f t="shared" ref="V479" si="548">((SUM(C479:F487))/20)*1.04</f>
+        <f t="shared" ref="V479" si="543">((SUM(C479:F487))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W479">
-        <f t="shared" ref="W479" si="549">(SUM(G479:H487))/10</f>
+        <f t="shared" ref="W479" si="544">(SUM(G479:H487))/10</f>
         <v>7</v>
       </c>
       <c r="X479">
-        <f t="shared" ref="X479" si="550">(SUM(I479:I487))/5</f>
+        <f t="shared" ref="X479" si="545">(SUM(I479:I487))/5</f>
         <v>2.6</v>
       </c>
       <c r="Y479">
-        <f t="shared" ref="Y479" si="551">SUM(K479:K487)-Z479</f>
+        <f t="shared" ref="Y479" si="546">SUM(K479:K487)-Z479</f>
         <v>26</v>
       </c>
       <c r="Z479">
-        <f t="shared" ref="Z479" si="552">SUM(L479:L487)</f>
+        <f t="shared" ref="Z479" si="547">SUM(L479:L487)</f>
         <v>2</v>
       </c>
       <c r="AA479" t="s">
@@ -68780,47 +68778,47 @@
         <v>29</v>
       </c>
       <c r="P488">
-        <f t="shared" ref="P488" si="553">M488*10</f>
+        <f t="shared" ref="P488" si="548">M488*10</f>
         <v>80</v>
       </c>
       <c r="Q488">
-        <f t="shared" ref="Q488" si="554">((SUM(C488:F488))/4)*1.04</f>
+        <f t="shared" ref="Q488" si="549">((SUM(C488:F488))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R488">
-        <f t="shared" ref="R488" si="555">((SUM(C490:F490))/4)*1.04</f>
+        <f t="shared" ref="R488" si="550">((SUM(C490:F490))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S488">
-        <f t="shared" ref="S488" si="556">((SUM(C492:F492))/4)*1.04</f>
+        <f t="shared" ref="S488" si="551">((SUM(C492:F492))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T488">
-        <f t="shared" ref="T488" si="557">((SUM(C494:F494))/4)*1.04</f>
+        <f t="shared" ref="T488" si="552">((SUM(C494:F494))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U488">
-        <f t="shared" ref="U488" si="558">((SUM(C496:F496))/4)*1.04</f>
+        <f t="shared" ref="U488" si="553">((SUM(C496:F496))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V488">
-        <f t="shared" ref="V488" si="559">((SUM(C488:F496))/20)*1.04</f>
+        <f t="shared" ref="V488" si="554">((SUM(C488:F496))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W488">
-        <f t="shared" ref="W488" si="560">(SUM(G488:H496))/10</f>
+        <f t="shared" ref="W488" si="555">(SUM(G488:H496))/10</f>
         <v>43.5</v>
       </c>
       <c r="X488">
-        <f t="shared" ref="X488" si="561">(SUM(I488:I496))/5</f>
+        <f t="shared" ref="X488" si="556">(SUM(I488:I496))/5</f>
         <v>2</v>
       </c>
       <c r="Y488">
-        <f t="shared" ref="Y488" si="562">SUM(K488:K496)-Z488</f>
+        <f t="shared" ref="Y488" si="557">SUM(K488:K496)-Z488</f>
         <v>10</v>
       </c>
       <c r="Z488">
-        <f t="shared" ref="Z488" si="563">SUM(L488:L496)</f>
+        <f t="shared" ref="Z488" si="558">SUM(L488:L496)</f>
         <v>8</v>
       </c>
       <c r="AA488" t="s">
@@ -69274,47 +69272,47 @@
         <v>43</v>
       </c>
       <c r="P497">
-        <f t="shared" ref="P497" si="564">M497*10</f>
+        <f t="shared" ref="P497" si="559">M497*10</f>
         <v>50</v>
       </c>
       <c r="Q497">
-        <f t="shared" ref="Q497" si="565">((SUM(C497:F497))/4)*1.04</f>
+        <f t="shared" ref="Q497" si="560">((SUM(C497:F497))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R497">
-        <f t="shared" ref="R497" si="566">((SUM(C499:F499))/4)*1.04</f>
+        <f t="shared" ref="R497" si="561">((SUM(C499:F499))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S497">
-        <f t="shared" ref="S497" si="567">((SUM(C501:F501))/4)*1.04</f>
+        <f t="shared" ref="S497" si="562">((SUM(C501:F501))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T497">
-        <f t="shared" ref="T497" si="568">((SUM(C503:F503))/4)*1.04</f>
+        <f t="shared" ref="T497" si="563">((SUM(C503:F503))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U497">
-        <f t="shared" ref="U497" si="569">((SUM(C505:F505))/4)*1.04</f>
+        <f t="shared" ref="U497" si="564">((SUM(C505:F505))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V497">
-        <f t="shared" ref="V497" si="570">((SUM(C497:F505))/20)*1.04</f>
+        <f t="shared" ref="V497" si="565">((SUM(C497:F505))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W497">
-        <f t="shared" ref="W497" si="571">(SUM(G497:H505))/10</f>
+        <f t="shared" ref="W497" si="566">(SUM(G497:H505))/10</f>
         <v>81</v>
       </c>
       <c r="X497">
-        <f t="shared" ref="X497" si="572">(SUM(I497:I505))/5</f>
+        <f t="shared" ref="X497" si="567">(SUM(I497:I505))/5</f>
         <v>1.6</v>
       </c>
       <c r="Y497">
-        <f t="shared" ref="Y497" si="573">SUM(K497:K505)-Z497</f>
+        <f t="shared" ref="Y497" si="568">SUM(K497:K505)-Z497</f>
         <v>30</v>
       </c>
       <c r="Z497">
-        <f t="shared" ref="Z497" si="574">SUM(L497:L505)</f>
+        <f t="shared" ref="Z497" si="569">SUM(L497:L505)</f>
         <v>0</v>
       </c>
       <c r="AA497" t="s">
@@ -69768,47 +69766,47 @@
         <v>784</v>
       </c>
       <c r="P506">
-        <f t="shared" ref="P506" si="575">M506*10</f>
+        <f t="shared" ref="P506" si="570">M506*10</f>
         <v>100</v>
       </c>
       <c r="Q506">
-        <f t="shared" ref="Q506" si="576">((SUM(C506:F506))/4)*1.04</f>
+        <f t="shared" ref="Q506" si="571">((SUM(C506:F506))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R506">
-        <f t="shared" ref="R506" si="577">((SUM(C508:F508))/4)*1.04</f>
+        <f t="shared" ref="R506" si="572">((SUM(C508:F508))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S506">
-        <f t="shared" ref="S506" si="578">((SUM(C510:F510))/4)*1.04</f>
+        <f t="shared" ref="S506" si="573">((SUM(C510:F510))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T506">
-        <f t="shared" ref="T506" si="579">((SUM(C512:F512))/4)*1.04</f>
+        <f t="shared" ref="T506" si="574">((SUM(C512:F512))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U506">
-        <f t="shared" ref="U506" si="580">((SUM(C514:F514))/4)*1.04</f>
+        <f t="shared" ref="U506" si="575">((SUM(C514:F514))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V506">
-        <f t="shared" ref="V506" si="581">((SUM(C506:F514))/20)*1.04</f>
+        <f t="shared" ref="V506" si="576">((SUM(C506:F514))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W506">
-        <f t="shared" ref="W506" si="582">(SUM(G506:H514))/10</f>
+        <f t="shared" ref="W506" si="577">(SUM(G506:H514))/10</f>
         <v>16.2</v>
       </c>
       <c r="X506">
-        <f t="shared" ref="X506" si="583">(SUM(I506:I514))/5</f>
+        <f t="shared" ref="X506" si="578">(SUM(I506:I514))/5</f>
         <v>2</v>
       </c>
       <c r="Y506">
-        <f t="shared" ref="Y506" si="584">SUM(K506:K514)-Z506</f>
+        <f t="shared" ref="Y506" si="579">SUM(K506:K514)-Z506</f>
         <v>69</v>
       </c>
       <c r="Z506">
-        <f t="shared" ref="Z506" si="585">SUM(L506:L514)</f>
+        <f t="shared" ref="Z506" si="580">SUM(L506:L514)</f>
         <v>10</v>
       </c>
       <c r="AA506" t="s">
@@ -70262,47 +70260,47 @@
         <v>240</v>
       </c>
       <c r="P515">
-        <f t="shared" ref="P515" si="586">M515*10</f>
+        <f t="shared" ref="P515" si="581">M515*10</f>
         <v>30</v>
       </c>
       <c r="Q515">
-        <f t="shared" ref="Q515" si="587">((SUM(C515:F515))/4)*1.04</f>
+        <f t="shared" ref="Q515" si="582">((SUM(C515:F515))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R515">
-        <f t="shared" ref="R515" si="588">((SUM(C517:F517))/4)*1.04</f>
+        <f t="shared" ref="R515" si="583">((SUM(C517:F517))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S515">
-        <f t="shared" ref="S515" si="589">((SUM(C519:F519))/4)*1.04</f>
+        <f t="shared" ref="S515" si="584">((SUM(C519:F519))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T515">
-        <f t="shared" ref="T515" si="590">((SUM(C521:F521))/4)*1.04</f>
+        <f t="shared" ref="T515" si="585">((SUM(C521:F521))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U515">
-        <f t="shared" ref="U515" si="591">((SUM(C523:F523))/4)*1.04</f>
+        <f t="shared" ref="U515" si="586">((SUM(C523:F523))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V515">
-        <f t="shared" ref="V515" si="592">((SUM(C515:F523))/20)*1.04</f>
+        <f t="shared" ref="V515" si="587">((SUM(C515:F523))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W515">
-        <f t="shared" ref="W515" si="593">(SUM(G515:H523))/10</f>
+        <f t="shared" ref="W515" si="588">(SUM(G515:H523))/10</f>
         <v>5.5</v>
       </c>
       <c r="X515">
-        <f t="shared" ref="X515" si="594">(SUM(I515:I523))/5</f>
+        <f t="shared" ref="X515" si="589">(SUM(I515:I523))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y515">
-        <f t="shared" ref="Y515" si="595">SUM(K515:K523)-Z515</f>
+        <f t="shared" ref="Y515" si="590">SUM(K515:K523)-Z515</f>
         <v>23</v>
       </c>
       <c r="Z515">
-        <f t="shared" ref="Z515" si="596">SUM(L515:L523)</f>
+        <f t="shared" ref="Z515" si="591">SUM(L515:L523)</f>
         <v>3</v>
       </c>
       <c r="AA515" t="s">
@@ -70756,47 +70754,47 @@
         <v>240</v>
       </c>
       <c r="P524">
-        <f t="shared" ref="P524" si="597">M524*10</f>
+        <f t="shared" ref="P524" si="592">M524*10</f>
         <v>60</v>
       </c>
       <c r="Q524">
-        <f t="shared" ref="Q524" si="598">((SUM(C524:F524))/4)*1.04</f>
+        <f t="shared" ref="Q524" si="593">((SUM(C524:F524))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R524">
-        <f t="shared" ref="R524" si="599">((SUM(C526:F526))/4)*1.04</f>
+        <f t="shared" ref="R524" si="594">((SUM(C526:F526))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S524">
-        <f t="shared" ref="S524" si="600">((SUM(C528:F528))/4)*1.04</f>
+        <f t="shared" ref="S524" si="595">((SUM(C528:F528))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T524">
-        <f t="shared" ref="T524" si="601">((SUM(C530:F530))/4)*1.04</f>
+        <f t="shared" ref="T524" si="596">((SUM(C530:F530))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U524">
-        <f t="shared" ref="U524" si="602">((SUM(C532:F532))/4)*1.04</f>
+        <f t="shared" ref="U524" si="597">((SUM(C532:F532))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V524">
-        <f t="shared" ref="V524" si="603">((SUM(C524:F532))/20)*1.04</f>
+        <f t="shared" ref="V524" si="598">((SUM(C524:F532))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W524">
-        <f t="shared" ref="W524" si="604">(SUM(G524:H532))/10</f>
+        <f t="shared" ref="W524" si="599">(SUM(G524:H532))/10</f>
         <v>11</v>
       </c>
       <c r="X524">
-        <f t="shared" ref="X524" si="605">(SUM(I524:I532))/5</f>
+        <f t="shared" ref="X524" si="600">(SUM(I524:I532))/5</f>
         <v>2.4</v>
       </c>
       <c r="Y524">
-        <f t="shared" ref="Y524" si="606">SUM(K524:K532)-Z524</f>
+        <f t="shared" ref="Y524" si="601">SUM(K524:K532)-Z524</f>
         <v>23</v>
       </c>
       <c r="Z524">
-        <f t="shared" ref="Z524" si="607">SUM(L524:L532)</f>
+        <f t="shared" ref="Z524" si="602">SUM(L524:L532)</f>
         <v>3</v>
       </c>
       <c r="AA524" t="s">
@@ -71250,47 +71248,47 @@
         <v>240</v>
       </c>
       <c r="P533">
-        <f t="shared" ref="P533" si="608">M533*10</f>
+        <f t="shared" ref="P533" si="603">M533*10</f>
         <v>70</v>
       </c>
       <c r="Q533">
-        <f t="shared" ref="Q533" si="609">((SUM(C533:F533))/4)*1.04</f>
+        <f t="shared" ref="Q533" si="604">((SUM(C533:F533))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R533">
-        <f t="shared" ref="R533" si="610">((SUM(C535:F535))/4)*1.04</f>
+        <f t="shared" ref="R533" si="605">((SUM(C535:F535))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S533">
-        <f t="shared" ref="S533" si="611">((SUM(C537:F537))/4)*1.04</f>
+        <f t="shared" ref="S533" si="606">((SUM(C537:F537))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T533">
-        <f t="shared" ref="T533" si="612">((SUM(C539:F539))/4)*1.04</f>
+        <f t="shared" ref="T533" si="607">((SUM(C539:F539))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U533">
-        <f t="shared" ref="U533" si="613">((SUM(C541:F541))/4)*1.04</f>
+        <f t="shared" ref="U533" si="608">((SUM(C541:F541))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V533">
-        <f t="shared" ref="V533" si="614">((SUM(C533:F541))/20)*1.04</f>
+        <f t="shared" ref="V533" si="609">((SUM(C533:F541))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W533">
-        <f t="shared" ref="W533" si="615">(SUM(G533:H541))/10</f>
+        <f t="shared" ref="W533" si="610">(SUM(G533:H541))/10</f>
         <v>4.5</v>
       </c>
       <c r="X533">
-        <f t="shared" ref="X533" si="616">(SUM(I533:I541))/5</f>
+        <f t="shared" ref="X533" si="611">(SUM(I533:I541))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y533">
-        <f t="shared" ref="Y533" si="617">SUM(K533:K541)-Z533</f>
+        <f t="shared" ref="Y533" si="612">SUM(K533:K541)-Z533</f>
         <v>19</v>
       </c>
       <c r="Z533">
-        <f t="shared" ref="Z533" si="618">SUM(L533:L541)</f>
+        <f t="shared" ref="Z533" si="613">SUM(L533:L541)</f>
         <v>4</v>
       </c>
       <c r="AA533" t="s">
@@ -71744,47 +71742,47 @@
         <v>240</v>
       </c>
       <c r="P542">
-        <f t="shared" ref="P542" si="619">M542*10</f>
+        <f t="shared" ref="P542" si="614">M542*10</f>
         <v>50</v>
       </c>
       <c r="Q542">
-        <f t="shared" ref="Q542" si="620">((SUM(C542:F542))/4)*1.04</f>
+        <f t="shared" ref="Q542" si="615">((SUM(C542:F542))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R542">
-        <f t="shared" ref="R542" si="621">((SUM(C544:F544))/4)*1.04</f>
+        <f t="shared" ref="R542" si="616">((SUM(C544:F544))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S542">
-        <f t="shared" ref="S542" si="622">((SUM(C546:F546))/4)*1.04</f>
+        <f t="shared" ref="S542" si="617">((SUM(C546:F546))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T542">
-        <f t="shared" ref="T542" si="623">((SUM(C548:F548))/4)*1.04</f>
+        <f t="shared" ref="T542" si="618">((SUM(C548:F548))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U542">
-        <f t="shared" ref="U542" si="624">((SUM(C550:F550))/4)*1.04</f>
+        <f t="shared" ref="U542" si="619">((SUM(C550:F550))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V542">
-        <f t="shared" ref="V542" si="625">((SUM(C542:F550))/20)*1.04</f>
+        <f t="shared" ref="V542" si="620">((SUM(C542:F550))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W542">
-        <f t="shared" ref="W542" si="626">(SUM(G542:H550))/10</f>
+        <f t="shared" ref="W542" si="621">(SUM(G542:H550))/10</f>
         <v>35.5</v>
       </c>
       <c r="X542">
-        <f t="shared" ref="X542" si="627">(SUM(I542:I550))/5</f>
+        <f t="shared" ref="X542" si="622">(SUM(I542:I550))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y542">
-        <f t="shared" ref="Y542" si="628">SUM(K542:K550)-Z542</f>
+        <f t="shared" ref="Y542" si="623">SUM(K542:K550)-Z542</f>
         <v>10</v>
       </c>
       <c r="Z542">
-        <f t="shared" ref="Z542" si="629">SUM(L542:L550)</f>
+        <f t="shared" ref="Z542" si="624">SUM(L542:L550)</f>
         <v>0</v>
       </c>
       <c r="AA542" t="s">
@@ -72238,47 +72236,47 @@
         <v>240</v>
       </c>
       <c r="P551">
-        <f t="shared" ref="P551" si="630">M551*10</f>
+        <f t="shared" ref="P551" si="625">M551*10</f>
         <v>50</v>
       </c>
       <c r="Q551">
-        <f t="shared" ref="Q551" si="631">((SUM(C551:F551))/4)*1.04</f>
+        <f t="shared" ref="Q551" si="626">((SUM(C551:F551))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R551">
-        <f t="shared" ref="R551" si="632">((SUM(C553:F553))/4)*1.04</f>
+        <f t="shared" ref="R551" si="627">((SUM(C553:F553))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S551">
-        <f t="shared" ref="S551" si="633">((SUM(C555:F555))/4)*1.04</f>
+        <f t="shared" ref="S551" si="628">((SUM(C555:F555))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T551">
-        <f t="shared" ref="T551" si="634">((SUM(C557:F557))/4)*1.04</f>
+        <f t="shared" ref="T551" si="629">((SUM(C557:F557))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U551">
-        <f t="shared" ref="U551" si="635">((SUM(C559:F559))/4)*1.04</f>
+        <f t="shared" ref="U551" si="630">((SUM(C559:F559))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V551">
-        <f t="shared" ref="V551" si="636">((SUM(C551:F559))/20)*1.04</f>
+        <f t="shared" ref="V551" si="631">((SUM(C551:F559))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W551">
-        <f t="shared" ref="W551" si="637">(SUM(G551:H559))/10</f>
+        <f t="shared" ref="W551" si="632">(SUM(G551:H559))/10</f>
         <v>49</v>
       </c>
       <c r="X551">
-        <f t="shared" ref="X551" si="638">(SUM(I551:I559))/5</f>
+        <f t="shared" ref="X551" si="633">(SUM(I551:I559))/5</f>
         <v>2.6</v>
       </c>
       <c r="Y551">
-        <f t="shared" ref="Y551" si="639">SUM(K551:K559)-Z551</f>
+        <f t="shared" ref="Y551" si="634">SUM(K551:K559)-Z551</f>
         <v>17</v>
       </c>
       <c r="Z551">
-        <f t="shared" ref="Z551" si="640">SUM(L551:L559)</f>
+        <f t="shared" ref="Z551" si="635">SUM(L551:L559)</f>
         <v>0</v>
       </c>
       <c r="AA551" t="s">
@@ -72732,47 +72730,47 @@
         <v>29</v>
       </c>
       <c r="P560">
-        <f t="shared" ref="P560" si="641">M560*10</f>
+        <f t="shared" ref="P560" si="636">M560*10</f>
         <v>70</v>
       </c>
       <c r="Q560">
-        <f t="shared" ref="Q560" si="642">((SUM(C560:F560))/4)*1.04</f>
+        <f t="shared" ref="Q560" si="637">((SUM(C560:F560))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R560">
-        <f t="shared" ref="R560" si="643">((SUM(C562:F562))/4)*1.04</f>
+        <f t="shared" ref="R560" si="638">((SUM(C562:F562))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S560">
-        <f t="shared" ref="S560" si="644">((SUM(C564:F564))/4)*1.04</f>
+        <f t="shared" ref="S560" si="639">((SUM(C564:F564))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T560">
-        <f t="shared" ref="T560" si="645">((SUM(C566:F566))/4)*1.04</f>
+        <f t="shared" ref="T560" si="640">((SUM(C566:F566))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U560">
-        <f t="shared" ref="U560" si="646">((SUM(C568:F568))/4)*1.04</f>
+        <f t="shared" ref="U560" si="641">((SUM(C568:F568))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V560">
-        <f t="shared" ref="V560" si="647">((SUM(C560:F568))/20)*1.04</f>
+        <f t="shared" ref="V560" si="642">((SUM(C560:F568))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W560">
-        <f t="shared" ref="W560" si="648">(SUM(G560:H568))/10</f>
+        <f t="shared" ref="W560" si="643">(SUM(G560:H568))/10</f>
         <v>11.8</v>
       </c>
       <c r="X560">
-        <f t="shared" ref="X560" si="649">(SUM(I560:I568))/5</f>
+        <f t="shared" ref="X560" si="644">(SUM(I560:I568))/5</f>
         <v>2</v>
       </c>
       <c r="Y560">
-        <f t="shared" ref="Y560" si="650">SUM(K560:K568)-Z560</f>
+        <f t="shared" ref="Y560" si="645">SUM(K560:K568)-Z560</f>
         <v>10</v>
       </c>
       <c r="Z560">
-        <f t="shared" ref="Z560" si="651">SUM(L560:L568)</f>
+        <f t="shared" ref="Z560" si="646">SUM(L560:L568)</f>
         <v>7</v>
       </c>
       <c r="AA560" t="s">
@@ -73226,47 +73224,47 @@
         <v>29</v>
       </c>
       <c r="P569" t="e">
-        <f t="shared" ref="P569" si="652">M569*10</f>
+        <f t="shared" ref="P569" si="647">M569*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q569">
-        <f t="shared" ref="Q569" si="653">((SUM(C569:F569))/4)*1.04</f>
+        <f t="shared" ref="Q569" si="648">((SUM(C569:F569))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R569">
-        <f t="shared" ref="R569" si="654">((SUM(C571:F571))/4)*1.04</f>
+        <f t="shared" ref="R569" si="649">((SUM(C571:F571))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S569">
-        <f t="shared" ref="S569" si="655">((SUM(C573:F573))/4)*1.04</f>
+        <f t="shared" ref="S569" si="650">((SUM(C573:F573))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T569">
-        <f t="shared" ref="T569" si="656">((SUM(C575:F575))/4)*1.04</f>
+        <f t="shared" ref="T569" si="651">((SUM(C575:F575))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U569">
-        <f t="shared" ref="U569" si="657">((SUM(C577:F577))/4)*1.04</f>
+        <f t="shared" ref="U569" si="652">((SUM(C577:F577))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V569">
-        <f t="shared" ref="V569" si="658">((SUM(C569:F577))/20)*1.04</f>
+        <f t="shared" ref="V569" si="653">((SUM(C569:F577))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W569">
-        <f t="shared" ref="W569" si="659">(SUM(G569:H577))/10</f>
+        <f t="shared" ref="W569" si="654">(SUM(G569:H577))/10</f>
         <v>3</v>
       </c>
       <c r="X569">
-        <f t="shared" ref="X569" si="660">(SUM(I569:I577))/5</f>
+        <f t="shared" ref="X569" si="655">(SUM(I569:I577))/5</f>
         <v>2.4</v>
       </c>
       <c r="Y569">
-        <f t="shared" ref="Y569" si="661">SUM(K569:K577)-Z569</f>
+        <f t="shared" ref="Y569" si="656">SUM(K569:K577)-Z569</f>
         <v>7</v>
       </c>
       <c r="Z569">
-        <f t="shared" ref="Z569" si="662">SUM(L569:L577)</f>
+        <f t="shared" ref="Z569" si="657">SUM(L569:L577)</f>
         <v>7</v>
       </c>
       <c r="AA569" t="s">
@@ -73720,47 +73718,47 @@
         <v>29</v>
       </c>
       <c r="P578">
-        <f t="shared" ref="P578" si="663">M578*10</f>
+        <f t="shared" ref="P578" si="658">M578*10</f>
         <v>120</v>
       </c>
       <c r="Q578">
-        <f t="shared" ref="Q578" si="664">((SUM(C578:F578))/4)*1.04</f>
+        <f t="shared" ref="Q578" si="659">((SUM(C578:F578))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R578">
-        <f t="shared" ref="R578" si="665">((SUM(C580:F580))/4)*1.04</f>
+        <f t="shared" ref="R578" si="660">((SUM(C580:F580))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S578">
-        <f t="shared" ref="S578" si="666">((SUM(C582:F582))/4)*1.04</f>
+        <f t="shared" ref="S578" si="661">((SUM(C582:F582))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T578">
-        <f t="shared" ref="T578" si="667">((SUM(C584:F584))/4)*1.04</f>
+        <f t="shared" ref="T578" si="662">((SUM(C584:F584))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U578">
-        <f t="shared" ref="U578" si="668">((SUM(C586:F586))/4)*1.04</f>
+        <f t="shared" ref="U578" si="663">((SUM(C586:F586))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V578">
-        <f t="shared" ref="V578" si="669">((SUM(C578:F586))/20)*1.04</f>
+        <f t="shared" ref="V578" si="664">((SUM(C578:F586))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W578">
-        <f t="shared" ref="W578" si="670">(SUM(G578:H586))/10</f>
+        <f t="shared" ref="W578" si="665">(SUM(G578:H586))/10</f>
         <v>0.3</v>
       </c>
       <c r="X578">
-        <f t="shared" ref="X578" si="671">(SUM(I578:I586))/5</f>
+        <f t="shared" ref="X578" si="666">(SUM(I578:I586))/5</f>
         <v>1.4</v>
       </c>
       <c r="Y578">
-        <f t="shared" ref="Y578" si="672">SUM(K578:K586)-Z578</f>
+        <f t="shared" ref="Y578" si="667">SUM(K578:K586)-Z578</f>
         <v>77</v>
       </c>
       <c r="Z578">
-        <f t="shared" ref="Z578" si="673">SUM(L578:L586)</f>
+        <f t="shared" ref="Z578" si="668">SUM(L578:L586)</f>
         <v>10</v>
       </c>
       <c r="AA578" t="s">
@@ -74214,47 +74212,47 @@
         <v>29</v>
       </c>
       <c r="P587">
-        <f t="shared" ref="P587" si="674">M587*10</f>
+        <f t="shared" ref="P587" si="669">M587*10</f>
         <v>160</v>
       </c>
       <c r="Q587">
-        <f t="shared" ref="Q587" si="675">((SUM(C587:F587))/4)*1.04</f>
+        <f t="shared" ref="Q587" si="670">((SUM(C587:F587))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R587">
-        <f t="shared" ref="R587" si="676">((SUM(C589:F589))/4)*1.04</f>
+        <f t="shared" ref="R587" si="671">((SUM(C589:F589))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S587">
-        <f t="shared" ref="S587" si="677">((SUM(C591:F591))/4)*1.04</f>
+        <f t="shared" ref="S587" si="672">((SUM(C591:F591))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T587">
-        <f t="shared" ref="T587" si="678">((SUM(C593:F593))/4)*1.04</f>
+        <f t="shared" ref="T587" si="673">((SUM(C593:F593))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U587">
-        <f t="shared" ref="U587" si="679">((SUM(C595:F595))/4)*1.04</f>
+        <f t="shared" ref="U587" si="674">((SUM(C595:F595))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V587">
-        <f t="shared" ref="V587" si="680">((SUM(C587:F595))/20)*1.04</f>
+        <f t="shared" ref="V587" si="675">((SUM(C587:F595))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W587">
-        <f t="shared" ref="W587" si="681">(SUM(G587:H595))/10</f>
+        <f t="shared" ref="W587" si="676">(SUM(G587:H595))/10</f>
         <v>0.5</v>
       </c>
       <c r="X587">
-        <f t="shared" ref="X587" si="682">(SUM(I587:I595))/5</f>
+        <f t="shared" ref="X587" si="677">(SUM(I587:I595))/5</f>
         <v>1.6</v>
       </c>
       <c r="Y587">
-        <f t="shared" ref="Y587" si="683">SUM(K587:K595)-Z587</f>
+        <f t="shared" ref="Y587" si="678">SUM(K587:K595)-Z587</f>
         <v>62</v>
       </c>
       <c r="Z587">
-        <f t="shared" ref="Z587" si="684">SUM(L587:L595)</f>
+        <f t="shared" ref="Z587" si="679">SUM(L587:L595)</f>
         <v>14</v>
       </c>
       <c r="AA587" t="s">
@@ -74708,47 +74706,47 @@
         <v>29</v>
       </c>
       <c r="P596">
-        <f t="shared" ref="P596" si="685">M596*10</f>
+        <f t="shared" ref="P596" si="680">M596*10</f>
         <v>150</v>
       </c>
       <c r="Q596">
-        <f t="shared" ref="Q596" si="686">((SUM(C596:F596))/4)*1.04</f>
+        <f t="shared" ref="Q596" si="681">((SUM(C596:F596))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R596">
-        <f t="shared" ref="R596" si="687">((SUM(C598:F598))/4)*1.04</f>
+        <f t="shared" ref="R596" si="682">((SUM(C598:F598))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S596">
-        <f t="shared" ref="S596" si="688">((SUM(C600:F600))/4)*1.04</f>
+        <f t="shared" ref="S596" si="683">((SUM(C600:F600))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T596">
-        <f t="shared" ref="T596" si="689">((SUM(C602:F602))/4)*1.04</f>
+        <f t="shared" ref="T596" si="684">((SUM(C602:F602))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U596">
-        <f t="shared" ref="U596" si="690">((SUM(C604:F604))/4)*1.04</f>
+        <f t="shared" ref="U596" si="685">((SUM(C604:F604))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V596">
-        <f t="shared" ref="V596" si="691">((SUM(C596:F604))/20)*1.04</f>
+        <f t="shared" ref="V596" si="686">((SUM(C596:F604))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W596">
-        <f t="shared" ref="W596" si="692">(SUM(G596:H604))/10</f>
+        <f t="shared" ref="W596" si="687">(SUM(G596:H604))/10</f>
         <v>9.8000000000000007</v>
       </c>
       <c r="X596">
-        <f t="shared" ref="X596" si="693">(SUM(I596:I604))/5</f>
+        <f t="shared" ref="X596" si="688">(SUM(I596:I604))/5</f>
         <v>2</v>
       </c>
       <c r="Y596">
-        <f t="shared" ref="Y596" si="694">SUM(K596:K604)-Z596</f>
+        <f t="shared" ref="Y596" si="689">SUM(K596:K604)-Z596</f>
         <v>29</v>
       </c>
       <c r="Z596">
-        <f t="shared" ref="Z596" si="695">SUM(L596:L604)</f>
+        <f t="shared" ref="Z596" si="690">SUM(L596:L604)</f>
         <v>8</v>
       </c>
       <c r="AA596" t="s">
@@ -75202,47 +75200,47 @@
         <v>29</v>
       </c>
       <c r="P605">
-        <f t="shared" ref="P605" si="696">M605*10</f>
+        <f t="shared" ref="P605" si="691">M605*10</f>
         <v>190</v>
       </c>
       <c r="Q605">
-        <f t="shared" ref="Q605" si="697">((SUM(C605:F605))/4)*1.04</f>
+        <f t="shared" ref="Q605" si="692">((SUM(C605:F605))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R605">
-        <f t="shared" ref="R605" si="698">((SUM(C607:F607))/4)*1.04</f>
+        <f t="shared" ref="R605" si="693">((SUM(C607:F607))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S605">
-        <f t="shared" ref="S605" si="699">((SUM(C609:F609))/4)*1.04</f>
+        <f t="shared" ref="S605" si="694">((SUM(C609:F609))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T605">
-        <f t="shared" ref="T605" si="700">((SUM(C611:F611))/4)*1.04</f>
+        <f t="shared" ref="T605" si="695">((SUM(C611:F611))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U605">
-        <f t="shared" ref="U605" si="701">((SUM(C613:F613))/4)*1.04</f>
+        <f t="shared" ref="U605" si="696">((SUM(C613:F613))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V605">
-        <f t="shared" ref="V605" si="702">((SUM(C605:F613))/20)*1.04</f>
+        <f t="shared" ref="V605" si="697">((SUM(C605:F613))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W605">
-        <f t="shared" ref="W605" si="703">(SUM(G605:H613))/10</f>
+        <f t="shared" ref="W605" si="698">(SUM(G605:H613))/10</f>
         <v>1.8</v>
       </c>
       <c r="X605">
-        <f t="shared" ref="X605" si="704">(SUM(I605:I613))/5</f>
+        <f t="shared" ref="X605" si="699">(SUM(I605:I613))/5</f>
         <v>3</v>
       </c>
       <c r="Y605">
-        <f t="shared" ref="Y605" si="705">SUM(K605:K613)-Z605</f>
+        <f t="shared" ref="Y605" si="700">SUM(K605:K613)-Z605</f>
         <v>93</v>
       </c>
       <c r="Z605">
-        <f t="shared" ref="Z605" si="706">SUM(L605:L613)</f>
+        <f t="shared" ref="Z605" si="701">SUM(L605:L613)</f>
         <v>2</v>
       </c>
       <c r="AA605" t="s">
@@ -75696,47 +75694,47 @@
         <v>29</v>
       </c>
       <c r="P614" t="e">
-        <f t="shared" ref="P614" si="707">M614*10</f>
+        <f t="shared" ref="P614" si="702">M614*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q614">
-        <f t="shared" ref="Q614" si="708">((SUM(C614:F614))/4)*1.04</f>
+        <f t="shared" ref="Q614" si="703">((SUM(C614:F614))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R614">
-        <f t="shared" ref="R614" si="709">((SUM(C616:F616))/4)*1.04</f>
+        <f t="shared" ref="R614" si="704">((SUM(C616:F616))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S614">
-        <f t="shared" ref="S614" si="710">((SUM(C618:F618))/4)*1.04</f>
+        <f t="shared" ref="S614" si="705">((SUM(C618:F618))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T614">
-        <f t="shared" ref="T614" si="711">((SUM(C620:F620))/4)*1.04</f>
+        <f t="shared" ref="T614" si="706">((SUM(C620:F620))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U614">
-        <f t="shared" ref="U614" si="712">((SUM(C622:F622))/4)*1.04</f>
+        <f t="shared" ref="U614" si="707">((SUM(C622:F622))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V614">
-        <f t="shared" ref="V614" si="713">((SUM(C614:F622))/20)*1.04</f>
+        <f t="shared" ref="V614" si="708">((SUM(C614:F622))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W614">
-        <f t="shared" ref="W614" si="714">(SUM(G614:H622))/10</f>
+        <f t="shared" ref="W614" si="709">(SUM(G614:H622))/10</f>
         <v>19.5</v>
       </c>
       <c r="X614">
-        <f t="shared" ref="X614" si="715">(SUM(I614:I622))/5</f>
+        <f t="shared" ref="X614" si="710">(SUM(I614:I622))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y614">
-        <f t="shared" ref="Y614" si="716">SUM(K614:K622)-Z614</f>
+        <f t="shared" ref="Y614" si="711">SUM(K614:K622)-Z614</f>
         <v>2</v>
       </c>
       <c r="Z614">
-        <f t="shared" ref="Z614" si="717">SUM(L614:L622)</f>
+        <f t="shared" ref="Z614" si="712">SUM(L614:L622)</f>
         <v>9</v>
       </c>
       <c r="AA614" t="s">
@@ -76190,47 +76188,47 @@
         <v>29</v>
       </c>
       <c r="P623">
-        <f t="shared" ref="P623" si="718">M623*10</f>
+        <f t="shared" ref="P623" si="713">M623*10</f>
         <v>50</v>
       </c>
       <c r="Q623">
-        <f t="shared" ref="Q623" si="719">((SUM(C623:F623))/4)*1.04</f>
+        <f t="shared" ref="Q623" si="714">((SUM(C623:F623))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R623">
-        <f t="shared" ref="R623" si="720">((SUM(C625:F625))/4)*1.04</f>
+        <f t="shared" ref="R623" si="715">((SUM(C625:F625))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S623">
-        <f t="shared" ref="S623" si="721">((SUM(C627:F627))/4)*1.04</f>
+        <f t="shared" ref="S623" si="716">((SUM(C627:F627))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T623">
-        <f t="shared" ref="T623" si="722">((SUM(C629:F629))/4)*1.04</f>
+        <f t="shared" ref="T623" si="717">((SUM(C629:F629))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U623">
-        <f t="shared" ref="U623" si="723">((SUM(C631:F631))/4)*1.04</f>
+        <f t="shared" ref="U623" si="718">((SUM(C631:F631))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V623">
-        <f t="shared" ref="V623" si="724">((SUM(C623:F631))/20)*1.04</f>
+        <f t="shared" ref="V623" si="719">((SUM(C623:F631))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W623">
-        <f t="shared" ref="W623" si="725">(SUM(G623:H631))/10</f>
+        <f t="shared" ref="W623" si="720">(SUM(G623:H631))/10</f>
         <v>25.6</v>
       </c>
       <c r="X623">
-        <f t="shared" ref="X623" si="726">(SUM(I623:I631))/5</f>
+        <f t="shared" ref="X623" si="721">(SUM(I623:I631))/5</f>
         <v>1.6</v>
       </c>
       <c r="Y623">
-        <f t="shared" ref="Y623" si="727">SUM(K623:K631)-Z623</f>
+        <f t="shared" ref="Y623" si="722">SUM(K623:K631)-Z623</f>
         <v>12</v>
       </c>
       <c r="Z623">
-        <f t="shared" ref="Z623" si="728">SUM(L623:L631)</f>
+        <f t="shared" ref="Z623" si="723">SUM(L623:L631)</f>
         <v>4</v>
       </c>
       <c r="AA623" t="s">
@@ -76684,47 +76682,47 @@
         <v>29</v>
       </c>
       <c r="P632">
-        <f t="shared" ref="P632" si="729">M632*10</f>
+        <f t="shared" ref="P632" si="724">M632*10</f>
         <v>70</v>
       </c>
       <c r="Q632">
-        <f t="shared" ref="Q632" si="730">((SUM(C632:F632))/4)*1.04</f>
+        <f t="shared" ref="Q632" si="725">((SUM(C632:F632))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R632">
-        <f t="shared" ref="R632" si="731">((SUM(C634:F634))/4)*1.04</f>
+        <f t="shared" ref="R632" si="726">((SUM(C634:F634))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S632">
-        <f t="shared" ref="S632" si="732">((SUM(C636:F636))/4)*1.04</f>
+        <f t="shared" ref="S632" si="727">((SUM(C636:F636))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T632">
-        <f t="shared" ref="T632" si="733">((SUM(C638:F638))/4)*1.04</f>
+        <f t="shared" ref="T632" si="728">((SUM(C638:F638))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U632">
-        <f t="shared" ref="U632" si="734">((SUM(C640:F640))/4)*1.04</f>
+        <f t="shared" ref="U632" si="729">((SUM(C640:F640))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V632">
-        <f t="shared" ref="V632" si="735">((SUM(C632:F640))/20)*1.04</f>
+        <f t="shared" ref="V632" si="730">((SUM(C632:F640))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W632">
-        <f t="shared" ref="W632" si="736">(SUM(G632:H640))/10</f>
+        <f t="shared" ref="W632" si="731">(SUM(G632:H640))/10</f>
         <v>50</v>
       </c>
       <c r="X632">
-        <f t="shared" ref="X632" si="737">(SUM(I632:I640))/5</f>
+        <f t="shared" ref="X632" si="732">(SUM(I632:I640))/5</f>
         <v>1.4</v>
       </c>
       <c r="Y632">
-        <f t="shared" ref="Y632" si="738">SUM(K632:K640)-Z632</f>
+        <f t="shared" ref="Y632" si="733">SUM(K632:K640)-Z632</f>
         <v>-2</v>
       </c>
       <c r="Z632">
-        <f t="shared" ref="Z632" si="739">SUM(L632:L640)</f>
+        <f t="shared" ref="Z632" si="734">SUM(L632:L640)</f>
         <v>6</v>
       </c>
       <c r="AA632" t="s">
@@ -77178,35 +77176,35 @@
         <v>29</v>
       </c>
       <c r="P641">
-        <f t="shared" ref="P641" si="740">M641*10</f>
+        <f t="shared" ref="P641" si="735">M641*10</f>
         <v>40</v>
       </c>
       <c r="Q641">
-        <f t="shared" ref="Q641" si="741">((SUM(C641:F641))/4)*1.04</f>
+        <f t="shared" ref="Q641" si="736">((SUM(C641:F641))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R641">
-        <f t="shared" ref="R641" si="742">((SUM(C643:F643))/4)*1.04</f>
+        <f t="shared" ref="R641" si="737">((SUM(C643:F643))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S641">
-        <f t="shared" ref="S641" si="743">((SUM(C645:F645))/4)*1.04</f>
+        <f t="shared" ref="S641" si="738">((SUM(C645:F645))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T641">
-        <f t="shared" ref="T641" si="744">((SUM(C647:F647))/4)*1.04</f>
+        <f t="shared" ref="T641" si="739">((SUM(C647:F647))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U641">
-        <f t="shared" ref="U641" si="745">((SUM(C649:F649))/4)*1.04</f>
+        <f t="shared" ref="U641" si="740">((SUM(C649:F649))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V641">
-        <f t="shared" ref="V641" si="746">((SUM(C641:F649))/20)*1.04</f>
+        <f t="shared" ref="V641" si="741">((SUM(C641:F649))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W641">
-        <f t="shared" ref="W641" si="747">(SUM(G641:H649))/10</f>
+        <f t="shared" ref="W641" si="742">(SUM(G641:H649))/10</f>
         <v>10.5</v>
       </c>
       <c r="X641">
@@ -77214,11 +77212,11 @@
         <v>1.8</v>
       </c>
       <c r="Y641">
-        <f t="shared" ref="Y641" si="748">SUM(K641:K649)-Z641</f>
+        <f t="shared" ref="Y641" si="743">SUM(K641:K649)-Z641</f>
         <v>6</v>
       </c>
       <c r="Z641">
-        <f t="shared" ref="Z641" si="749">SUM(L641:L649)</f>
+        <f t="shared" ref="Z641" si="744">SUM(L641:L649)</f>
         <v>6</v>
       </c>
       <c r="AA641" t="s">

</xml_diff>

<commit_message>
correct some NAs in original data column for category. Creat R script for species level analysis. Plot height by edge by species for different forests and create loop to run GLM models for all species abundance by edge distances
</commit_message>
<xml_diff>
--- a/raw_data/arabuko_sokoke_11.xlsx
+++ b/raw_data/arabuko_sokoke_11.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesseborden/Dropbox/Research/research_projects/arabuko_sokoke/ASF/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesseborden/Dropbox/SCIENCE/RESEARCH/arabuko_sokoke/ASF/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0E372E-99DE-5C47-A84B-61E0E3D527C1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6E5F79-96AD-FC4A-A979-4C35F2CF897A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="780" windowWidth="27800" windowHeight="16600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="520" windowWidth="27800" windowHeight="16600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Herps" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17471" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17472" uniqueCount="886">
   <si>
     <t>ind_numb</t>
   </si>
@@ -2637,9 +2637,6 @@
     <t>500 = 500m ± 10m</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>MAT_1</t>
   </si>
   <si>
@@ -2674,6 +2671,18 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>hab_type</t>
+  </si>
+  <si>
+    <t>Canopy</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Soil</t>
   </si>
 </sst>
 </file>
@@ -37675,9 +37684,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37760,7 +37769,7 @@
         <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D3" t="s">
         <v>719</v>
@@ -38320,7 +38329,7 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D19" t="s">
         <v>719</v>
@@ -38355,7 +38364,7 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D20" t="s">
         <v>719</v>
@@ -38390,7 +38399,7 @@
         <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>718</v>
       </c>
       <c r="D21" t="s">
         <v>727</v>
@@ -38425,7 +38434,7 @@
         <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>718</v>
       </c>
       <c r="D22" t="s">
         <v>719</v>
@@ -38460,7 +38469,7 @@
         <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>718</v>
       </c>
       <c r="D23" t="s">
         <v>719</v>
@@ -38495,7 +38504,7 @@
         <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D24" t="s">
         <v>719</v>
@@ -38530,7 +38539,7 @@
         <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>718</v>
       </c>
       <c r="D25" t="s">
         <v>719</v>
@@ -38565,7 +38574,7 @@
         <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D26" t="s">
         <v>719</v>
@@ -38600,7 +38609,7 @@
         <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>718</v>
       </c>
       <c r="D27" t="s">
         <v>719</v>
@@ -38670,7 +38679,7 @@
         <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D29" t="s">
         <v>719</v>
@@ -38810,7 +38819,7 @@
         <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D33" t="s">
         <v>719</v>
@@ -39399,7 +39408,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B50" t="s">
         <v>53</v>
@@ -40140,7 +40149,7 @@
         <v>39</v>
       </c>
       <c r="C71" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D71" t="s">
         <v>736</v>
@@ -40175,7 +40184,7 @@
         <v>39</v>
       </c>
       <c r="C72" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D72" t="s">
         <v>736</v>
@@ -40210,7 +40219,7 @@
         <v>39</v>
       </c>
       <c r="C73" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D73" t="s">
         <v>735</v>
@@ -40245,7 +40254,7 @@
         <v>39</v>
       </c>
       <c r="C74" t="s">
-        <v>30</v>
+        <v>718</v>
       </c>
       <c r="D74" t="s">
         <v>736</v>
@@ -40280,7 +40289,7 @@
         <v>39</v>
       </c>
       <c r="C75" t="s">
-        <v>30</v>
+        <v>718</v>
       </c>
       <c r="D75" t="s">
         <v>736</v>
@@ -40315,7 +40324,7 @@
         <v>39</v>
       </c>
       <c r="C76" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D76" t="s">
         <v>735</v>
@@ -40350,7 +40359,7 @@
         <v>39</v>
       </c>
       <c r="C77" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D77" t="s">
         <v>735</v>
@@ -40420,7 +40429,7 @@
         <v>39</v>
       </c>
       <c r="C79" t="s">
-        <v>30</v>
+        <v>718</v>
       </c>
       <c r="D79" t="s">
         <v>736</v>
@@ -40455,7 +40464,7 @@
         <v>39</v>
       </c>
       <c r="C80" t="s">
-        <v>30</v>
+        <v>723</v>
       </c>
       <c r="D80" t="s">
         <v>735</v>
@@ -41392,31 +41401,31 @@
         <v>768</v>
       </c>
       <c r="P1" t="s">
+        <v>873</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>875</v>
+      </c>
+      <c r="R1" t="s">
+        <v>876</v>
+      </c>
+      <c r="S1" t="s">
+        <v>877</v>
+      </c>
+      <c r="T1" t="s">
+        <v>878</v>
+      </c>
+      <c r="U1" t="s">
+        <v>879</v>
+      </c>
+      <c r="V1" t="s">
         <v>874</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>876</v>
-      </c>
-      <c r="R1" t="s">
-        <v>877</v>
-      </c>
-      <c r="S1" t="s">
-        <v>878</v>
-      </c>
-      <c r="T1" t="s">
-        <v>879</v>
-      </c>
-      <c r="U1" t="s">
-        <v>880</v>
-      </c>
-      <c r="V1" t="s">
-        <v>875</v>
       </c>
       <c r="W1" t="s">
         <v>769</v>
       </c>
       <c r="X1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="Y1" t="s">
         <v>770</v>
@@ -62705,7 +62714,7 @@
         <v>30</v>
       </c>
       <c r="M389" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="N389">
         <v>10</v>
@@ -77000,10 +77009,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -77011,7 +77020,7 @@
     <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -77033,13 +77042,16 @@
       <c r="G1" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>883</v>
       </c>
       <c r="C2">
         <v>17</v>
@@ -77057,12 +77069,12 @@
         <v>0.65277777777777779</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>884</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -77080,12 +77092,12 @@
         <v>0.65277777777777779</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>870</v>
+        <v>885</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
@@ -77103,12 +77115,12 @@
         <v>0.65277777777777779</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>883</v>
       </c>
       <c r="C5">
         <v>19</v>
@@ -77126,12 +77138,12 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>884</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -77149,12 +77161,12 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>224</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>883</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -77172,12 +77184,12 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>224</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>884</v>
       </c>
       <c r="C8">
         <v>11</v>
@@ -77195,12 +77207,12 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>185</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>883</v>
       </c>
       <c r="C9">
         <v>18</v>
@@ -77218,12 +77230,12 @@
         <v>0.67361111111111116</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>185</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>884</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -77241,12 +77253,12 @@
         <v>0.67361111111111116</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -77264,12 +77276,12 @@
         <v>0.77083333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>3</v>

</xml_diff>

<commit_message>
more data entry, rerun starting code, and write code for cannonical correspondance analysis (CCA)
</commit_message>
<xml_diff>
--- a/raw_data/arabuko_sokoke_11.xlsx
+++ b/raw_data/arabuko_sokoke_11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesseborden/Dropbox/SCIENCE/RESEARCH/arabuko_sokoke/ASF/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6E5F79-96AD-FC4A-A979-4C35F2CF897A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20EB8E4-D0D8-0640-91E4-C42ED824CCC3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="520" windowWidth="27800" windowHeight="16600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="960" windowWidth="27800" windowHeight="16600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Herps" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17472" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17197" uniqueCount="886">
   <si>
     <t>ind_numb</t>
   </si>
@@ -41340,9 +41340,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AA649"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C200" sqref="C200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A312" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B325" sqref="B325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -52309,17 +52309,17 @@
       <c r="B200" t="s">
         <v>772</v>
       </c>
-      <c r="C200" t="s">
-        <v>30</v>
-      </c>
-      <c r="D200" t="s">
-        <v>30</v>
-      </c>
-      <c r="E200" t="s">
-        <v>30</v>
-      </c>
-      <c r="F200" t="s">
-        <v>30</v>
+      <c r="C200">
+        <v>11</v>
+      </c>
+      <c r="D200">
+        <v>20</v>
+      </c>
+      <c r="E200">
+        <v>21</v>
+      </c>
+      <c r="F200">
+        <v>5</v>
       </c>
       <c r="G200">
         <v>20</v>
@@ -52354,27 +52354,27 @@
       </c>
       <c r="Q200">
         <f t="shared" ref="Q200" si="198">((SUM(C200:F200))/4)*1.04</f>
-        <v>0</v>
+        <v>14.82</v>
       </c>
       <c r="R200">
         <f t="shared" ref="R200" si="199">((SUM(C202:F202))/4)*1.04</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="S200">
         <f t="shared" ref="S200" si="200">((SUM(C204:F204))/4)*1.04</f>
-        <v>0</v>
+        <v>26.78</v>
       </c>
       <c r="T200">
         <f t="shared" ref="T200" si="201">((SUM(C206:F206))/4)*1.04</f>
-        <v>0</v>
+        <v>10.14</v>
       </c>
       <c r="U200">
         <f t="shared" ref="U200" si="202">((SUM(C208:F208))/4)*1.04</f>
-        <v>0</v>
+        <v>20.54</v>
       </c>
       <c r="V200">
         <f t="shared" ref="V200" si="203">((SUM(C200:F208))/20)*1.04</f>
-        <v>0</v>
+        <v>17.055999999999997</v>
       </c>
       <c r="W200">
         <f t="shared" ref="W200" si="204">(SUM(G200:H208))/10</f>
@@ -52453,17 +52453,17 @@
       <c r="B202" t="s">
         <v>775</v>
       </c>
-      <c r="C202" t="s">
-        <v>30</v>
-      </c>
-      <c r="D202" t="s">
-        <v>30</v>
-      </c>
-      <c r="E202" t="s">
-        <v>30</v>
-      </c>
-      <c r="F202" t="s">
-        <v>30</v>
+      <c r="C202">
+        <v>8</v>
+      </c>
+      <c r="D202">
+        <v>26</v>
+      </c>
+      <c r="E202">
+        <v>12</v>
+      </c>
+      <c r="F202">
+        <v>4</v>
       </c>
       <c r="G202">
         <v>35</v>
@@ -52553,17 +52553,17 @@
       <c r="B204" t="s">
         <v>777</v>
       </c>
-      <c r="C204" t="s">
-        <v>30</v>
-      </c>
-      <c r="D204" t="s">
-        <v>30</v>
-      </c>
-      <c r="E204" t="s">
-        <v>30</v>
-      </c>
-      <c r="F204" t="s">
-        <v>30</v>
+      <c r="C204">
+        <v>2</v>
+      </c>
+      <c r="D204">
+        <v>12</v>
+      </c>
+      <c r="E204">
+        <v>44</v>
+      </c>
+      <c r="F204">
+        <v>45</v>
       </c>
       <c r="G204">
         <v>15</v>
@@ -52653,17 +52653,17 @@
       <c r="B206" t="s">
         <v>779</v>
       </c>
-      <c r="C206" t="s">
-        <v>30</v>
-      </c>
-      <c r="D206" t="s">
-        <v>30</v>
-      </c>
-      <c r="E206" t="s">
-        <v>30</v>
-      </c>
-      <c r="F206" t="s">
-        <v>30</v>
+      <c r="C206">
+        <v>4</v>
+      </c>
+      <c r="D206">
+        <v>7</v>
+      </c>
+      <c r="E206">
+        <v>21</v>
+      </c>
+      <c r="F206">
+        <v>7</v>
       </c>
       <c r="G206">
         <v>70</v>
@@ -52753,17 +52753,17 @@
       <c r="B208" t="s">
         <v>781</v>
       </c>
-      <c r="C208" t="s">
-        <v>30</v>
-      </c>
-      <c r="D208" t="s">
-        <v>30</v>
-      </c>
-      <c r="E208" t="s">
-        <v>30</v>
-      </c>
-      <c r="F208" t="s">
-        <v>30</v>
+      <c r="C208">
+        <v>9</v>
+      </c>
+      <c r="D208">
+        <v>26</v>
+      </c>
+      <c r="E208">
+        <v>30</v>
+      </c>
+      <c r="F208">
+        <v>14</v>
       </c>
       <c r="G208">
         <v>5</v>
@@ -52803,17 +52803,17 @@
       <c r="B209" t="s">
         <v>772</v>
       </c>
-      <c r="C209" t="s">
-        <v>30</v>
-      </c>
-      <c r="D209" t="s">
-        <v>30</v>
-      </c>
-      <c r="E209" t="s">
-        <v>30</v>
-      </c>
-      <c r="F209" t="s">
-        <v>30</v>
+      <c r="C209">
+        <v>8</v>
+      </c>
+      <c r="D209">
+        <v>7</v>
+      </c>
+      <c r="E209">
+        <v>8</v>
+      </c>
+      <c r="F209">
+        <v>3</v>
       </c>
       <c r="G209">
         <v>1</v>
@@ -52848,27 +52848,27 @@
       </c>
       <c r="Q209">
         <f t="shared" ref="Q209" si="209">((SUM(C209:F209))/4)*1.04</f>
-        <v>0</v>
+        <v>6.76</v>
       </c>
       <c r="R209">
         <f t="shared" ref="R209" si="210">((SUM(C211:F211))/4)*1.04</f>
-        <v>0</v>
+        <v>8.32</v>
       </c>
       <c r="S209">
         <f t="shared" ref="S209" si="211">((SUM(C213:F213))/4)*1.04</f>
-        <v>0</v>
+        <v>10.4</v>
       </c>
       <c r="T209">
         <f t="shared" ref="T209" si="212">((SUM(C215:F215))/4)*1.04</f>
-        <v>0</v>
+        <v>12.22</v>
       </c>
       <c r="U209">
         <f t="shared" ref="U209" si="213">((SUM(C217:F217))/4)*1.04</f>
-        <v>0</v>
+        <v>8.84</v>
       </c>
       <c r="V209">
         <f t="shared" ref="V209" si="214">((SUM(C209:F217))/20)*1.04</f>
-        <v>0</v>
+        <v>9.3079999999999998</v>
       </c>
       <c r="W209">
         <f t="shared" ref="W209" si="215">(SUM(G209:H217))/10</f>
@@ -52947,17 +52947,17 @@
       <c r="B211" t="s">
         <v>775</v>
       </c>
-      <c r="C211" t="s">
-        <v>30</v>
-      </c>
-      <c r="D211" t="s">
-        <v>30</v>
-      </c>
-      <c r="E211" t="s">
-        <v>30</v>
-      </c>
-      <c r="F211" t="s">
-        <v>30</v>
+      <c r="C211">
+        <v>9</v>
+      </c>
+      <c r="D211">
+        <v>7</v>
+      </c>
+      <c r="E211">
+        <v>10</v>
+      </c>
+      <c r="F211">
+        <v>6</v>
       </c>
       <c r="G211">
         <v>0</v>
@@ -53047,17 +53047,17 @@
       <c r="B213" t="s">
         <v>777</v>
       </c>
-      <c r="C213" t="s">
-        <v>30</v>
-      </c>
-      <c r="D213" t="s">
-        <v>30</v>
-      </c>
-      <c r="E213" t="s">
-        <v>30</v>
-      </c>
-      <c r="F213" t="s">
-        <v>30</v>
+      <c r="C213">
+        <v>6</v>
+      </c>
+      <c r="D213">
+        <v>15</v>
+      </c>
+      <c r="E213">
+        <v>5</v>
+      </c>
+      <c r="F213">
+        <v>14</v>
       </c>
       <c r="G213">
         <v>1</v>
@@ -53147,17 +53147,17 @@
       <c r="B215" t="s">
         <v>779</v>
       </c>
-      <c r="C215" t="s">
-        <v>30</v>
-      </c>
-      <c r="D215" t="s">
-        <v>30</v>
-      </c>
-      <c r="E215" t="s">
-        <v>30</v>
-      </c>
-      <c r="F215" t="s">
-        <v>30</v>
+      <c r="C215">
+        <v>6</v>
+      </c>
+      <c r="D215">
+        <v>20</v>
+      </c>
+      <c r="E215">
+        <v>16</v>
+      </c>
+      <c r="F215">
+        <v>5</v>
       </c>
       <c r="G215">
         <v>0</v>
@@ -53247,17 +53247,17 @@
       <c r="B217" t="s">
         <v>781</v>
       </c>
-      <c r="C217" t="s">
-        <v>30</v>
-      </c>
-      <c r="D217" t="s">
-        <v>30</v>
-      </c>
-      <c r="E217" t="s">
-        <v>30</v>
-      </c>
-      <c r="F217" t="s">
-        <v>30</v>
+      <c r="C217">
+        <v>9</v>
+      </c>
+      <c r="D217">
+        <v>8</v>
+      </c>
+      <c r="E217">
+        <v>8</v>
+      </c>
+      <c r="F217">
+        <v>9</v>
       </c>
       <c r="G217">
         <v>0</v>
@@ -53297,17 +53297,17 @@
       <c r="B218" t="s">
         <v>772</v>
       </c>
-      <c r="C218" t="s">
-        <v>30</v>
-      </c>
-      <c r="D218" t="s">
-        <v>30</v>
-      </c>
-      <c r="E218" t="s">
-        <v>30</v>
-      </c>
-      <c r="F218" t="s">
-        <v>30</v>
+      <c r="C218">
+        <v>9</v>
+      </c>
+      <c r="D218">
+        <v>6</v>
+      </c>
+      <c r="E218">
+        <v>2</v>
+      </c>
+      <c r="F218">
+        <v>4</v>
       </c>
       <c r="G218">
         <v>0</v>
@@ -53342,27 +53342,27 @@
       </c>
       <c r="Q218">
         <f t="shared" ref="Q218" si="220">((SUM(C218:F218))/4)*1.04</f>
-        <v>0</v>
+        <v>5.46</v>
       </c>
       <c r="R218">
         <f t="shared" ref="R218" si="221">((SUM(C220:F220))/4)*1.04</f>
-        <v>0</v>
+        <v>7.28</v>
       </c>
       <c r="S218">
         <f t="shared" ref="S218" si="222">((SUM(C222:F222))/4)*1.04</f>
-        <v>0</v>
+        <v>4.68</v>
       </c>
       <c r="T218">
         <f t="shared" ref="T218" si="223">((SUM(C224:F224))/4)*1.04</f>
-        <v>0</v>
+        <v>6.76</v>
       </c>
       <c r="U218">
         <f t="shared" ref="U218" si="224">((SUM(C226:F226))/4)*1.04</f>
-        <v>0</v>
+        <v>6.24</v>
       </c>
       <c r="V218">
         <f t="shared" ref="V218" si="225">((SUM(C218:F226))/20)*1.04</f>
-        <v>0</v>
+        <v>6.0839999999999996</v>
       </c>
       <c r="W218">
         <f t="shared" ref="W218" si="226">(SUM(G218:H226))/10</f>
@@ -53441,17 +53441,17 @@
       <c r="B220" t="s">
         <v>775</v>
       </c>
-      <c r="C220" t="s">
-        <v>30</v>
-      </c>
-      <c r="D220" t="s">
-        <v>30</v>
-      </c>
-      <c r="E220" t="s">
-        <v>30</v>
-      </c>
-      <c r="F220" t="s">
-        <v>30</v>
+      <c r="C220">
+        <v>12</v>
+      </c>
+      <c r="D220">
+        <v>10</v>
+      </c>
+      <c r="E220">
+        <v>4</v>
+      </c>
+      <c r="F220">
+        <v>2</v>
       </c>
       <c r="G220">
         <v>2</v>
@@ -53541,17 +53541,17 @@
       <c r="B222" t="s">
         <v>777</v>
       </c>
-      <c r="C222" t="s">
-        <v>30</v>
-      </c>
-      <c r="D222" t="s">
-        <v>30</v>
-      </c>
-      <c r="E222" t="s">
-        <v>30</v>
-      </c>
-      <c r="F222" t="s">
-        <v>30</v>
+      <c r="C222">
+        <v>6</v>
+      </c>
+      <c r="D222">
+        <v>4</v>
+      </c>
+      <c r="E222">
+        <v>3</v>
+      </c>
+      <c r="F222">
+        <v>5</v>
       </c>
       <c r="G222">
         <v>0</v>
@@ -53641,17 +53641,17 @@
       <c r="B224" t="s">
         <v>779</v>
       </c>
-      <c r="C224" t="s">
-        <v>30</v>
-      </c>
-      <c r="D224" t="s">
-        <v>30</v>
-      </c>
-      <c r="E224" t="s">
-        <v>30</v>
-      </c>
-      <c r="F224" t="s">
-        <v>30</v>
+      <c r="C224">
+        <v>8</v>
+      </c>
+      <c r="D224">
+        <v>5</v>
+      </c>
+      <c r="E224">
+        <v>10</v>
+      </c>
+      <c r="F224">
+        <v>3</v>
       </c>
       <c r="G224">
         <v>0</v>
@@ -53741,17 +53741,17 @@
       <c r="B226" t="s">
         <v>781</v>
       </c>
-      <c r="C226" t="s">
-        <v>30</v>
-      </c>
-      <c r="D226" t="s">
-        <v>30</v>
-      </c>
-      <c r="E226" t="s">
-        <v>30</v>
-      </c>
-      <c r="F226" t="s">
-        <v>30</v>
+      <c r="C226">
+        <v>5</v>
+      </c>
+      <c r="D226">
+        <v>4</v>
+      </c>
+      <c r="E226">
+        <v>6</v>
+      </c>
+      <c r="F226">
+        <v>9</v>
       </c>
       <c r="G226">
         <v>0</v>
@@ -53791,16 +53791,16 @@
       <c r="B227" t="s">
         <v>772</v>
       </c>
-      <c r="C227" t="s">
-        <v>30</v>
-      </c>
-      <c r="D227" t="s">
-        <v>30</v>
-      </c>
-      <c r="E227" t="s">
-        <v>30</v>
-      </c>
-      <c r="F227" t="s">
+      <c r="C227">
+        <v>6</v>
+      </c>
+      <c r="D227">
+        <v>12</v>
+      </c>
+      <c r="E227">
+        <v>16</v>
+      </c>
+      <c r="F227">
         <v>30</v>
       </c>
       <c r="G227">
@@ -53836,27 +53836,27 @@
       </c>
       <c r="Q227">
         <f t="shared" ref="Q227" si="231">((SUM(C227:F227))/4)*1.04</f>
-        <v>0</v>
+        <v>16.64</v>
       </c>
       <c r="R227">
         <f t="shared" ref="R227" si="232">((SUM(C229:F229))/4)*1.04</f>
-        <v>0</v>
+        <v>9.8800000000000008</v>
       </c>
       <c r="S227">
         <f t="shared" ref="S227" si="233">((SUM(C231:F231))/4)*1.04</f>
-        <v>0</v>
+        <v>10.14</v>
       </c>
       <c r="T227">
         <f t="shared" ref="T227" si="234">((SUM(C233:F233))/4)*1.04</f>
-        <v>0</v>
+        <v>24.18</v>
       </c>
       <c r="U227">
         <f t="shared" ref="U227" si="235">((SUM(C235:F235))/4)*1.04</f>
-        <v>0</v>
+        <v>40.04</v>
       </c>
       <c r="V227">
         <f t="shared" ref="V227" si="236">((SUM(C227:F235))/20)*1.04</f>
-        <v>0</v>
+        <v>20.175999999999998</v>
       </c>
       <c r="W227">
         <f t="shared" ref="W227" si="237">(SUM(G227:H235))/10</f>
@@ -53935,17 +53935,17 @@
       <c r="B229" t="s">
         <v>775</v>
       </c>
-      <c r="C229" t="s">
-        <v>30</v>
-      </c>
-      <c r="D229" t="s">
-        <v>30</v>
-      </c>
-      <c r="E229" t="s">
-        <v>30</v>
-      </c>
-      <c r="F229" t="s">
-        <v>30</v>
+      <c r="C229">
+        <v>6</v>
+      </c>
+      <c r="D229">
+        <v>20</v>
+      </c>
+      <c r="E229">
+        <v>9</v>
+      </c>
+      <c r="F229">
+        <v>3</v>
       </c>
       <c r="G229">
         <v>15</v>
@@ -54035,17 +54035,17 @@
       <c r="B231" t="s">
         <v>777</v>
       </c>
-      <c r="C231" t="s">
-        <v>30</v>
-      </c>
-      <c r="D231" t="s">
-        <v>30</v>
-      </c>
-      <c r="E231" t="s">
-        <v>30</v>
-      </c>
-      <c r="F231" t="s">
-        <v>30</v>
+      <c r="C231">
+        <v>2</v>
+      </c>
+      <c r="D231">
+        <v>10</v>
+      </c>
+      <c r="E231">
+        <v>13</v>
+      </c>
+      <c r="F231">
+        <v>14</v>
       </c>
       <c r="G231">
         <v>20</v>
@@ -54135,17 +54135,17 @@
       <c r="B233" t="s">
         <v>779</v>
       </c>
-      <c r="C233" t="s">
-        <v>30</v>
-      </c>
-      <c r="D233" t="s">
-        <v>30</v>
-      </c>
-      <c r="E233" t="s">
-        <v>30</v>
-      </c>
-      <c r="F233" t="s">
-        <v>30</v>
+      <c r="C233">
+        <v>3</v>
+      </c>
+      <c r="D233">
+        <v>20</v>
+      </c>
+      <c r="E233">
+        <v>48</v>
+      </c>
+      <c r="F233">
+        <v>22</v>
       </c>
       <c r="G233">
         <v>20</v>
@@ -54235,17 +54235,17 @@
       <c r="B235" t="s">
         <v>781</v>
       </c>
-      <c r="C235" t="s">
-        <v>30</v>
-      </c>
-      <c r="D235" t="s">
-        <v>30</v>
-      </c>
-      <c r="E235" t="s">
-        <v>30</v>
-      </c>
-      <c r="F235" t="s">
-        <v>30</v>
+      <c r="C235">
+        <v>4</v>
+      </c>
+      <c r="D235">
+        <v>45</v>
+      </c>
+      <c r="E235">
+        <v>55</v>
+      </c>
+      <c r="F235">
+        <v>50</v>
       </c>
       <c r="G235">
         <v>55</v>
@@ -54285,17 +54285,17 @@
       <c r="B236" t="s">
         <v>772</v>
       </c>
-      <c r="C236" t="s">
-        <v>30</v>
-      </c>
-      <c r="D236" t="s">
-        <v>30</v>
-      </c>
-      <c r="E236" t="s">
-        <v>30</v>
-      </c>
-      <c r="F236" t="s">
-        <v>30</v>
+      <c r="C236">
+        <v>13</v>
+      </c>
+      <c r="D236">
+        <v>23</v>
+      </c>
+      <c r="E236">
+        <v>24</v>
+      </c>
+      <c r="F236">
+        <v>19</v>
       </c>
       <c r="G236">
         <v>15</v>
@@ -54330,27 +54330,27 @@
       </c>
       <c r="Q236">
         <f t="shared" ref="Q236" si="242">((SUM(C236:F236))/4)*1.04</f>
-        <v>0</v>
+        <v>20.54</v>
       </c>
       <c r="R236">
         <f t="shared" ref="R236" si="243">((SUM(C238:F238))/4)*1.04</f>
-        <v>0</v>
+        <v>31.200000000000003</v>
       </c>
       <c r="S236">
         <f t="shared" ref="S236" si="244">((SUM(C240:F240))/4)*1.04</f>
-        <v>0</v>
+        <v>36.4</v>
       </c>
       <c r="T236">
         <f t="shared" ref="T236" si="245">((SUM(C242:F242))/4)*1.04</f>
-        <v>0</v>
+        <v>47.32</v>
       </c>
       <c r="U236">
         <f t="shared" ref="U236" si="246">((SUM(C244:F244))/4)*1.04</f>
-        <v>0</v>
+        <v>43.68</v>
       </c>
       <c r="V236">
         <f t="shared" ref="V236" si="247">((SUM(C236:F244))/20)*1.04</f>
-        <v>0</v>
+        <v>35.828000000000003</v>
       </c>
       <c r="W236">
         <f t="shared" ref="W236" si="248">(SUM(G236:H244))/10</f>
@@ -54429,17 +54429,17 @@
       <c r="B238" t="s">
         <v>775</v>
       </c>
-      <c r="C238" t="s">
-        <v>30</v>
-      </c>
-      <c r="D238" t="s">
-        <v>30</v>
-      </c>
-      <c r="E238" t="s">
-        <v>30</v>
-      </c>
-      <c r="F238" t="s">
-        <v>30</v>
+      <c r="C238">
+        <v>33</v>
+      </c>
+      <c r="D238">
+        <v>24</v>
+      </c>
+      <c r="E238">
+        <v>27</v>
+      </c>
+      <c r="F238">
+        <v>36</v>
       </c>
       <c r="G238">
         <v>75</v>
@@ -54529,17 +54529,17 @@
       <c r="B240" t="s">
         <v>777</v>
       </c>
-      <c r="C240" t="s">
-        <v>30</v>
-      </c>
-      <c r="D240" t="s">
-        <v>30</v>
-      </c>
-      <c r="E240" t="s">
-        <v>30</v>
-      </c>
-      <c r="F240" t="s">
-        <v>30</v>
+      <c r="C240">
+        <v>34</v>
+      </c>
+      <c r="D240">
+        <v>37</v>
+      </c>
+      <c r="E240">
+        <v>58</v>
+      </c>
+      <c r="F240">
+        <v>11</v>
       </c>
       <c r="G240">
         <v>55</v>
@@ -54629,17 +54629,17 @@
       <c r="B242" t="s">
         <v>779</v>
       </c>
-      <c r="C242" t="s">
-        <v>30</v>
-      </c>
-      <c r="D242" t="s">
-        <v>30</v>
-      </c>
-      <c r="E242" t="s">
-        <v>30</v>
-      </c>
-      <c r="F242" t="s">
-        <v>30</v>
+      <c r="C242">
+        <v>21</v>
+      </c>
+      <c r="D242">
+        <v>45</v>
+      </c>
+      <c r="E242">
+        <v>40</v>
+      </c>
+      <c r="F242">
+        <v>76</v>
       </c>
       <c r="G242">
         <v>25</v>
@@ -54729,17 +54729,17 @@
       <c r="B244" t="s">
         <v>781</v>
       </c>
-      <c r="C244" t="s">
-        <v>30</v>
-      </c>
-      <c r="D244" t="s">
-        <v>30</v>
-      </c>
-      <c r="E244" t="s">
-        <v>30</v>
-      </c>
-      <c r="F244" t="s">
-        <v>30</v>
+      <c r="C244">
+        <v>38</v>
+      </c>
+      <c r="D244">
+        <v>37</v>
+      </c>
+      <c r="E244">
+        <v>25</v>
+      </c>
+      <c r="F244">
+        <v>68</v>
       </c>
       <c r="G244">
         <v>80</v>
@@ -54779,17 +54779,17 @@
       <c r="B245" t="s">
         <v>772</v>
       </c>
-      <c r="C245" t="s">
-        <v>30</v>
-      </c>
-      <c r="D245" t="s">
-        <v>30</v>
-      </c>
-      <c r="E245" t="s">
-        <v>30</v>
-      </c>
-      <c r="F245" t="s">
-        <v>30</v>
+      <c r="C245">
+        <v>40</v>
+      </c>
+      <c r="D245">
+        <v>8</v>
+      </c>
+      <c r="E245">
+        <v>10</v>
+      </c>
+      <c r="F245">
+        <v>27</v>
       </c>
       <c r="G245">
         <v>1</v>
@@ -54824,27 +54824,27 @@
       </c>
       <c r="Q245">
         <f t="shared" ref="Q245" si="253">((SUM(C245:F245))/4)*1.04</f>
-        <v>0</v>
+        <v>22.1</v>
       </c>
       <c r="R245">
         <f t="shared" ref="R245" si="254">((SUM(C247:F247))/4)*1.04</f>
-        <v>0</v>
+        <v>18.72</v>
       </c>
       <c r="S245">
         <f t="shared" ref="S245" si="255">((SUM(C249:F249))/4)*1.04</f>
-        <v>0</v>
+        <v>26.52</v>
       </c>
       <c r="T245">
         <f t="shared" ref="T245" si="256">((SUM(C251:F251))/4)*1.04</f>
-        <v>0</v>
+        <v>9.36</v>
       </c>
       <c r="U245">
         <f t="shared" ref="U245" si="257">((SUM(C253:F253))/4)*1.04</f>
-        <v>0</v>
+        <v>27.3</v>
       </c>
       <c r="V245">
         <f t="shared" ref="V245" si="258">((SUM(C245:F253))/20)*1.04</f>
-        <v>0</v>
+        <v>20.8</v>
       </c>
       <c r="W245">
         <f t="shared" ref="W245" si="259">(SUM(G245:H253))/10</f>
@@ -54923,17 +54923,17 @@
       <c r="B247" t="s">
         <v>775</v>
       </c>
-      <c r="C247" t="s">
-        <v>30</v>
-      </c>
-      <c r="D247" t="s">
-        <v>30</v>
-      </c>
-      <c r="E247" t="s">
-        <v>30</v>
-      </c>
-      <c r="F247" t="s">
-        <v>30</v>
+      <c r="C247">
+        <v>15</v>
+      </c>
+      <c r="D247">
+        <v>25</v>
+      </c>
+      <c r="E247">
+        <v>15</v>
+      </c>
+      <c r="F247">
+        <v>17</v>
       </c>
       <c r="G247">
         <v>10</v>
@@ -55023,16 +55023,16 @@
       <c r="B249" t="s">
         <v>777</v>
       </c>
-      <c r="C249" t="s">
-        <v>30</v>
-      </c>
-      <c r="D249" t="s">
-        <v>30</v>
-      </c>
-      <c r="E249" t="s">
-        <v>30</v>
-      </c>
-      <c r="F249" t="s">
+      <c r="C249">
+        <v>31</v>
+      </c>
+      <c r="D249">
+        <v>8</v>
+      </c>
+      <c r="E249">
+        <v>33</v>
+      </c>
+      <c r="F249">
         <v>30</v>
       </c>
       <c r="G249">
@@ -55123,17 +55123,17 @@
       <c r="B251" t="s">
         <v>779</v>
       </c>
-      <c r="C251" t="s">
-        <v>30</v>
-      </c>
-      <c r="D251" t="s">
-        <v>30</v>
-      </c>
-      <c r="E251" t="s">
-        <v>30</v>
-      </c>
-      <c r="F251" t="s">
-        <v>30</v>
+      <c r="C251">
+        <v>17</v>
+      </c>
+      <c r="D251">
+        <v>3</v>
+      </c>
+      <c r="E251">
+        <v>12</v>
+      </c>
+      <c r="F251">
+        <v>4</v>
       </c>
       <c r="G251">
         <v>0</v>
@@ -55223,17 +55223,17 @@
       <c r="B253" t="s">
         <v>781</v>
       </c>
-      <c r="C253" t="s">
-        <v>30</v>
-      </c>
-      <c r="D253" t="s">
-        <v>30</v>
-      </c>
-      <c r="E253" t="s">
-        <v>30</v>
-      </c>
-      <c r="F253" t="s">
-        <v>30</v>
+      <c r="C253">
+        <v>20</v>
+      </c>
+      <c r="D253">
+        <v>37</v>
+      </c>
+      <c r="E253">
+        <v>30</v>
+      </c>
+      <c r="F253">
+        <v>18</v>
       </c>
       <c r="G253">
         <v>3</v>
@@ -55273,17 +55273,17 @@
       <c r="B254" t="s">
         <v>772</v>
       </c>
-      <c r="C254" t="s">
-        <v>30</v>
-      </c>
-      <c r="D254" t="s">
-        <v>30</v>
-      </c>
-      <c r="E254" t="s">
-        <v>30</v>
-      </c>
-      <c r="F254" t="s">
-        <v>30</v>
+      <c r="C254">
+        <v>24</v>
+      </c>
+      <c r="D254">
+        <v>15</v>
+      </c>
+      <c r="E254">
+        <v>15</v>
+      </c>
+      <c r="F254">
+        <v>10</v>
       </c>
       <c r="G254">
         <v>0</v>
@@ -55318,42 +55318,41 @@
       </c>
       <c r="Q254">
         <f t="shared" ref="Q254" si="264">((SUM(C254:F254))/4)*1.04</f>
-        <v>0</v>
+        <v>16.64</v>
       </c>
       <c r="R254">
         <f t="shared" ref="R254" si="265">((SUM(C256:F256))/4)*1.04</f>
-        <v>0</v>
+        <v>34.840000000000003</v>
       </c>
       <c r="S254">
         <f t="shared" ref="S254" si="266">((SUM(C258:F258))/4)*1.04</f>
-        <v>0</v>
+        <v>24.96</v>
       </c>
       <c r="T254">
         <f t="shared" ref="T254" si="267">((SUM(C260:F260))/4)*1.04</f>
-        <v>0</v>
-      </c>
-      <c r="U254">
-        <f t="shared" ref="U254" si="268">((SUM(C262:F262))/4)*1.04</f>
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="U254" t="s">
+        <v>30</v>
       </c>
       <c r="V254">
-        <f t="shared" ref="V254" si="269">((SUM(C254:F262))/20)*1.04</f>
-        <v>0</v>
+        <f>((SUM(C254:F262))/16)*1.04</f>
+        <v>22.36</v>
       </c>
       <c r="W254">
-        <f t="shared" ref="W254" si="270">(SUM(G254:H262))/10</f>
+        <f t="shared" ref="W254" si="268">(SUM(G254:H262))/10</f>
         <v>15.6</v>
       </c>
       <c r="X254">
-        <f t="shared" ref="X254" si="271">(SUM(I254:I262))/5</f>
+        <f t="shared" ref="X254" si="269">(SUM(I254:I262))/5</f>
         <v>2</v>
       </c>
       <c r="Y254">
-        <f t="shared" ref="Y254" si="272">SUM(K254:K262)-Z254</f>
+        <f t="shared" ref="Y254" si="270">SUM(K254:K262)-Z254</f>
         <v>58</v>
       </c>
       <c r="Z254">
-        <f t="shared" ref="Z254" si="273">SUM(L254:L262)</f>
+        <f t="shared" ref="Z254" si="271">SUM(L254:L262)</f>
         <v>12</v>
       </c>
       <c r="AA254" t="s">
@@ -55417,17 +55416,17 @@
       <c r="B256" t="s">
         <v>775</v>
       </c>
-      <c r="C256" t="s">
-        <v>30</v>
-      </c>
-      <c r="D256" t="s">
-        <v>30</v>
-      </c>
-      <c r="E256" t="s">
-        <v>30</v>
-      </c>
-      <c r="F256" t="s">
-        <v>30</v>
+      <c r="C256">
+        <v>20</v>
+      </c>
+      <c r="D256">
+        <v>5</v>
+      </c>
+      <c r="E256">
+        <v>64</v>
+      </c>
+      <c r="F256">
+        <v>45</v>
       </c>
       <c r="G256">
         <v>15</v>
@@ -55517,16 +55516,16 @@
       <c r="B258" t="s">
         <v>777</v>
       </c>
-      <c r="C258" t="s">
-        <v>30</v>
-      </c>
-      <c r="D258" t="s">
-        <v>30</v>
-      </c>
-      <c r="E258" t="s">
-        <v>30</v>
-      </c>
-      <c r="F258" t="s">
+      <c r="C258">
+        <v>24</v>
+      </c>
+      <c r="D258">
+        <v>12</v>
+      </c>
+      <c r="E258">
+        <v>30</v>
+      </c>
+      <c r="F258">
         <v>30</v>
       </c>
       <c r="G258">
@@ -55617,17 +55616,17 @@
       <c r="B260" t="s">
         <v>779</v>
       </c>
-      <c r="C260" t="s">
-        <v>30</v>
-      </c>
-      <c r="D260" t="s">
-        <v>30</v>
-      </c>
-      <c r="E260" t="s">
-        <v>30</v>
-      </c>
-      <c r="F260" t="s">
-        <v>30</v>
+      <c r="C260">
+        <v>7</v>
+      </c>
+      <c r="D260">
+        <v>11</v>
+      </c>
+      <c r="E260">
+        <v>15</v>
+      </c>
+      <c r="F260">
+        <v>17</v>
       </c>
       <c r="G260">
         <v>0</v>
@@ -55767,17 +55766,17 @@
       <c r="B263" t="s">
         <v>772</v>
       </c>
-      <c r="C263" t="s">
-        <v>30</v>
-      </c>
-      <c r="D263" t="s">
-        <v>30</v>
-      </c>
-      <c r="E263" t="s">
-        <v>30</v>
-      </c>
-      <c r="F263" t="s">
-        <v>30</v>
+      <c r="C263">
+        <v>3</v>
+      </c>
+      <c r="D263">
+        <v>11</v>
+      </c>
+      <c r="E263">
+        <v>15</v>
+      </c>
+      <c r="F263">
+        <v>4</v>
       </c>
       <c r="G263">
         <v>5</v>
@@ -55807,47 +55806,47 @@
         <v>240</v>
       </c>
       <c r="P263">
-        <f t="shared" ref="P263" si="274">M263*10</f>
+        <f t="shared" ref="P263" si="272">M263*10</f>
         <v>60</v>
       </c>
       <c r="Q263">
-        <f t="shared" ref="Q263" si="275">((SUM(C263:F263))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="Q263" si="273">((SUM(C263:F263))/4)*1.04</f>
+        <v>8.58</v>
       </c>
       <c r="R263">
-        <f t="shared" ref="R263" si="276">((SUM(C265:F265))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="R263" si="274">((SUM(C265:F265))/4)*1.04</f>
+        <v>25.48</v>
       </c>
       <c r="S263">
-        <f t="shared" ref="S263" si="277">((SUM(C267:F267))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="S263" si="275">((SUM(C267:F267))/4)*1.04</f>
+        <v>7.0200000000000005</v>
       </c>
       <c r="T263">
-        <f t="shared" ref="T263" si="278">((SUM(C269:F269))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="T263" si="276">((SUM(C269:F269))/4)*1.04</f>
+        <v>28.6</v>
       </c>
       <c r="U263">
-        <f t="shared" ref="U263" si="279">((SUM(C271:F271))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="U263" si="277">((SUM(C271:F271))/4)*1.04</f>
+        <v>27.82</v>
       </c>
       <c r="V263">
-        <f t="shared" ref="V263" si="280">((SUM(C263:F271))/20)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="V263" si="278">((SUM(C263:F271))/20)*1.04</f>
+        <v>19.5</v>
       </c>
       <c r="W263">
-        <f t="shared" ref="W263" si="281">(SUM(G263:H271))/10</f>
+        <f t="shared" ref="W263" si="279">(SUM(G263:H271))/10</f>
         <v>4.5</v>
       </c>
       <c r="X263">
-        <f t="shared" ref="X263" si="282">(SUM(I263:I271))/5</f>
+        <f t="shared" ref="X263" si="280">(SUM(I263:I271))/5</f>
         <v>4</v>
       </c>
       <c r="Y263">
-        <f t="shared" ref="Y263" si="283">SUM(K263:K271)-Z263</f>
+        <f t="shared" ref="Y263" si="281">SUM(K263:K271)-Z263</f>
         <v>16</v>
       </c>
       <c r="Z263">
-        <f t="shared" ref="Z263" si="284">SUM(L263:L271)</f>
+        <f t="shared" ref="Z263" si="282">SUM(L263:L271)</f>
         <v>3</v>
       </c>
       <c r="AA263" t="s">
@@ -55911,17 +55910,17 @@
       <c r="B265" t="s">
         <v>775</v>
       </c>
-      <c r="C265" t="s">
-        <v>30</v>
-      </c>
-      <c r="D265" t="s">
-        <v>30</v>
-      </c>
-      <c r="E265" t="s">
-        <v>30</v>
-      </c>
-      <c r="F265" t="s">
-        <v>30</v>
+      <c r="C265">
+        <v>21</v>
+      </c>
+      <c r="D265">
+        <v>12</v>
+      </c>
+      <c r="E265">
+        <v>15</v>
+      </c>
+      <c r="F265">
+        <v>50</v>
       </c>
       <c r="G265">
         <v>5</v>
@@ -56011,17 +56010,17 @@
       <c r="B267" t="s">
         <v>777</v>
       </c>
-      <c r="C267" t="s">
-        <v>30</v>
-      </c>
-      <c r="D267" t="s">
-        <v>30</v>
-      </c>
-      <c r="E267" t="s">
-        <v>30</v>
-      </c>
-      <c r="F267" t="s">
-        <v>30</v>
+      <c r="C267">
+        <v>9</v>
+      </c>
+      <c r="D267">
+        <v>8</v>
+      </c>
+      <c r="E267">
+        <v>4</v>
+      </c>
+      <c r="F267">
+        <v>6</v>
       </c>
       <c r="G267">
         <v>0</v>
@@ -56111,17 +56110,17 @@
       <c r="B269" t="s">
         <v>779</v>
       </c>
-      <c r="C269" t="s">
-        <v>30</v>
-      </c>
-      <c r="D269" t="s">
-        <v>30</v>
-      </c>
-      <c r="E269" t="s">
-        <v>30</v>
-      </c>
-      <c r="F269" t="s">
-        <v>30</v>
+      <c r="C269">
+        <v>35</v>
+      </c>
+      <c r="D269">
+        <v>37</v>
+      </c>
+      <c r="E269">
+        <v>11</v>
+      </c>
+      <c r="F269">
+        <v>27</v>
       </c>
       <c r="G269">
         <v>0</v>
@@ -56211,17 +56210,17 @@
       <c r="B271" t="s">
         <v>781</v>
       </c>
-      <c r="C271" t="s">
-        <v>30</v>
-      </c>
-      <c r="D271" t="s">
-        <v>30</v>
-      </c>
-      <c r="E271" t="s">
-        <v>30</v>
-      </c>
-      <c r="F271" t="s">
-        <v>30</v>
+      <c r="C271">
+        <v>35</v>
+      </c>
+      <c r="D271">
+        <v>40</v>
+      </c>
+      <c r="E271">
+        <v>14</v>
+      </c>
+      <c r="F271">
+        <v>18</v>
       </c>
       <c r="G271">
         <v>10</v>
@@ -56261,17 +56260,17 @@
       <c r="B272" t="s">
         <v>772</v>
       </c>
-      <c r="C272" t="s">
-        <v>30</v>
-      </c>
-      <c r="D272" t="s">
-        <v>30</v>
-      </c>
-      <c r="E272" t="s">
-        <v>30</v>
-      </c>
-      <c r="F272" t="s">
-        <v>30</v>
+      <c r="C272">
+        <v>21</v>
+      </c>
+      <c r="D272">
+        <v>15</v>
+      </c>
+      <c r="E272">
+        <v>19</v>
+      </c>
+      <c r="F272">
+        <v>11</v>
       </c>
       <c r="G272">
         <v>30</v>
@@ -56301,47 +56300,47 @@
         <v>240</v>
       </c>
       <c r="P272">
-        <f t="shared" ref="P272" si="285">M272*10</f>
+        <f t="shared" ref="P272" si="283">M272*10</f>
         <v>30</v>
       </c>
       <c r="Q272">
-        <f t="shared" ref="Q272" si="286">((SUM(C272:F272))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="Q272" si="284">((SUM(C272:F272))/4)*1.04</f>
+        <v>17.16</v>
       </c>
       <c r="R272">
-        <f t="shared" ref="R272" si="287">((SUM(C274:F274))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="R272" si="285">((SUM(C274:F274))/4)*1.04</f>
+        <v>13</v>
       </c>
       <c r="S272">
-        <f t="shared" ref="S272" si="288">((SUM(C276:F276))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="S272" si="286">((SUM(C276:F276))/4)*1.04</f>
+        <v>16.64</v>
       </c>
       <c r="T272">
-        <f t="shared" ref="T272" si="289">((SUM(C278:F278))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="T272" si="287">((SUM(C278:F278))/4)*1.04</f>
+        <v>7.28</v>
       </c>
       <c r="U272">
-        <f t="shared" ref="U272" si="290">((SUM(C280:F280))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="U272" si="288">((SUM(C280:F280))/4)*1.04</f>
+        <v>12.22</v>
       </c>
       <c r="V272">
-        <f t="shared" ref="V272" si="291">((SUM(C272:F280))/20)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="V272" si="289">((SUM(C272:F280))/20)*1.04</f>
+        <v>13.26</v>
       </c>
       <c r="W272">
-        <f t="shared" ref="W272" si="292">(SUM(G272:H280))/10</f>
+        <f t="shared" ref="W272" si="290">(SUM(G272:H280))/10</f>
         <v>6</v>
       </c>
       <c r="X272">
-        <f t="shared" ref="X272" si="293">(SUM(I272:I280))/5</f>
+        <f t="shared" ref="X272" si="291">(SUM(I272:I280))/5</f>
         <v>2.6</v>
       </c>
       <c r="Y272">
-        <f t="shared" ref="Y272" si="294">SUM(K272:K280)-Z272</f>
+        <f t="shared" ref="Y272" si="292">SUM(K272:K280)-Z272</f>
         <v>12</v>
       </c>
       <c r="Z272">
-        <f t="shared" ref="Z272" si="295">SUM(L272:L280)</f>
+        <f t="shared" ref="Z272" si="293">SUM(L272:L280)</f>
         <v>3</v>
       </c>
       <c r="AA272" t="s">
@@ -56405,17 +56404,17 @@
       <c r="B274" t="s">
         <v>775</v>
       </c>
-      <c r="C274" t="s">
-        <v>30</v>
-      </c>
-      <c r="D274" t="s">
-        <v>30</v>
-      </c>
-      <c r="E274" t="s">
-        <v>30</v>
-      </c>
-      <c r="F274" t="s">
-        <v>30</v>
+      <c r="C274">
+        <v>17</v>
+      </c>
+      <c r="D274">
+        <v>11</v>
+      </c>
+      <c r="E274">
+        <v>13</v>
+      </c>
+      <c r="F274">
+        <v>9</v>
       </c>
       <c r="G274">
         <v>0</v>
@@ -56505,17 +56504,17 @@
       <c r="B276" t="s">
         <v>777</v>
       </c>
-      <c r="C276" t="s">
-        <v>30</v>
-      </c>
-      <c r="D276" t="s">
-        <v>30</v>
-      </c>
-      <c r="E276" t="s">
-        <v>30</v>
-      </c>
-      <c r="F276" t="s">
-        <v>30</v>
+      <c r="C276">
+        <v>7</v>
+      </c>
+      <c r="D276">
+        <v>11</v>
+      </c>
+      <c r="E276">
+        <v>22</v>
+      </c>
+      <c r="F276">
+        <v>24</v>
       </c>
       <c r="G276">
         <v>0</v>
@@ -56605,17 +56604,17 @@
       <c r="B278" t="s">
         <v>779</v>
       </c>
-      <c r="C278" t="s">
-        <v>30</v>
-      </c>
-      <c r="D278" t="s">
-        <v>30</v>
-      </c>
-      <c r="E278" t="s">
-        <v>30</v>
-      </c>
-      <c r="F278" t="s">
-        <v>30</v>
+      <c r="C278">
+        <v>8</v>
+      </c>
+      <c r="D278">
+        <v>6</v>
+      </c>
+      <c r="E278">
+        <v>5</v>
+      </c>
+      <c r="F278">
+        <v>9</v>
       </c>
       <c r="G278">
         <v>0</v>
@@ -56705,17 +56704,17 @@
       <c r="B280" t="s">
         <v>781</v>
       </c>
-      <c r="C280" t="s">
-        <v>30</v>
-      </c>
-      <c r="D280" t="s">
-        <v>30</v>
-      </c>
-      <c r="E280" t="s">
-        <v>30</v>
-      </c>
-      <c r="F280" t="s">
-        <v>30</v>
+      <c r="C280">
+        <v>3</v>
+      </c>
+      <c r="D280">
+        <v>13</v>
+      </c>
+      <c r="E280">
+        <v>15</v>
+      </c>
+      <c r="F280">
+        <v>16</v>
       </c>
       <c r="G280">
         <v>10</v>
@@ -56755,17 +56754,17 @@
       <c r="B281" t="s">
         <v>772</v>
       </c>
-      <c r="C281" t="s">
-        <v>30</v>
-      </c>
-      <c r="D281" t="s">
-        <v>30</v>
-      </c>
-      <c r="E281" t="s">
-        <v>30</v>
-      </c>
-      <c r="F281" t="s">
-        <v>30</v>
+      <c r="C281">
+        <v>17</v>
+      </c>
+      <c r="D281">
+        <v>17</v>
+      </c>
+      <c r="E281">
+        <v>14</v>
+      </c>
+      <c r="F281">
+        <v>11</v>
       </c>
       <c r="G281">
         <v>40</v>
@@ -56795,47 +56794,47 @@
         <v>240</v>
       </c>
       <c r="P281">
-        <f t="shared" ref="P281" si="296">M281*10</f>
+        <f t="shared" ref="P281" si="294">M281*10</f>
         <v>50</v>
       </c>
       <c r="Q281">
-        <f t="shared" ref="Q281" si="297">((SUM(C281:F281))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="Q281" si="295">((SUM(C281:F281))/4)*1.04</f>
+        <v>15.34</v>
       </c>
       <c r="R281">
-        <f t="shared" ref="R281" si="298">((SUM(C283:F283))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="R281" si="296">((SUM(C283:F283))/4)*1.04</f>
+        <v>24.96</v>
       </c>
       <c r="S281">
-        <f t="shared" ref="S281" si="299">((SUM(C285:F285))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="S281" si="297">((SUM(C285:F285))/4)*1.04</f>
+        <v>21.060000000000002</v>
       </c>
       <c r="T281">
-        <f t="shared" ref="T281" si="300">((SUM(C287:F287))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="T281" si="298">((SUM(C287:F287))/4)*1.04</f>
+        <v>19.5</v>
       </c>
       <c r="U281">
-        <f t="shared" ref="U281" si="301">((SUM(C289:F289))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="U281" si="299">((SUM(C289:F289))/4)*1.04</f>
+        <v>17.16</v>
       </c>
       <c r="V281">
-        <f t="shared" ref="V281" si="302">((SUM(C281:F289))/20)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="V281" si="300">((SUM(C281:F289))/20)*1.04</f>
+        <v>19.604000000000003</v>
       </c>
       <c r="W281">
-        <f t="shared" ref="W281" si="303">(SUM(G281:H289))/10</f>
+        <f t="shared" ref="W281" si="301">(SUM(G281:H289))/10</f>
         <v>21</v>
       </c>
       <c r="X281">
-        <f t="shared" ref="X281" si="304">(SUM(I281:I289))/5</f>
+        <f t="shared" ref="X281" si="302">(SUM(I281:I289))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y281">
-        <f t="shared" ref="Y281" si="305">SUM(K281:K289)-Z281</f>
+        <f t="shared" ref="Y281" si="303">SUM(K281:K289)-Z281</f>
         <v>11</v>
       </c>
       <c r="Z281">
-        <f t="shared" ref="Z281" si="306">SUM(L281:L289)</f>
+        <f t="shared" ref="Z281" si="304">SUM(L281:L289)</f>
         <v>4</v>
       </c>
       <c r="AA281" t="s">
@@ -56899,17 +56898,17 @@
       <c r="B283" t="s">
         <v>775</v>
       </c>
-      <c r="C283" t="s">
-        <v>30</v>
-      </c>
-      <c r="D283" t="s">
-        <v>30</v>
-      </c>
-      <c r="E283" t="s">
-        <v>30</v>
-      </c>
-      <c r="F283" t="s">
-        <v>30</v>
+      <c r="C283">
+        <v>28</v>
+      </c>
+      <c r="D283">
+        <v>32</v>
+      </c>
+      <c r="E283">
+        <v>13</v>
+      </c>
+      <c r="F283">
+        <v>23</v>
       </c>
       <c r="G283">
         <v>20</v>
@@ -56999,17 +56998,17 @@
       <c r="B285" t="s">
         <v>777</v>
       </c>
-      <c r="C285" t="s">
-        <v>30</v>
-      </c>
-      <c r="D285" t="s">
-        <v>30</v>
-      </c>
-      <c r="E285" t="s">
-        <v>30</v>
-      </c>
-      <c r="F285" t="s">
-        <v>30</v>
+      <c r="C285">
+        <v>9</v>
+      </c>
+      <c r="D285">
+        <v>28</v>
+      </c>
+      <c r="E285">
+        <v>27</v>
+      </c>
+      <c r="F285">
+        <v>17</v>
       </c>
       <c r="G285">
         <v>50</v>
@@ -57099,17 +57098,17 @@
       <c r="B287" t="s">
         <v>779</v>
       </c>
-      <c r="C287" t="s">
-        <v>30</v>
-      </c>
-      <c r="D287" t="s">
-        <v>30</v>
-      </c>
-      <c r="E287" t="s">
-        <v>30</v>
-      </c>
-      <c r="F287" t="s">
-        <v>30</v>
+      <c r="C287">
+        <v>17</v>
+      </c>
+      <c r="D287">
+        <v>20</v>
+      </c>
+      <c r="E287">
+        <v>20</v>
+      </c>
+      <c r="F287">
+        <v>18</v>
       </c>
       <c r="G287">
         <v>5</v>
@@ -57199,17 +57198,17 @@
       <c r="B289" t="s">
         <v>781</v>
       </c>
-      <c r="C289" t="s">
-        <v>30</v>
-      </c>
-      <c r="D289" t="s">
-        <v>30</v>
-      </c>
-      <c r="E289" t="s">
-        <v>30</v>
-      </c>
-      <c r="F289" t="s">
-        <v>30</v>
+      <c r="C289">
+        <v>15</v>
+      </c>
+      <c r="D289">
+        <v>17</v>
+      </c>
+      <c r="E289">
+        <v>20</v>
+      </c>
+      <c r="F289">
+        <v>14</v>
       </c>
       <c r="G289">
         <v>20</v>
@@ -57249,17 +57248,17 @@
       <c r="B290" t="s">
         <v>772</v>
       </c>
-      <c r="C290" t="s">
-        <v>30</v>
-      </c>
-      <c r="D290" t="s">
-        <v>30</v>
-      </c>
-      <c r="E290" t="s">
-        <v>30</v>
-      </c>
-      <c r="F290" t="s">
-        <v>30</v>
+      <c r="C290">
+        <v>28</v>
+      </c>
+      <c r="D290">
+        <v>27</v>
+      </c>
+      <c r="E290">
+        <v>5</v>
+      </c>
+      <c r="F290">
+        <v>4</v>
       </c>
       <c r="G290">
         <v>1</v>
@@ -57289,47 +57288,47 @@
         <v>43</v>
       </c>
       <c r="P290">
-        <f t="shared" ref="P290" si="307">M290*10</f>
+        <f t="shared" ref="P290" si="305">M290*10</f>
         <v>90</v>
       </c>
       <c r="Q290">
-        <f t="shared" ref="Q290" si="308">((SUM(C290:F290))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="Q290" si="306">((SUM(C290:F290))/4)*1.04</f>
+        <v>16.64</v>
       </c>
       <c r="R290">
-        <f t="shared" ref="R290" si="309">((SUM(C292:F292))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="R290" si="307">((SUM(C292:F292))/4)*1.04</f>
+        <v>15.08</v>
       </c>
       <c r="S290">
-        <f t="shared" ref="S290" si="310">((SUM(C294:F294))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="S290" si="308">((SUM(C294:F294))/4)*1.04</f>
+        <v>15.860000000000001</v>
       </c>
       <c r="T290">
-        <f t="shared" ref="T290" si="311">((SUM(C296:F296))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="T290" si="309">((SUM(C296:F296))/4)*1.04</f>
+        <v>14.3</v>
       </c>
       <c r="U290">
-        <f t="shared" ref="U290" si="312">((SUM(C298:F298))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="U290" si="310">((SUM(C298:F298))/4)*1.04</f>
+        <v>13.26</v>
       </c>
       <c r="V290">
-        <f t="shared" ref="V290" si="313">((SUM(C290:F298))/20)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="V290" si="311">((SUM(C290:F298))/20)*1.04</f>
+        <v>15.028</v>
       </c>
       <c r="W290">
-        <f t="shared" ref="W290" si="314">(SUM(G290:H298))/10</f>
+        <f t="shared" ref="W290" si="312">(SUM(G290:H298))/10</f>
         <v>3.2</v>
       </c>
       <c r="X290">
-        <f t="shared" ref="X290" si="315">(SUM(I290:I298))/5</f>
+        <f t="shared" ref="X290" si="313">(SUM(I290:I298))/5</f>
         <v>2.6</v>
       </c>
       <c r="Y290">
-        <f t="shared" ref="Y290" si="316">SUM(K290:K298)-Z290</f>
+        <f t="shared" ref="Y290" si="314">SUM(K290:K298)-Z290</f>
         <v>65</v>
       </c>
       <c r="Z290">
-        <f t="shared" ref="Z290" si="317">SUM(L290:L298)</f>
+        <f t="shared" ref="Z290" si="315">SUM(L290:L298)</f>
         <v>2</v>
       </c>
       <c r="AA290" t="s">
@@ -57393,17 +57392,17 @@
       <c r="B292" t="s">
         <v>775</v>
       </c>
-      <c r="C292" t="s">
-        <v>30</v>
-      </c>
-      <c r="D292" t="s">
-        <v>30</v>
-      </c>
-      <c r="E292" t="s">
-        <v>30</v>
-      </c>
-      <c r="F292" t="s">
-        <v>30</v>
+      <c r="C292">
+        <v>9</v>
+      </c>
+      <c r="D292">
+        <v>17</v>
+      </c>
+      <c r="E292">
+        <v>18</v>
+      </c>
+      <c r="F292">
+        <v>14</v>
       </c>
       <c r="G292">
         <v>0</v>
@@ -57493,17 +57492,17 @@
       <c r="B294" t="s">
         <v>777</v>
       </c>
-      <c r="C294" t="s">
-        <v>30</v>
-      </c>
-      <c r="D294" t="s">
-        <v>30</v>
-      </c>
-      <c r="E294" t="s">
-        <v>30</v>
-      </c>
-      <c r="F294" t="s">
-        <v>30</v>
+      <c r="C294">
+        <v>29</v>
+      </c>
+      <c r="D294">
+        <v>12</v>
+      </c>
+      <c r="E294">
+        <v>15</v>
+      </c>
+      <c r="F294">
+        <v>5</v>
       </c>
       <c r="G294">
         <v>2</v>
@@ -57593,17 +57592,17 @@
       <c r="B296" t="s">
         <v>779</v>
       </c>
-      <c r="C296" t="s">
-        <v>30</v>
-      </c>
-      <c r="D296" t="s">
-        <v>30</v>
-      </c>
-      <c r="E296" t="s">
-        <v>30</v>
-      </c>
-      <c r="F296" t="s">
-        <v>30</v>
+      <c r="C296">
+        <v>11</v>
+      </c>
+      <c r="D296">
+        <v>22</v>
+      </c>
+      <c r="E296">
+        <v>3</v>
+      </c>
+      <c r="F296">
+        <v>19</v>
       </c>
       <c r="G296">
         <v>4</v>
@@ -57693,17 +57692,17 @@
       <c r="B298" t="s">
         <v>781</v>
       </c>
-      <c r="C298" t="s">
-        <v>30</v>
-      </c>
-      <c r="D298" t="s">
-        <v>30</v>
-      </c>
-      <c r="E298" t="s">
-        <v>30</v>
-      </c>
-      <c r="F298" t="s">
-        <v>30</v>
+      <c r="C298">
+        <v>17</v>
+      </c>
+      <c r="D298">
+        <v>10</v>
+      </c>
+      <c r="E298">
+        <v>10</v>
+      </c>
+      <c r="F298">
+        <v>14</v>
       </c>
       <c r="G298">
         <v>10</v>
@@ -57743,17 +57742,17 @@
       <c r="B299" t="s">
         <v>772</v>
       </c>
-      <c r="C299" t="s">
-        <v>30</v>
-      </c>
-      <c r="D299" t="s">
-        <v>30</v>
-      </c>
-      <c r="E299" t="s">
-        <v>30</v>
-      </c>
-      <c r="F299" t="s">
-        <v>30</v>
+      <c r="C299">
+        <v>5</v>
+      </c>
+      <c r="D299">
+        <v>12</v>
+      </c>
+      <c r="E299">
+        <v>17</v>
+      </c>
+      <c r="F299">
+        <v>15</v>
       </c>
       <c r="G299">
         <v>0</v>
@@ -57783,47 +57782,47 @@
         <v>29</v>
       </c>
       <c r="P299">
-        <f t="shared" ref="P299" si="318">M299*10</f>
+        <f t="shared" ref="P299" si="316">M299*10</f>
         <v>90</v>
       </c>
       <c r="Q299">
-        <f t="shared" ref="Q299" si="319">((SUM(C299:F299))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="Q299" si="317">((SUM(C299:F299))/4)*1.04</f>
+        <v>12.74</v>
       </c>
       <c r="R299">
-        <f t="shared" ref="R299" si="320">((SUM(C301:F301))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="R299" si="318">((SUM(C301:F301))/4)*1.04</f>
+        <v>15.600000000000001</v>
       </c>
       <c r="S299">
-        <f t="shared" ref="S299" si="321">((SUM(C303:F303))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="S299" si="319">((SUM(C303:F303))/4)*1.04</f>
+        <v>5.98</v>
       </c>
       <c r="T299">
-        <f t="shared" ref="T299" si="322">((SUM(C305:F305))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="T299" si="320">((SUM(C305:F305))/4)*1.04</f>
+        <v>11.440000000000001</v>
       </c>
       <c r="U299">
-        <f t="shared" ref="U299" si="323">((SUM(C307:F307))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="U299" si="321">((SUM(C307:F307))/4)*1.04</f>
+        <v>8.58</v>
       </c>
       <c r="V299">
-        <f t="shared" ref="V299" si="324">((SUM(C299:F307))/20)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="V299" si="322">((SUM(C299:F307))/20)*1.04</f>
+        <v>10.868</v>
       </c>
       <c r="W299">
-        <f t="shared" ref="W299" si="325">(SUM(G299:H307))/10</f>
+        <f t="shared" ref="W299" si="323">(SUM(G299:H307))/10</f>
         <v>0.4</v>
       </c>
       <c r="X299">
-        <f t="shared" ref="X299" si="326">(SUM(I299:I307))/5</f>
+        <f t="shared" ref="X299" si="324">(SUM(I299:I307))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y299">
-        <f t="shared" ref="Y299" si="327">SUM(K299:K307)-Z299</f>
+        <f t="shared" ref="Y299" si="325">SUM(K299:K307)-Z299</f>
         <v>76</v>
       </c>
       <c r="Z299">
-        <f t="shared" ref="Z299" si="328">SUM(L299:L307)</f>
+        <f t="shared" ref="Z299" si="326">SUM(L299:L307)</f>
         <v>10</v>
       </c>
       <c r="AA299" t="s">
@@ -57887,17 +57886,17 @@
       <c r="B301" t="s">
         <v>775</v>
       </c>
-      <c r="C301" t="s">
-        <v>30</v>
-      </c>
-      <c r="D301" t="s">
-        <v>30</v>
-      </c>
-      <c r="E301" t="s">
-        <v>30</v>
-      </c>
-      <c r="F301" t="s">
-        <v>30</v>
+      <c r="C301">
+        <v>15</v>
+      </c>
+      <c r="D301">
+        <v>15</v>
+      </c>
+      <c r="E301">
+        <v>14</v>
+      </c>
+      <c r="F301">
+        <v>16</v>
       </c>
       <c r="G301">
         <v>0</v>
@@ -57987,17 +57986,17 @@
       <c r="B303" t="s">
         <v>777</v>
       </c>
-      <c r="C303" t="s">
-        <v>30</v>
-      </c>
-      <c r="D303" t="s">
-        <v>30</v>
-      </c>
-      <c r="E303" t="s">
-        <v>30</v>
-      </c>
-      <c r="F303" t="s">
-        <v>30</v>
+      <c r="C303">
+        <v>5</v>
+      </c>
+      <c r="D303">
+        <v>4</v>
+      </c>
+      <c r="E303">
+        <v>8</v>
+      </c>
+      <c r="F303">
+        <v>6</v>
       </c>
       <c r="G303">
         <v>1</v>
@@ -58087,17 +58086,17 @@
       <c r="B305" t="s">
         <v>779</v>
       </c>
-      <c r="C305" t="s">
-        <v>30</v>
-      </c>
-      <c r="D305" t="s">
-        <v>30</v>
-      </c>
-      <c r="E305" t="s">
-        <v>30</v>
-      </c>
-      <c r="F305" t="s">
-        <v>30</v>
+      <c r="C305">
+        <v>8</v>
+      </c>
+      <c r="D305">
+        <v>12</v>
+      </c>
+      <c r="E305">
+        <v>11</v>
+      </c>
+      <c r="F305">
+        <v>13</v>
       </c>
       <c r="G305">
         <v>0</v>
@@ -58187,17 +58186,17 @@
       <c r="B307" t="s">
         <v>781</v>
       </c>
-      <c r="C307" t="s">
-        <v>30</v>
-      </c>
-      <c r="D307" t="s">
-        <v>30</v>
-      </c>
-      <c r="E307" t="s">
-        <v>30</v>
-      </c>
-      <c r="F307" t="s">
-        <v>30</v>
+      <c r="C307">
+        <v>14</v>
+      </c>
+      <c r="D307">
+        <v>7</v>
+      </c>
+      <c r="E307">
+        <v>5</v>
+      </c>
+      <c r="F307">
+        <v>7</v>
       </c>
       <c r="G307">
         <v>0</v>
@@ -58237,17 +58236,17 @@
       <c r="B308" t="s">
         <v>772</v>
       </c>
-      <c r="C308" t="s">
-        <v>30</v>
-      </c>
-      <c r="D308" t="s">
-        <v>30</v>
-      </c>
-      <c r="E308" t="s">
-        <v>30</v>
-      </c>
-      <c r="F308" t="s">
-        <v>30</v>
+      <c r="C308">
+        <v>15</v>
+      </c>
+      <c r="D308">
+        <v>18</v>
+      </c>
+      <c r="E308">
+        <v>10</v>
+      </c>
+      <c r="F308">
+        <v>10</v>
       </c>
       <c r="G308">
         <v>0</v>
@@ -58277,47 +58276,47 @@
         <v>29</v>
       </c>
       <c r="P308">
-        <f t="shared" ref="P308" si="329">M308*10</f>
+        <f t="shared" ref="P308" si="327">M308*10</f>
         <v>60</v>
       </c>
       <c r="Q308">
-        <f t="shared" ref="Q308" si="330">((SUM(C308:F308))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="Q308" si="328">((SUM(C308:F308))/4)*1.04</f>
+        <v>13.780000000000001</v>
       </c>
       <c r="R308">
-        <f t="shared" ref="R308" si="331">((SUM(C310:F310))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="R308" si="329">((SUM(C310:F310))/4)*1.04</f>
+        <v>10.66</v>
       </c>
       <c r="S308">
-        <f t="shared" ref="S308" si="332">((SUM(C312:F312))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="S308" si="330">((SUM(C312:F312))/4)*1.04</f>
+        <v>8.06</v>
       </c>
       <c r="T308">
-        <f t="shared" ref="T308" si="333">((SUM(C314:F314))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="T308" si="331">((SUM(C314:F314))/4)*1.04</f>
+        <v>10.4</v>
       </c>
       <c r="U308">
-        <f t="shared" ref="U308" si="334">((SUM(C316:F316))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="U308" si="332">((SUM(C316:F316))/4)*1.04</f>
+        <v>18.98</v>
       </c>
       <c r="V308">
-        <f t="shared" ref="V308" si="335">((SUM(C308:F316))/20)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="V308" si="333">((SUM(C308:F316))/20)*1.04</f>
+        <v>12.376000000000001</v>
       </c>
       <c r="W308">
-        <f t="shared" ref="W308" si="336">(SUM(G308:H316))/10</f>
+        <f t="shared" ref="W308" si="334">(SUM(G308:H316))/10</f>
         <v>42.7</v>
       </c>
       <c r="X308">
-        <f t="shared" ref="X308" si="337">(SUM(I308:I316))/5</f>
+        <f t="shared" ref="X308" si="335">(SUM(I308:I316))/5</f>
         <v>2</v>
       </c>
       <c r="Y308">
-        <f t="shared" ref="Y308" si="338">SUM(K308:K316)-Z308</f>
+        <f t="shared" ref="Y308" si="336">SUM(K308:K316)-Z308</f>
         <v>80</v>
       </c>
       <c r="Z308">
-        <f t="shared" ref="Z308" si="339">SUM(L308:L316)</f>
+        <f t="shared" ref="Z308" si="337">SUM(L308:L316)</f>
         <v>5</v>
       </c>
       <c r="AA308" t="s">
@@ -58381,17 +58380,17 @@
       <c r="B310" t="s">
         <v>775</v>
       </c>
-      <c r="C310" t="s">
-        <v>30</v>
-      </c>
-      <c r="D310" t="s">
-        <v>30</v>
-      </c>
-      <c r="E310" t="s">
-        <v>30</v>
-      </c>
-      <c r="F310" t="s">
-        <v>30</v>
+      <c r="C310">
+        <v>17</v>
+      </c>
+      <c r="D310">
+        <v>4</v>
+      </c>
+      <c r="E310">
+        <v>8</v>
+      </c>
+      <c r="F310">
+        <v>12</v>
       </c>
       <c r="G310">
         <v>75</v>
@@ -58481,17 +58480,17 @@
       <c r="B312" t="s">
         <v>777</v>
       </c>
-      <c r="C312" t="s">
-        <v>30</v>
-      </c>
-      <c r="D312" t="s">
-        <v>30</v>
-      </c>
-      <c r="E312" t="s">
-        <v>30</v>
-      </c>
-      <c r="F312" t="s">
-        <v>30</v>
+      <c r="C312">
+        <v>5</v>
+      </c>
+      <c r="D312">
+        <v>11</v>
+      </c>
+      <c r="E312">
+        <v>5</v>
+      </c>
+      <c r="F312">
+        <v>10</v>
       </c>
       <c r="G312">
         <v>80</v>
@@ -58581,17 +58580,17 @@
       <c r="B314" t="s">
         <v>779</v>
       </c>
-      <c r="C314" t="s">
-        <v>30</v>
-      </c>
-      <c r="D314" t="s">
-        <v>30</v>
-      </c>
-      <c r="E314" t="s">
-        <v>30</v>
-      </c>
-      <c r="F314" t="s">
-        <v>30</v>
+      <c r="C314">
+        <v>8</v>
+      </c>
+      <c r="D314">
+        <v>10</v>
+      </c>
+      <c r="E314">
+        <v>8</v>
+      </c>
+      <c r="F314">
+        <v>14</v>
       </c>
       <c r="G314">
         <v>80</v>
@@ -58681,17 +58680,17 @@
       <c r="B316" t="s">
         <v>781</v>
       </c>
-      <c r="C316" t="s">
-        <v>30</v>
-      </c>
-      <c r="D316" t="s">
-        <v>30</v>
-      </c>
-      <c r="E316" t="s">
-        <v>30</v>
-      </c>
-      <c r="F316" t="s">
-        <v>30</v>
+      <c r="C316">
+        <v>16</v>
+      </c>
+      <c r="D316">
+        <v>16</v>
+      </c>
+      <c r="E316">
+        <v>19</v>
+      </c>
+      <c r="F316">
+        <v>22</v>
       </c>
       <c r="G316">
         <v>20</v>
@@ -58731,17 +58730,17 @@
       <c r="B317" t="s">
         <v>772</v>
       </c>
-      <c r="C317" t="s">
-        <v>30</v>
-      </c>
-      <c r="D317" t="s">
-        <v>30</v>
-      </c>
-      <c r="E317" t="s">
-        <v>30</v>
-      </c>
-      <c r="F317" t="s">
-        <v>30</v>
+      <c r="C317">
+        <v>15</v>
+      </c>
+      <c r="D317">
+        <v>27</v>
+      </c>
+      <c r="E317">
+        <v>20</v>
+      </c>
+      <c r="F317">
+        <v>25</v>
       </c>
       <c r="G317">
         <v>30</v>
@@ -58771,47 +58770,47 @@
         <v>240</v>
       </c>
       <c r="P317">
-        <f t="shared" ref="P317" si="340">M317*10</f>
+        <f t="shared" ref="P317" si="338">M317*10</f>
         <v>60</v>
       </c>
       <c r="Q317">
-        <f t="shared" ref="Q317" si="341">((SUM(C317:F317))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="Q317" si="339">((SUM(C317:F317))/4)*1.04</f>
+        <v>22.62</v>
       </c>
       <c r="R317">
-        <f t="shared" ref="R317" si="342">((SUM(C319:F319))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="R317" si="340">((SUM(C319:F319))/4)*1.04</f>
+        <v>21.32</v>
       </c>
       <c r="S317">
-        <f t="shared" ref="S317" si="343">((SUM(C321:F321))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="S317" si="341">((SUM(C321:F321))/4)*1.04</f>
+        <v>26.78</v>
       </c>
       <c r="T317">
-        <f t="shared" ref="T317" si="344">((SUM(C323:F323))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="T317" si="342">((SUM(C323:F323))/4)*1.04</f>
+        <v>23.14</v>
       </c>
       <c r="U317">
-        <f t="shared" ref="U317" si="345">((SUM(C325:F325))/4)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="U317" si="343">((SUM(C325:F325))/4)*1.04</f>
+        <v>43.940000000000005</v>
       </c>
       <c r="V317">
-        <f t="shared" ref="V317" si="346">((SUM(C317:F325))/20)*1.04</f>
-        <v>0</v>
+        <f t="shared" ref="V317" si="344">((SUM(C317:F325))/20)*1.04</f>
+        <v>27.560000000000002</v>
       </c>
       <c r="W317">
-        <f t="shared" ref="W317" si="347">(SUM(G317:H325))/10</f>
+        <f t="shared" ref="W317" si="345">(SUM(G317:H325))/10</f>
         <v>16.5</v>
       </c>
       <c r="X317">
-        <f t="shared" ref="X317" si="348">(SUM(I317:I325))/5</f>
+        <f t="shared" ref="X317" si="346">(SUM(I317:I325))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y317">
-        <f t="shared" ref="Y317" si="349">SUM(K317:K325)-Z317</f>
+        <f t="shared" ref="Y317" si="347">SUM(K317:K325)-Z317</f>
         <v>19</v>
       </c>
       <c r="Z317">
-        <f t="shared" ref="Z317" si="350">SUM(L317:L325)</f>
+        <f t="shared" ref="Z317" si="348">SUM(L317:L325)</f>
         <v>2</v>
       </c>
       <c r="AA317" t="s">
@@ -58875,17 +58874,17 @@
       <c r="B319" t="s">
         <v>775</v>
       </c>
-      <c r="C319" t="s">
-        <v>30</v>
-      </c>
-      <c r="D319" t="s">
-        <v>30</v>
-      </c>
-      <c r="E319" t="s">
-        <v>30</v>
-      </c>
-      <c r="F319" t="s">
-        <v>30</v>
+      <c r="C319">
+        <v>22</v>
+      </c>
+      <c r="D319">
+        <v>29</v>
+      </c>
+      <c r="E319">
+        <v>16</v>
+      </c>
+      <c r="F319">
+        <v>15</v>
       </c>
       <c r="G319">
         <v>10</v>
@@ -58975,17 +58974,17 @@
       <c r="B321" t="s">
         <v>777</v>
       </c>
-      <c r="C321" t="s">
-        <v>30</v>
-      </c>
-      <c r="D321" t="s">
-        <v>30</v>
-      </c>
-      <c r="E321" t="s">
-        <v>30</v>
-      </c>
-      <c r="F321" t="s">
-        <v>30</v>
+      <c r="C321">
+        <v>35</v>
+      </c>
+      <c r="D321">
+        <v>37</v>
+      </c>
+      <c r="E321">
+        <v>6</v>
+      </c>
+      <c r="F321">
+        <v>25</v>
       </c>
       <c r="G321">
         <v>20</v>
@@ -59075,17 +59074,17 @@
       <c r="B323" t="s">
         <v>779</v>
       </c>
-      <c r="C323" t="s">
-        <v>30</v>
-      </c>
-      <c r="D323" t="s">
-        <v>30</v>
-      </c>
-      <c r="E323" t="s">
-        <v>30</v>
-      </c>
-      <c r="F323" t="s">
-        <v>30</v>
+      <c r="C323">
+        <v>34</v>
+      </c>
+      <c r="D323">
+        <v>18</v>
+      </c>
+      <c r="E323">
+        <v>17</v>
+      </c>
+      <c r="F323">
+        <v>20</v>
       </c>
       <c r="G323">
         <v>10</v>
@@ -59175,17 +59174,17 @@
       <c r="B325" t="s">
         <v>781</v>
       </c>
-      <c r="C325" t="s">
-        <v>30</v>
-      </c>
-      <c r="D325" t="s">
-        <v>30</v>
-      </c>
-      <c r="E325" t="s">
-        <v>30</v>
-      </c>
-      <c r="F325" t="s">
-        <v>30</v>
+      <c r="C325">
+        <v>45</v>
+      </c>
+      <c r="D325">
+        <v>42</v>
+      </c>
+      <c r="E325">
+        <v>40</v>
+      </c>
+      <c r="F325">
+        <v>42</v>
       </c>
       <c r="G325">
         <v>10</v>
@@ -59265,47 +59264,47 @@
         <v>43</v>
       </c>
       <c r="P326" t="e">
-        <f t="shared" ref="P326" si="351">M326*10</f>
+        <f t="shared" ref="P326" si="349">M326*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q326">
-        <f t="shared" ref="Q326" si="352">((SUM(C326:F326))/4)*1.04</f>
+        <f t="shared" ref="Q326" si="350">((SUM(C326:F326))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R326">
-        <f t="shared" ref="R326" si="353">((SUM(C328:F328))/4)*1.04</f>
+        <f t="shared" ref="R326" si="351">((SUM(C328:F328))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S326">
-        <f t="shared" ref="S326" si="354">((SUM(C330:F330))/4)*1.04</f>
+        <f t="shared" ref="S326" si="352">((SUM(C330:F330))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T326">
-        <f t="shared" ref="T326" si="355">((SUM(C332:F332))/4)*1.04</f>
+        <f t="shared" ref="T326" si="353">((SUM(C332:F332))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U326">
-        <f t="shared" ref="U326" si="356">((SUM(C334:F334))/4)*1.04</f>
+        <f t="shared" ref="U326" si="354">((SUM(C334:F334))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V326">
-        <f t="shared" ref="V326" si="357">((SUM(C326:F334))/20)*1.04</f>
+        <f t="shared" ref="V326" si="355">((SUM(C326:F334))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W326">
-        <f t="shared" ref="W326" si="358">(SUM(G326:H334))/10</f>
+        <f t="shared" ref="W326" si="356">(SUM(G326:H334))/10</f>
         <v>50.5</v>
       </c>
       <c r="X326">
-        <f t="shared" ref="X326" si="359">(SUM(I326:I334))/5</f>
+        <f t="shared" ref="X326" si="357">(SUM(I326:I334))/5</f>
         <v>1.6</v>
       </c>
       <c r="Y326">
-        <f t="shared" ref="Y326" si="360">SUM(K326:K334)-Z326</f>
+        <f t="shared" ref="Y326" si="358">SUM(K326:K334)-Z326</f>
         <v>32</v>
       </c>
       <c r="Z326">
-        <f t="shared" ref="Z326" si="361">SUM(L326:L334)</f>
+        <f t="shared" ref="Z326" si="359">SUM(L326:L334)</f>
         <v>2</v>
       </c>
       <c r="AA326" t="s">
@@ -59759,47 +59758,47 @@
         <v>240</v>
       </c>
       <c r="P335" t="e">
-        <f t="shared" ref="P335" si="362">M335*10</f>
+        <f t="shared" ref="P335" si="360">M335*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q335">
-        <f t="shared" ref="Q335" si="363">((SUM(C335:F335))/4)*1.04</f>
+        <f t="shared" ref="Q335" si="361">((SUM(C335:F335))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R335">
-        <f t="shared" ref="R335" si="364">((SUM(C337:F337))/4)*1.04</f>
+        <f t="shared" ref="R335" si="362">((SUM(C337:F337))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S335">
-        <f t="shared" ref="S335" si="365">((SUM(C339:F339))/4)*1.04</f>
+        <f t="shared" ref="S335" si="363">((SUM(C339:F339))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T335">
-        <f t="shared" ref="T335" si="366">((SUM(C341:F341))/4)*1.04</f>
+        <f t="shared" ref="T335" si="364">((SUM(C341:F341))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U335">
-        <f t="shared" ref="U335" si="367">((SUM(C343:F343))/4)*1.04</f>
+        <f t="shared" ref="U335" si="365">((SUM(C343:F343))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V335">
-        <f t="shared" ref="V335" si="368">((SUM(C335:F343))/20)*1.04</f>
+        <f t="shared" ref="V335" si="366">((SUM(C335:F343))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W335">
-        <f t="shared" ref="W335" si="369">(SUM(G335:H343))/10</f>
+        <f t="shared" ref="W335" si="367">(SUM(G335:H343))/10</f>
         <v>47</v>
       </c>
       <c r="X335">
-        <f t="shared" ref="X335" si="370">(SUM(I335:I343))/5</f>
+        <f t="shared" ref="X335" si="368">(SUM(I335:I343))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y335">
-        <f t="shared" ref="Y335" si="371">SUM(K335:K343)-Z335</f>
+        <f t="shared" ref="Y335" si="369">SUM(K335:K343)-Z335</f>
         <v>24</v>
       </c>
       <c r="Z335">
-        <f t="shared" ref="Z335" si="372">SUM(L335:L343)</f>
+        <f t="shared" ref="Z335" si="370">SUM(L335:L343)</f>
         <v>0</v>
       </c>
       <c r="AA335" t="s">
@@ -60253,47 +60252,47 @@
         <v>43</v>
       </c>
       <c r="P344">
-        <f t="shared" ref="P344" si="373">M344*10</f>
+        <f t="shared" ref="P344" si="371">M344*10</f>
         <v>100</v>
       </c>
       <c r="Q344">
-        <f t="shared" ref="Q344" si="374">((SUM(C344:F344))/4)*1.04</f>
+        <f t="shared" ref="Q344" si="372">((SUM(C344:F344))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R344">
-        <f t="shared" ref="R344" si="375">((SUM(C346:F346))/4)*1.04</f>
+        <f t="shared" ref="R344" si="373">((SUM(C346:F346))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S344">
-        <f t="shared" ref="S344" si="376">((SUM(C348:F348))/4)*1.04</f>
+        <f t="shared" ref="S344" si="374">((SUM(C348:F348))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T344">
-        <f t="shared" ref="T344" si="377">((SUM(C350:F350))/4)*1.04</f>
+        <f t="shared" ref="T344" si="375">((SUM(C350:F350))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U344">
-        <f t="shared" ref="U344" si="378">((SUM(C352:F352))/4)*1.04</f>
+        <f t="shared" ref="U344" si="376">((SUM(C352:F352))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V344">
-        <f t="shared" ref="V344" si="379">((SUM(C344:F352))/20)*1.04</f>
+        <f t="shared" ref="V344" si="377">((SUM(C344:F352))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W344">
-        <f t="shared" ref="W344" si="380">(SUM(G344:H352))/10</f>
+        <f t="shared" ref="W344" si="378">(SUM(G344:H352))/10</f>
         <v>1.7</v>
       </c>
       <c r="X344">
-        <f t="shared" ref="X344" si="381">(SUM(I344:I352))/5</f>
+        <f t="shared" ref="X344" si="379">(SUM(I344:I352))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y344">
-        <f t="shared" ref="Y344" si="382">SUM(K344:K352)-Z344</f>
+        <f t="shared" ref="Y344" si="380">SUM(K344:K352)-Z344</f>
         <v>62</v>
       </c>
       <c r="Z344">
-        <f t="shared" ref="Z344" si="383">SUM(L344:L352)</f>
+        <f t="shared" ref="Z344" si="381">SUM(L344:L352)</f>
         <v>7</v>
       </c>
       <c r="AA344" t="s">
@@ -60747,47 +60746,47 @@
         <v>43</v>
       </c>
       <c r="P353">
-        <f t="shared" ref="P353" si="384">M353*10</f>
+        <f t="shared" ref="P353" si="382">M353*10</f>
         <v>90</v>
       </c>
       <c r="Q353">
-        <f t="shared" ref="Q353" si="385">((SUM(C353:F353))/4)*1.04</f>
+        <f t="shared" ref="Q353" si="383">((SUM(C353:F353))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R353">
-        <f t="shared" ref="R353" si="386">((SUM(C355:F355))/4)*1.04</f>
+        <f t="shared" ref="R353" si="384">((SUM(C355:F355))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S353">
-        <f t="shared" ref="S353" si="387">((SUM(C357:F357))/4)*1.04</f>
+        <f t="shared" ref="S353" si="385">((SUM(C357:F357))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T353">
-        <f t="shared" ref="T353" si="388">((SUM(C359:F359))/4)*1.04</f>
+        <f t="shared" ref="T353" si="386">((SUM(C359:F359))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U353">
-        <f t="shared" ref="U353" si="389">((SUM(C361:F361))/4)*1.04</f>
+        <f t="shared" ref="U353" si="387">((SUM(C361:F361))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V353">
-        <f t="shared" ref="V353" si="390">((SUM(C353:F361))/20)*1.04</f>
+        <f t="shared" ref="V353" si="388">((SUM(C353:F361))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W353">
-        <f t="shared" ref="W353" si="391">(SUM(G353:H361))/10</f>
+        <f t="shared" ref="W353" si="389">(SUM(G353:H361))/10</f>
         <v>2.4</v>
       </c>
       <c r="X353">
-        <f t="shared" ref="X353" si="392">(SUM(I353:I361))/5</f>
+        <f t="shared" ref="X353" si="390">(SUM(I353:I361))/5</f>
         <v>3.8</v>
       </c>
       <c r="Y353">
-        <f t="shared" ref="Y353" si="393">SUM(K353:K361)-Z353</f>
+        <f t="shared" ref="Y353" si="391">SUM(K353:K361)-Z353</f>
         <v>54</v>
       </c>
       <c r="Z353">
-        <f t="shared" ref="Z353" si="394">SUM(L353:L361)</f>
+        <f t="shared" ref="Z353" si="392">SUM(L353:L361)</f>
         <v>6</v>
       </c>
       <c r="AA353" t="s">
@@ -61241,47 +61240,47 @@
         <v>29</v>
       </c>
       <c r="P362">
-        <f t="shared" ref="P362" si="395">M362*10</f>
+        <f t="shared" ref="P362" si="393">M362*10</f>
         <v>50</v>
       </c>
       <c r="Q362">
-        <f t="shared" ref="Q362" si="396">((SUM(C362:F362))/4)*1.04</f>
+        <f t="shared" ref="Q362" si="394">((SUM(C362:F362))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R362">
-        <f t="shared" ref="R362" si="397">((SUM(C364:F364))/4)*1.04</f>
+        <f t="shared" ref="R362" si="395">((SUM(C364:F364))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S362">
-        <f t="shared" ref="S362" si="398">((SUM(C366:F366))/4)*1.04</f>
+        <f t="shared" ref="S362" si="396">((SUM(C366:F366))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T362">
-        <f t="shared" ref="T362" si="399">((SUM(C368:F368))/4)*1.04</f>
+        <f t="shared" ref="T362" si="397">((SUM(C368:F368))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U362">
-        <f t="shared" ref="U362" si="400">((SUM(C370:F370))/4)*1.04</f>
+        <f t="shared" ref="U362" si="398">((SUM(C370:F370))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V362">
-        <f t="shared" ref="V362" si="401">((SUM(C362:F370))/20)*1.04</f>
+        <f t="shared" ref="V362" si="399">((SUM(C362:F370))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W362">
-        <f t="shared" ref="W362" si="402">(SUM(G362:H370))/10</f>
+        <f t="shared" ref="W362" si="400">(SUM(G362:H370))/10</f>
         <v>18.100000000000001</v>
       </c>
       <c r="X362">
-        <f t="shared" ref="X362" si="403">(SUM(I362:I370))/5</f>
+        <f t="shared" ref="X362" si="401">(SUM(I362:I370))/5</f>
         <v>2.4</v>
       </c>
       <c r="Y362">
-        <f t="shared" ref="Y362" si="404">SUM(K362:K370)-Z362</f>
+        <f t="shared" ref="Y362" si="402">SUM(K362:K370)-Z362</f>
         <v>60</v>
       </c>
       <c r="Z362">
-        <f t="shared" ref="Z362" si="405">SUM(L362:L370)</f>
+        <f t="shared" ref="Z362" si="403">SUM(L362:L370)</f>
         <v>8</v>
       </c>
       <c r="AA362" t="s">
@@ -61735,47 +61734,47 @@
         <v>29</v>
       </c>
       <c r="P371">
-        <f t="shared" ref="P371" si="406">M371*10</f>
+        <f t="shared" ref="P371" si="404">M371*10</f>
         <v>100</v>
       </c>
       <c r="Q371">
-        <f t="shared" ref="Q371" si="407">((SUM(C371:F371))/4)*1.04</f>
+        <f t="shared" ref="Q371" si="405">((SUM(C371:F371))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R371">
-        <f t="shared" ref="R371" si="408">((SUM(C373:F373))/4)*1.04</f>
+        <f t="shared" ref="R371" si="406">((SUM(C373:F373))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S371">
-        <f t="shared" ref="S371" si="409">((SUM(C375:F375))/4)*1.04</f>
+        <f t="shared" ref="S371" si="407">((SUM(C375:F375))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T371">
-        <f t="shared" ref="T371" si="410">((SUM(C377:F377))/4)*1.04</f>
+        <f t="shared" ref="T371" si="408">((SUM(C377:F377))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U371">
-        <f t="shared" ref="U371" si="411">((SUM(C379:F379))/4)*1.04</f>
+        <f t="shared" ref="U371" si="409">((SUM(C379:F379))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V371">
-        <f t="shared" ref="V371" si="412">((SUM(C371:F379))/20)*1.04</f>
+        <f t="shared" ref="V371" si="410">((SUM(C371:F379))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W371">
-        <f t="shared" ref="W371" si="413">(SUM(G371:H379))/10</f>
+        <f t="shared" ref="W371" si="411">(SUM(G371:H379))/10</f>
         <v>88.7</v>
       </c>
       <c r="X371">
-        <f t="shared" ref="X371" si="414">(SUM(I371:I379))/5</f>
+        <f t="shared" ref="X371" si="412">(SUM(I371:I379))/5</f>
         <v>1</v>
       </c>
       <c r="Y371">
-        <f t="shared" ref="Y371" si="415">SUM(K371:K379)-Z371</f>
+        <f t="shared" ref="Y371" si="413">SUM(K371:K379)-Z371</f>
         <v>33</v>
       </c>
       <c r="Z371">
-        <f t="shared" ref="Z371" si="416">SUM(L371:L379)</f>
+        <f t="shared" ref="Z371" si="414">SUM(L371:L379)</f>
         <v>6</v>
       </c>
       <c r="AA371" t="s">
@@ -62229,47 +62228,47 @@
         <v>67</v>
       </c>
       <c r="P380">
-        <f t="shared" ref="P380" si="417">M380*10</f>
+        <f t="shared" ref="P380" si="415">M380*10</f>
         <v>100</v>
       </c>
       <c r="Q380">
-        <f t="shared" ref="Q380" si="418">((SUM(C380:F380))/4)*1.04</f>
+        <f t="shared" ref="Q380" si="416">((SUM(C380:F380))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R380">
-        <f t="shared" ref="R380" si="419">((SUM(C382:F382))/4)*1.04</f>
+        <f t="shared" ref="R380" si="417">((SUM(C382:F382))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S380">
-        <f t="shared" ref="S380" si="420">((SUM(C384:F384))/4)*1.04</f>
+        <f t="shared" ref="S380" si="418">((SUM(C384:F384))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T380">
-        <f t="shared" ref="T380" si="421">((SUM(C386:F386))/4)*1.04</f>
+        <f t="shared" ref="T380" si="419">((SUM(C386:F386))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U380">
-        <f t="shared" ref="U380" si="422">((SUM(C388:F388))/4)*1.04</f>
+        <f t="shared" ref="U380" si="420">((SUM(C388:F388))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V380">
-        <f t="shared" ref="V380" si="423">((SUM(C380:F388))/20)*1.04</f>
+        <f t="shared" ref="V380" si="421">((SUM(C380:F388))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W380">
-        <f t="shared" ref="W380" si="424">(SUM(G380:H388))/10</f>
+        <f t="shared" ref="W380" si="422">(SUM(G380:H388))/10</f>
         <v>35.1</v>
       </c>
       <c r="X380">
-        <f t="shared" ref="X380" si="425">(SUM(I380:I388))/5</f>
+        <f t="shared" ref="X380" si="423">(SUM(I380:I388))/5</f>
         <v>2</v>
       </c>
       <c r="Y380">
-        <f t="shared" ref="Y380" si="426">SUM(K380:K388)-Z380</f>
+        <f t="shared" ref="Y380" si="424">SUM(K380:K388)-Z380</f>
         <v>57</v>
       </c>
       <c r="Z380">
-        <f t="shared" ref="Z380" si="427">SUM(L380:L388)</f>
+        <f t="shared" ref="Z380" si="425">SUM(L380:L388)</f>
         <v>5</v>
       </c>
       <c r="AA380" t="s">
@@ -62727,43 +62726,43 @@
         <v>#VALUE!</v>
       </c>
       <c r="Q389">
-        <f t="shared" ref="Q389" si="428">((SUM(C389:F389))/4)*1.04</f>
+        <f t="shared" ref="Q389" si="426">((SUM(C389:F389))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R389">
-        <f t="shared" ref="R389" si="429">((SUM(C391:F391))/4)*1.04</f>
+        <f t="shared" ref="R389" si="427">((SUM(C391:F391))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S389">
-        <f t="shared" ref="S389" si="430">((SUM(C393:F393))/4)*1.04</f>
+        <f t="shared" ref="S389" si="428">((SUM(C393:F393))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T389">
-        <f t="shared" ref="T389" si="431">((SUM(C395:F395))/4)*1.04</f>
+        <f t="shared" ref="T389" si="429">((SUM(C395:F395))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U389">
-        <f t="shared" ref="U389" si="432">((SUM(C397:F397))/4)*1.04</f>
+        <f t="shared" ref="U389" si="430">((SUM(C397:F397))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V389">
-        <f t="shared" ref="V389" si="433">((SUM(C389:F397))/20)*1.04</f>
+        <f t="shared" ref="V389" si="431">((SUM(C389:F397))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W389">
-        <f t="shared" ref="W389" si="434">(SUM(G389:H397))/10</f>
+        <f t="shared" ref="W389" si="432">(SUM(G389:H397))/10</f>
         <v>1.7</v>
       </c>
       <c r="X389">
-        <f t="shared" ref="X389" si="435">(SUM(I389:I397))/5</f>
+        <f t="shared" ref="X389" si="433">(SUM(I389:I397))/5</f>
         <v>2.4</v>
       </c>
       <c r="Y389">
-        <f t="shared" ref="Y389" si="436">SUM(K389:K397)-Z389</f>
+        <f t="shared" ref="Y389" si="434">SUM(K389:K397)-Z389</f>
         <v>84</v>
       </c>
       <c r="Z389">
-        <f t="shared" ref="Z389" si="437">SUM(L389:L397)</f>
+        <f t="shared" ref="Z389" si="435">SUM(L389:L397)</f>
         <v>11</v>
       </c>
       <c r="AA389" t="s">
@@ -63217,47 +63216,47 @@
         <v>43</v>
       </c>
       <c r="P398">
-        <f t="shared" ref="P398" si="438">M398*10</f>
+        <f t="shared" ref="P398" si="436">M398*10</f>
         <v>40</v>
       </c>
       <c r="Q398">
-        <f t="shared" ref="Q398" si="439">((SUM(C398:F398))/4)*1.04</f>
+        <f t="shared" ref="Q398" si="437">((SUM(C398:F398))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R398">
-        <f t="shared" ref="R398" si="440">((SUM(C400:F400))/4)*1.04</f>
+        <f t="shared" ref="R398" si="438">((SUM(C400:F400))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S398">
-        <f t="shared" ref="S398" si="441">((SUM(C402:F402))/4)*1.04</f>
+        <f t="shared" ref="S398" si="439">((SUM(C402:F402))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T398">
-        <f t="shared" ref="T398" si="442">((SUM(C404:F404))/4)*1.04</f>
+        <f t="shared" ref="T398" si="440">((SUM(C404:F404))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U398">
-        <f t="shared" ref="U398" si="443">((SUM(C406:F406))/4)*1.04</f>
+        <f t="shared" ref="U398" si="441">((SUM(C406:F406))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V398">
-        <f t="shared" ref="V398" si="444">((SUM(C398:F406))/20)*1.04</f>
+        <f t="shared" ref="V398" si="442">((SUM(C398:F406))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W398">
-        <f t="shared" ref="W398" si="445">(SUM(G398:H406))/10</f>
+        <f t="shared" ref="W398" si="443">(SUM(G398:H406))/10</f>
         <v>19.7</v>
       </c>
       <c r="X398">
-        <f t="shared" ref="X398" si="446">(SUM(I398:I406))/5</f>
+        <f t="shared" ref="X398" si="444">(SUM(I398:I406))/5</f>
         <v>3.6</v>
       </c>
       <c r="Y398">
-        <f t="shared" ref="Y398" si="447">SUM(K398:K406)-Z398</f>
+        <f t="shared" ref="Y398" si="445">SUM(K398:K406)-Z398</f>
         <v>68</v>
       </c>
       <c r="Z398">
-        <f t="shared" ref="Z398" si="448">SUM(L398:L406)</f>
+        <f t="shared" ref="Z398" si="446">SUM(L398:L406)</f>
         <v>2</v>
       </c>
       <c r="AA398" t="s">
@@ -63711,47 +63710,47 @@
         <v>67</v>
       </c>
       <c r="P407">
-        <f t="shared" ref="P407" si="449">M407*10</f>
+        <f t="shared" ref="P407" si="447">M407*10</f>
         <v>40</v>
       </c>
       <c r="Q407">
-        <f t="shared" ref="Q407" si="450">((SUM(C407:F407))/4)*1.04</f>
+        <f t="shared" ref="Q407" si="448">((SUM(C407:F407))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R407">
-        <f t="shared" ref="R407" si="451">((SUM(C409:F409))/4)*1.04</f>
+        <f t="shared" ref="R407" si="449">((SUM(C409:F409))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S407">
-        <f t="shared" ref="S407" si="452">((SUM(C411:F411))/4)*1.04</f>
+        <f t="shared" ref="S407" si="450">((SUM(C411:F411))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T407">
-        <f t="shared" ref="T407" si="453">((SUM(C413:F413))/4)*1.04</f>
+        <f t="shared" ref="T407" si="451">((SUM(C413:F413))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U407">
-        <f t="shared" ref="U407" si="454">((SUM(C415:F415))/4)*1.04</f>
+        <f t="shared" ref="U407" si="452">((SUM(C415:F415))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V407">
-        <f t="shared" ref="V407" si="455">((SUM(C407:F415))/20)*1.04</f>
+        <f t="shared" ref="V407" si="453">((SUM(C407:F415))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W407">
-        <f t="shared" ref="W407" si="456">(SUM(G407:H415))/10</f>
+        <f t="shared" ref="W407" si="454">(SUM(G407:H415))/10</f>
         <v>41.3</v>
       </c>
       <c r="X407">
-        <f t="shared" ref="X407" si="457">(SUM(I407:I415))/5</f>
+        <f t="shared" ref="X407" si="455">(SUM(I407:I415))/5</f>
         <v>2.4</v>
       </c>
       <c r="Y407">
-        <f t="shared" ref="Y407" si="458">SUM(K407:K415)-Z407</f>
+        <f t="shared" ref="Y407" si="456">SUM(K407:K415)-Z407</f>
         <v>81</v>
       </c>
       <c r="Z407">
-        <f t="shared" ref="Z407" si="459">SUM(L407:L415)</f>
+        <f t="shared" ref="Z407" si="457">SUM(L407:L415)</f>
         <v>12</v>
       </c>
       <c r="AA407" t="s">
@@ -64205,47 +64204,47 @@
         <v>560</v>
       </c>
       <c r="P416" t="e">
-        <f t="shared" ref="P416" si="460">M416*10</f>
+        <f t="shared" ref="P416" si="458">M416*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q416">
-        <f t="shared" ref="Q416" si="461">((SUM(C416:F416))/4)*1.04</f>
+        <f t="shared" ref="Q416" si="459">((SUM(C416:F416))/4)*1.04</f>
         <v>37.700000000000003</v>
       </c>
       <c r="R416">
-        <f t="shared" ref="R416" si="462">((SUM(C418:F418))/4)*1.04</f>
+        <f t="shared" ref="R416" si="460">((SUM(C418:F418))/4)*1.04</f>
         <v>18.46</v>
       </c>
       <c r="S416">
-        <f t="shared" ref="S416" si="463">((SUM(C420:F420))/4)*1.04</f>
+        <f t="shared" ref="S416" si="461">((SUM(C420:F420))/4)*1.04</f>
         <v>5.2</v>
       </c>
       <c r="T416">
-        <f t="shared" ref="T416" si="464">((SUM(C422:F422))/4)*1.04</f>
+        <f t="shared" ref="T416" si="462">((SUM(C422:F422))/4)*1.04</f>
         <v>7.8000000000000007</v>
       </c>
       <c r="U416">
-        <f t="shared" ref="U416" si="465">((SUM(C424:F424))/4)*1.04</f>
+        <f t="shared" ref="U416" si="463">((SUM(C424:F424))/4)*1.04</f>
         <v>11.96</v>
       </c>
       <c r="V416">
-        <f t="shared" ref="V416" si="466">((SUM(C416:F424))/20)*1.04</f>
+        <f t="shared" ref="V416" si="464">((SUM(C416:F424))/20)*1.04</f>
         <v>16.224</v>
       </c>
       <c r="W416">
-        <f t="shared" ref="W416" si="467">(SUM(G416:H424))/10</f>
+        <f t="shared" ref="W416" si="465">(SUM(G416:H424))/10</f>
         <v>19.5</v>
       </c>
       <c r="X416">
-        <f t="shared" ref="X416" si="468">(SUM(I416:I424))/5</f>
+        <f t="shared" ref="X416" si="466">(SUM(I416:I424))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y416">
-        <f t="shared" ref="Y416" si="469">SUM(K416:K424)-Z416</f>
+        <f t="shared" ref="Y416" si="467">SUM(K416:K424)-Z416</f>
         <v>36</v>
       </c>
       <c r="Z416">
-        <f t="shared" ref="Z416" si="470">SUM(L416:L424)</f>
+        <f t="shared" ref="Z416" si="468">SUM(L416:L424)</f>
         <v>3</v>
       </c>
       <c r="AA416" t="s">
@@ -64699,47 +64698,47 @@
         <v>560</v>
       </c>
       <c r="P425" t="e">
-        <f t="shared" ref="P425" si="471">M425*10</f>
+        <f t="shared" ref="P425" si="469">M425*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q425">
-        <f t="shared" ref="Q425" si="472">((SUM(C425:F425))/4)*1.04</f>
+        <f t="shared" ref="Q425" si="470">((SUM(C425:F425))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R425">
-        <f t="shared" ref="R425" si="473">((SUM(C427:F427))/4)*1.04</f>
+        <f t="shared" ref="R425" si="471">((SUM(C427:F427))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S425">
-        <f t="shared" ref="S425" si="474">((SUM(C429:F429))/4)*1.04</f>
+        <f t="shared" ref="S425" si="472">((SUM(C429:F429))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T425">
-        <f t="shared" ref="T425" si="475">((SUM(C431:F431))/4)*1.04</f>
+        <f t="shared" ref="T425" si="473">((SUM(C431:F431))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U425">
-        <f t="shared" ref="U425" si="476">((SUM(C433:F433))/4)*1.04</f>
+        <f t="shared" ref="U425" si="474">((SUM(C433:F433))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V425">
-        <f t="shared" ref="V425" si="477">((SUM(C425:F433))/20)*1.04</f>
+        <f t="shared" ref="V425" si="475">((SUM(C425:F433))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W425">
-        <f t="shared" ref="W425" si="478">(SUM(G425:H433))/10</f>
+        <f t="shared" ref="W425" si="476">(SUM(G425:H433))/10</f>
         <v>26.2</v>
       </c>
       <c r="X425">
-        <f t="shared" ref="X425" si="479">(SUM(I425:I433))/5</f>
+        <f t="shared" ref="X425" si="477">(SUM(I425:I433))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y425">
-        <f t="shared" ref="Y425" si="480">SUM(K425:K433)-Z425</f>
+        <f t="shared" ref="Y425" si="478">SUM(K425:K433)-Z425</f>
         <v>32</v>
       </c>
       <c r="Z425">
-        <f t="shared" ref="Z425" si="481">SUM(L425:L433)</f>
+        <f t="shared" ref="Z425" si="479">SUM(L425:L433)</f>
         <v>1</v>
       </c>
       <c r="AA425" t="s">
@@ -65193,47 +65192,47 @@
         <v>240</v>
       </c>
       <c r="P434">
-        <f t="shared" ref="P434" si="482">M434*10</f>
+        <f t="shared" ref="P434" si="480">M434*10</f>
         <v>20</v>
       </c>
       <c r="Q434">
-        <f t="shared" ref="Q434" si="483">((SUM(C434:F434))/4)*1.04</f>
+        <f t="shared" ref="Q434" si="481">((SUM(C434:F434))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R434">
-        <f t="shared" ref="R434" si="484">((SUM(C436:F436))/4)*1.04</f>
+        <f t="shared" ref="R434" si="482">((SUM(C436:F436))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S434">
-        <f t="shared" ref="S434" si="485">((SUM(C438:F438))/4)*1.04</f>
+        <f t="shared" ref="S434" si="483">((SUM(C438:F438))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T434">
-        <f t="shared" ref="T434" si="486">((SUM(C440:F440))/4)*1.04</f>
+        <f t="shared" ref="T434" si="484">((SUM(C440:F440))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U434">
-        <f t="shared" ref="U434" si="487">((SUM(C442:F442))/4)*1.04</f>
+        <f t="shared" ref="U434" si="485">((SUM(C442:F442))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V434">
-        <f t="shared" ref="V434" si="488">((SUM(C434:F442))/20)*1.04</f>
+        <f t="shared" ref="V434" si="486">((SUM(C434:F442))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W434">
-        <f t="shared" ref="W434" si="489">(SUM(G434:H442))/10</f>
+        <f t="shared" ref="W434" si="487">(SUM(G434:H442))/10</f>
         <v>10.5</v>
       </c>
       <c r="X434">
-        <f t="shared" ref="X434" si="490">(SUM(I434:I442))/5</f>
+        <f t="shared" ref="X434" si="488">(SUM(I434:I442))/5</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="Y434">
-        <f t="shared" ref="Y434" si="491">SUM(K434:K442)-Z434</f>
+        <f t="shared" ref="Y434" si="489">SUM(K434:K442)-Z434</f>
         <v>15</v>
       </c>
       <c r="Z434">
-        <f t="shared" ref="Z434" si="492">SUM(L434:L442)</f>
+        <f t="shared" ref="Z434" si="490">SUM(L434:L442)</f>
         <v>3</v>
       </c>
       <c r="AA434" t="s">
@@ -65687,47 +65686,47 @@
         <v>240</v>
       </c>
       <c r="P443">
-        <f t="shared" ref="P443" si="493">M443*10</f>
+        <f t="shared" ref="P443" si="491">M443*10</f>
         <v>40</v>
       </c>
       <c r="Q443">
-        <f t="shared" ref="Q443" si="494">((SUM(C443:F443))/4)*1.04</f>
+        <f t="shared" ref="Q443" si="492">((SUM(C443:F443))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R443">
-        <f t="shared" ref="R443" si="495">((SUM(C445:F445))/4)*1.04</f>
+        <f t="shared" ref="R443" si="493">((SUM(C445:F445))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S443">
-        <f t="shared" ref="S443" si="496">((SUM(C447:F447))/4)*1.04</f>
+        <f t="shared" ref="S443" si="494">((SUM(C447:F447))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T443">
-        <f t="shared" ref="T443" si="497">((SUM(C449:F449))/4)*1.04</f>
+        <f t="shared" ref="T443" si="495">((SUM(C449:F449))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U443">
-        <f t="shared" ref="U443" si="498">((SUM(C451:F451))/4)*1.04</f>
+        <f t="shared" ref="U443" si="496">((SUM(C451:F451))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V443">
-        <f t="shared" ref="V443" si="499">((SUM(C443:F451))/20)*1.04</f>
+        <f t="shared" ref="V443" si="497">((SUM(C443:F451))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W443">
-        <f t="shared" ref="W443" si="500">(SUM(G443:H451))/10</f>
+        <f t="shared" ref="W443" si="498">(SUM(G443:H451))/10</f>
         <v>37.5</v>
       </c>
       <c r="X443">
-        <f t="shared" ref="X443" si="501">(SUM(I443:I451))/5</f>
+        <f t="shared" ref="X443" si="499">(SUM(I443:I451))/5</f>
         <v>1.6</v>
       </c>
       <c r="Y443">
-        <f t="shared" ref="Y443" si="502">SUM(K443:K451)-Z443</f>
+        <f t="shared" ref="Y443" si="500">SUM(K443:K451)-Z443</f>
         <v>19</v>
       </c>
       <c r="Z443">
-        <f t="shared" ref="Z443" si="503">SUM(L443:L451)</f>
+        <f t="shared" ref="Z443" si="501">SUM(L443:L451)</f>
         <v>1</v>
       </c>
       <c r="AA443" t="s">
@@ -66181,47 +66180,47 @@
         <v>240</v>
       </c>
       <c r="P452">
-        <f t="shared" ref="P452" si="504">M452*10</f>
+        <f t="shared" ref="P452" si="502">M452*10</f>
         <v>40</v>
       </c>
       <c r="Q452">
-        <f t="shared" ref="Q452" si="505">((SUM(C452:F452))/4)*1.04</f>
+        <f t="shared" ref="Q452" si="503">((SUM(C452:F452))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R452">
-        <f t="shared" ref="R452" si="506">((SUM(C454:F454))/4)*1.04</f>
+        <f t="shared" ref="R452" si="504">((SUM(C454:F454))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S452">
-        <f t="shared" ref="S452" si="507">((SUM(C456:F456))/4)*1.04</f>
+        <f t="shared" ref="S452" si="505">((SUM(C456:F456))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T452">
-        <f t="shared" ref="T452" si="508">((SUM(C458:F458))/4)*1.04</f>
+        <f t="shared" ref="T452" si="506">((SUM(C458:F458))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U452">
-        <f t="shared" ref="U452" si="509">((SUM(C460:F460))/4)*1.04</f>
+        <f t="shared" ref="U452" si="507">((SUM(C460:F460))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V452">
-        <f t="shared" ref="V452" si="510">((SUM(C452:F460))/20)*1.04</f>
+        <f t="shared" ref="V452" si="508">((SUM(C452:F460))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W452">
-        <f t="shared" ref="W452" si="511">(SUM(G452:H460))/10</f>
+        <f t="shared" ref="W452" si="509">(SUM(G452:H460))/10</f>
         <v>14</v>
       </c>
       <c r="X452">
-        <f t="shared" ref="X452" si="512">(SUM(I452:I460))/5</f>
+        <f t="shared" ref="X452" si="510">(SUM(I452:I460))/5</f>
         <v>3.2</v>
       </c>
       <c r="Y452">
-        <f t="shared" ref="Y452" si="513">SUM(K452:K460)-Z452</f>
+        <f t="shared" ref="Y452" si="511">SUM(K452:K460)-Z452</f>
         <v>16</v>
       </c>
       <c r="Z452">
-        <f t="shared" ref="Z452" si="514">SUM(L452:L460)</f>
+        <f t="shared" ref="Z452" si="512">SUM(L452:L460)</f>
         <v>4</v>
       </c>
       <c r="AA452" t="s">
@@ -66675,47 +66674,47 @@
         <v>240</v>
       </c>
       <c r="P461" t="e">
-        <f t="shared" ref="P461" si="515">M461*10</f>
+        <f t="shared" ref="P461" si="513">M461*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q461">
-        <f t="shared" ref="Q461" si="516">((SUM(C461:F461))/4)*1.04</f>
+        <f t="shared" ref="Q461" si="514">((SUM(C461:F461))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R461">
-        <f t="shared" ref="R461" si="517">((SUM(C463:F463))/4)*1.04</f>
+        <f t="shared" ref="R461" si="515">((SUM(C463:F463))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S461">
-        <f t="shared" ref="S461" si="518">((SUM(C465:F465))/4)*1.04</f>
+        <f t="shared" ref="S461" si="516">((SUM(C465:F465))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T461">
-        <f t="shared" ref="T461" si="519">((SUM(C467:F467))/4)*1.04</f>
+        <f t="shared" ref="T461" si="517">((SUM(C467:F467))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U461">
-        <f t="shared" ref="U461" si="520">((SUM(C469:F469))/4)*1.04</f>
+        <f t="shared" ref="U461" si="518">((SUM(C469:F469))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V461">
-        <f t="shared" ref="V461" si="521">((SUM(C461:F469))/20)*1.04</f>
+        <f t="shared" ref="V461" si="519">((SUM(C461:F469))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W461">
-        <f t="shared" ref="W461" si="522">(SUM(G461:H469))/10</f>
+        <f t="shared" ref="W461" si="520">(SUM(G461:H469))/10</f>
         <v>19</v>
       </c>
       <c r="X461">
-        <f t="shared" ref="X461" si="523">(SUM(I461:I469))/5</f>
+        <f t="shared" ref="X461" si="521">(SUM(I461:I469))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y461">
-        <f t="shared" ref="Y461" si="524">SUM(K461:K469)-Z461</f>
+        <f t="shared" ref="Y461" si="522">SUM(K461:K469)-Z461</f>
         <v>33</v>
       </c>
       <c r="Z461">
-        <f t="shared" ref="Z461" si="525">SUM(L461:L469)</f>
+        <f t="shared" ref="Z461" si="523">SUM(L461:L469)</f>
         <v>3</v>
       </c>
       <c r="AA461" t="s">
@@ -67169,47 +67168,47 @@
         <v>240</v>
       </c>
       <c r="P470" t="e">
-        <f t="shared" ref="P470" si="526">M470*10</f>
+        <f t="shared" ref="P470" si="524">M470*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q470">
-        <f t="shared" ref="Q470" si="527">((SUM(C470:F470))/4)*1.04</f>
+        <f t="shared" ref="Q470" si="525">((SUM(C470:F470))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R470">
-        <f t="shared" ref="R470" si="528">((SUM(C472:F472))/4)*1.04</f>
+        <f t="shared" ref="R470" si="526">((SUM(C472:F472))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S470">
-        <f t="shared" ref="S470" si="529">((SUM(C474:F474))/4)*1.04</f>
+        <f t="shared" ref="S470" si="527">((SUM(C474:F474))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T470">
-        <f t="shared" ref="T470" si="530">((SUM(C476:F476))/4)*1.04</f>
+        <f t="shared" ref="T470" si="528">((SUM(C476:F476))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U470">
-        <f t="shared" ref="U470" si="531">((SUM(C478:F478))/4)*1.04</f>
+        <f t="shared" ref="U470" si="529">((SUM(C478:F478))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V470">
-        <f t="shared" ref="V470" si="532">((SUM(C470:F478))/20)*1.04</f>
+        <f t="shared" ref="V470" si="530">((SUM(C470:F478))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W470">
-        <f t="shared" ref="W470" si="533">(SUM(G470:H478))/10</f>
+        <f t="shared" ref="W470" si="531">(SUM(G470:H478))/10</f>
         <v>31</v>
       </c>
       <c r="X470">
-        <f t="shared" ref="X470" si="534">(SUM(I470:I478))/5</f>
+        <f t="shared" ref="X470" si="532">(SUM(I470:I478))/5</f>
         <v>3.4</v>
       </c>
       <c r="Y470">
-        <f t="shared" ref="Y470" si="535">SUM(K470:K478)-Z470</f>
+        <f t="shared" ref="Y470" si="533">SUM(K470:K478)-Z470</f>
         <v>42</v>
       </c>
       <c r="Z470">
-        <f t="shared" ref="Z470" si="536">SUM(L470:L478)</f>
+        <f t="shared" ref="Z470" si="534">SUM(L470:L478)</f>
         <v>4</v>
       </c>
       <c r="AA470" t="s">
@@ -67663,47 +67662,47 @@
         <v>240</v>
       </c>
       <c r="P479" t="e">
-        <f t="shared" ref="P479" si="537">M479*10</f>
+        <f t="shared" ref="P479" si="535">M479*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q479">
-        <f t="shared" ref="Q479" si="538">((SUM(C479:F479))/4)*1.04</f>
+        <f t="shared" ref="Q479" si="536">((SUM(C479:F479))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R479">
-        <f t="shared" ref="R479" si="539">((SUM(C481:F481))/4)*1.04</f>
+        <f t="shared" ref="R479" si="537">((SUM(C481:F481))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S479">
-        <f t="shared" ref="S479" si="540">((SUM(C483:F483))/4)*1.04</f>
+        <f t="shared" ref="S479" si="538">((SUM(C483:F483))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T479">
-        <f t="shared" ref="T479" si="541">((SUM(C485:F485))/4)*1.04</f>
+        <f t="shared" ref="T479" si="539">((SUM(C485:F485))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U479">
-        <f t="shared" ref="U479" si="542">((SUM(C487:F487))/4)*1.04</f>
+        <f t="shared" ref="U479" si="540">((SUM(C487:F487))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V479">
-        <f t="shared" ref="V479" si="543">((SUM(C479:F487))/20)*1.04</f>
+        <f t="shared" ref="V479" si="541">((SUM(C479:F487))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W479">
-        <f t="shared" ref="W479" si="544">(SUM(G479:H487))/10</f>
+        <f t="shared" ref="W479" si="542">(SUM(G479:H487))/10</f>
         <v>7</v>
       </c>
       <c r="X479">
-        <f t="shared" ref="X479" si="545">(SUM(I479:I487))/5</f>
+        <f t="shared" ref="X479" si="543">(SUM(I479:I487))/5</f>
         <v>2.6</v>
       </c>
       <c r="Y479">
-        <f t="shared" ref="Y479" si="546">SUM(K479:K487)-Z479</f>
+        <f t="shared" ref="Y479" si="544">SUM(K479:K487)-Z479</f>
         <v>26</v>
       </c>
       <c r="Z479">
-        <f t="shared" ref="Z479" si="547">SUM(L479:L487)</f>
+        <f t="shared" ref="Z479" si="545">SUM(L479:L487)</f>
         <v>2</v>
       </c>
       <c r="AA479" t="s">
@@ -68157,47 +68156,47 @@
         <v>29</v>
       </c>
       <c r="P488">
-        <f t="shared" ref="P488" si="548">M488*10</f>
+        <f t="shared" ref="P488" si="546">M488*10</f>
         <v>80</v>
       </c>
       <c r="Q488">
-        <f t="shared" ref="Q488" si="549">((SUM(C488:F488))/4)*1.04</f>
+        <f t="shared" ref="Q488" si="547">((SUM(C488:F488))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R488">
-        <f t="shared" ref="R488" si="550">((SUM(C490:F490))/4)*1.04</f>
+        <f t="shared" ref="R488" si="548">((SUM(C490:F490))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S488">
-        <f t="shared" ref="S488" si="551">((SUM(C492:F492))/4)*1.04</f>
+        <f t="shared" ref="S488" si="549">((SUM(C492:F492))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T488">
-        <f t="shared" ref="T488" si="552">((SUM(C494:F494))/4)*1.04</f>
+        <f t="shared" ref="T488" si="550">((SUM(C494:F494))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U488">
-        <f t="shared" ref="U488" si="553">((SUM(C496:F496))/4)*1.04</f>
+        <f t="shared" ref="U488" si="551">((SUM(C496:F496))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V488">
-        <f t="shared" ref="V488" si="554">((SUM(C488:F496))/20)*1.04</f>
+        <f t="shared" ref="V488" si="552">((SUM(C488:F496))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W488">
-        <f t="shared" ref="W488" si="555">(SUM(G488:H496))/10</f>
+        <f t="shared" ref="W488" si="553">(SUM(G488:H496))/10</f>
         <v>43.5</v>
       </c>
       <c r="X488">
-        <f t="shared" ref="X488" si="556">(SUM(I488:I496))/5</f>
+        <f t="shared" ref="X488" si="554">(SUM(I488:I496))/5</f>
         <v>2</v>
       </c>
       <c r="Y488">
-        <f t="shared" ref="Y488" si="557">SUM(K488:K496)-Z488</f>
+        <f t="shared" ref="Y488" si="555">SUM(K488:K496)-Z488</f>
         <v>10</v>
       </c>
       <c r="Z488">
-        <f t="shared" ref="Z488" si="558">SUM(L488:L496)</f>
+        <f t="shared" ref="Z488" si="556">SUM(L488:L496)</f>
         <v>8</v>
       </c>
       <c r="AA488" t="s">
@@ -68651,47 +68650,47 @@
         <v>43</v>
       </c>
       <c r="P497">
-        <f t="shared" ref="P497" si="559">M497*10</f>
+        <f t="shared" ref="P497" si="557">M497*10</f>
         <v>50</v>
       </c>
       <c r="Q497">
-        <f t="shared" ref="Q497" si="560">((SUM(C497:F497))/4)*1.04</f>
+        <f t="shared" ref="Q497" si="558">((SUM(C497:F497))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R497">
-        <f t="shared" ref="R497" si="561">((SUM(C499:F499))/4)*1.04</f>
+        <f t="shared" ref="R497" si="559">((SUM(C499:F499))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S497">
-        <f t="shared" ref="S497" si="562">((SUM(C501:F501))/4)*1.04</f>
+        <f t="shared" ref="S497" si="560">((SUM(C501:F501))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T497">
-        <f t="shared" ref="T497" si="563">((SUM(C503:F503))/4)*1.04</f>
+        <f t="shared" ref="T497" si="561">((SUM(C503:F503))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U497">
-        <f t="shared" ref="U497" si="564">((SUM(C505:F505))/4)*1.04</f>
+        <f t="shared" ref="U497" si="562">((SUM(C505:F505))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V497">
-        <f t="shared" ref="V497" si="565">((SUM(C497:F505))/20)*1.04</f>
+        <f t="shared" ref="V497" si="563">((SUM(C497:F505))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W497">
-        <f t="shared" ref="W497" si="566">(SUM(G497:H505))/10</f>
+        <f t="shared" ref="W497" si="564">(SUM(G497:H505))/10</f>
         <v>81</v>
       </c>
       <c r="X497">
-        <f t="shared" ref="X497" si="567">(SUM(I497:I505))/5</f>
+        <f t="shared" ref="X497" si="565">(SUM(I497:I505))/5</f>
         <v>1.6</v>
       </c>
       <c r="Y497">
-        <f t="shared" ref="Y497" si="568">SUM(K497:K505)-Z497</f>
+        <f t="shared" ref="Y497" si="566">SUM(K497:K505)-Z497</f>
         <v>30</v>
       </c>
       <c r="Z497">
-        <f t="shared" ref="Z497" si="569">SUM(L497:L505)</f>
+        <f t="shared" ref="Z497" si="567">SUM(L497:L505)</f>
         <v>0</v>
       </c>
       <c r="AA497" t="s">
@@ -69145,47 +69144,47 @@
         <v>782</v>
       </c>
       <c r="P506">
-        <f t="shared" ref="P506" si="570">M506*10</f>
+        <f t="shared" ref="P506" si="568">M506*10</f>
         <v>100</v>
       </c>
       <c r="Q506">
-        <f t="shared" ref="Q506" si="571">((SUM(C506:F506))/4)*1.04</f>
+        <f t="shared" ref="Q506" si="569">((SUM(C506:F506))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R506">
-        <f t="shared" ref="R506" si="572">((SUM(C508:F508))/4)*1.04</f>
+        <f t="shared" ref="R506" si="570">((SUM(C508:F508))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S506">
-        <f t="shared" ref="S506" si="573">((SUM(C510:F510))/4)*1.04</f>
+        <f t="shared" ref="S506" si="571">((SUM(C510:F510))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T506">
-        <f t="shared" ref="T506" si="574">((SUM(C512:F512))/4)*1.04</f>
+        <f t="shared" ref="T506" si="572">((SUM(C512:F512))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U506">
-        <f t="shared" ref="U506" si="575">((SUM(C514:F514))/4)*1.04</f>
+        <f t="shared" ref="U506" si="573">((SUM(C514:F514))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V506">
-        <f t="shared" ref="V506" si="576">((SUM(C506:F514))/20)*1.04</f>
+        <f t="shared" ref="V506" si="574">((SUM(C506:F514))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W506">
-        <f t="shared" ref="W506" si="577">(SUM(G506:H514))/10</f>
+        <f t="shared" ref="W506" si="575">(SUM(G506:H514))/10</f>
         <v>16.2</v>
       </c>
       <c r="X506">
-        <f t="shared" ref="X506" si="578">(SUM(I506:I514))/5</f>
+        <f t="shared" ref="X506" si="576">(SUM(I506:I514))/5</f>
         <v>2</v>
       </c>
       <c r="Y506">
-        <f t="shared" ref="Y506" si="579">SUM(K506:K514)-Z506</f>
+        <f t="shared" ref="Y506" si="577">SUM(K506:K514)-Z506</f>
         <v>69</v>
       </c>
       <c r="Z506">
-        <f t="shared" ref="Z506" si="580">SUM(L506:L514)</f>
+        <f t="shared" ref="Z506" si="578">SUM(L506:L514)</f>
         <v>10</v>
       </c>
       <c r="AA506" t="s">
@@ -69639,47 +69638,47 @@
         <v>240</v>
       </c>
       <c r="P515">
-        <f t="shared" ref="P515" si="581">M515*10</f>
+        <f t="shared" ref="P515" si="579">M515*10</f>
         <v>30</v>
       </c>
       <c r="Q515">
-        <f t="shared" ref="Q515" si="582">((SUM(C515:F515))/4)*1.04</f>
+        <f t="shared" ref="Q515" si="580">((SUM(C515:F515))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R515">
-        <f t="shared" ref="R515" si="583">((SUM(C517:F517))/4)*1.04</f>
+        <f t="shared" ref="R515" si="581">((SUM(C517:F517))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S515">
-        <f t="shared" ref="S515" si="584">((SUM(C519:F519))/4)*1.04</f>
+        <f t="shared" ref="S515" si="582">((SUM(C519:F519))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T515">
-        <f t="shared" ref="T515" si="585">((SUM(C521:F521))/4)*1.04</f>
+        <f t="shared" ref="T515" si="583">((SUM(C521:F521))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U515">
-        <f t="shared" ref="U515" si="586">((SUM(C523:F523))/4)*1.04</f>
+        <f t="shared" ref="U515" si="584">((SUM(C523:F523))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V515">
-        <f t="shared" ref="V515" si="587">((SUM(C515:F523))/20)*1.04</f>
+        <f t="shared" ref="V515" si="585">((SUM(C515:F523))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W515">
-        <f t="shared" ref="W515" si="588">(SUM(G515:H523))/10</f>
+        <f t="shared" ref="W515" si="586">(SUM(G515:H523))/10</f>
         <v>5.5</v>
       </c>
       <c r="X515">
-        <f t="shared" ref="X515" si="589">(SUM(I515:I523))/5</f>
+        <f t="shared" ref="X515" si="587">(SUM(I515:I523))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y515">
-        <f t="shared" ref="Y515" si="590">SUM(K515:K523)-Z515</f>
+        <f t="shared" ref="Y515" si="588">SUM(K515:K523)-Z515</f>
         <v>23</v>
       </c>
       <c r="Z515">
-        <f t="shared" ref="Z515" si="591">SUM(L515:L523)</f>
+        <f t="shared" ref="Z515" si="589">SUM(L515:L523)</f>
         <v>3</v>
       </c>
       <c r="AA515" t="s">
@@ -70133,47 +70132,47 @@
         <v>240</v>
       </c>
       <c r="P524">
-        <f t="shared" ref="P524" si="592">M524*10</f>
+        <f t="shared" ref="P524" si="590">M524*10</f>
         <v>60</v>
       </c>
       <c r="Q524">
-        <f t="shared" ref="Q524" si="593">((SUM(C524:F524))/4)*1.04</f>
+        <f t="shared" ref="Q524" si="591">((SUM(C524:F524))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R524">
-        <f t="shared" ref="R524" si="594">((SUM(C526:F526))/4)*1.04</f>
+        <f t="shared" ref="R524" si="592">((SUM(C526:F526))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S524">
-        <f t="shared" ref="S524" si="595">((SUM(C528:F528))/4)*1.04</f>
+        <f t="shared" ref="S524" si="593">((SUM(C528:F528))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T524">
-        <f t="shared" ref="T524" si="596">((SUM(C530:F530))/4)*1.04</f>
+        <f t="shared" ref="T524" si="594">((SUM(C530:F530))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U524">
-        <f t="shared" ref="U524" si="597">((SUM(C532:F532))/4)*1.04</f>
+        <f t="shared" ref="U524" si="595">((SUM(C532:F532))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V524">
-        <f t="shared" ref="V524" si="598">((SUM(C524:F532))/20)*1.04</f>
+        <f t="shared" ref="V524" si="596">((SUM(C524:F532))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W524">
-        <f t="shared" ref="W524" si="599">(SUM(G524:H532))/10</f>
+        <f t="shared" ref="W524" si="597">(SUM(G524:H532))/10</f>
         <v>11</v>
       </c>
       <c r="X524">
-        <f t="shared" ref="X524" si="600">(SUM(I524:I532))/5</f>
+        <f t="shared" ref="X524" si="598">(SUM(I524:I532))/5</f>
         <v>2.4</v>
       </c>
       <c r="Y524">
-        <f t="shared" ref="Y524" si="601">SUM(K524:K532)-Z524</f>
+        <f t="shared" ref="Y524" si="599">SUM(K524:K532)-Z524</f>
         <v>23</v>
       </c>
       <c r="Z524">
-        <f t="shared" ref="Z524" si="602">SUM(L524:L532)</f>
+        <f t="shared" ref="Z524" si="600">SUM(L524:L532)</f>
         <v>3</v>
       </c>
       <c r="AA524" t="s">
@@ -70627,47 +70626,47 @@
         <v>240</v>
       </c>
       <c r="P533">
-        <f t="shared" ref="P533" si="603">M533*10</f>
+        <f t="shared" ref="P533" si="601">M533*10</f>
         <v>70</v>
       </c>
       <c r="Q533">
-        <f t="shared" ref="Q533" si="604">((SUM(C533:F533))/4)*1.04</f>
+        <f t="shared" ref="Q533" si="602">((SUM(C533:F533))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R533">
-        <f t="shared" ref="R533" si="605">((SUM(C535:F535))/4)*1.04</f>
+        <f t="shared" ref="R533" si="603">((SUM(C535:F535))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S533">
-        <f t="shared" ref="S533" si="606">((SUM(C537:F537))/4)*1.04</f>
+        <f t="shared" ref="S533" si="604">((SUM(C537:F537))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T533">
-        <f t="shared" ref="T533" si="607">((SUM(C539:F539))/4)*1.04</f>
+        <f t="shared" ref="T533" si="605">((SUM(C539:F539))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U533">
-        <f t="shared" ref="U533" si="608">((SUM(C541:F541))/4)*1.04</f>
+        <f t="shared" ref="U533" si="606">((SUM(C541:F541))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V533">
-        <f t="shared" ref="V533" si="609">((SUM(C533:F541))/20)*1.04</f>
+        <f t="shared" ref="V533" si="607">((SUM(C533:F541))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W533">
-        <f t="shared" ref="W533" si="610">(SUM(G533:H541))/10</f>
+        <f t="shared" ref="W533" si="608">(SUM(G533:H541))/10</f>
         <v>4.5</v>
       </c>
       <c r="X533">
-        <f t="shared" ref="X533" si="611">(SUM(I533:I541))/5</f>
+        <f t="shared" ref="X533" si="609">(SUM(I533:I541))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y533">
-        <f t="shared" ref="Y533" si="612">SUM(K533:K541)-Z533</f>
+        <f t="shared" ref="Y533" si="610">SUM(K533:K541)-Z533</f>
         <v>19</v>
       </c>
       <c r="Z533">
-        <f t="shared" ref="Z533" si="613">SUM(L533:L541)</f>
+        <f t="shared" ref="Z533" si="611">SUM(L533:L541)</f>
         <v>4</v>
       </c>
       <c r="AA533" t="s">
@@ -71121,47 +71120,47 @@
         <v>240</v>
       </c>
       <c r="P542">
-        <f t="shared" ref="P542" si="614">M542*10</f>
+        <f t="shared" ref="P542" si="612">M542*10</f>
         <v>50</v>
       </c>
       <c r="Q542">
-        <f t="shared" ref="Q542" si="615">((SUM(C542:F542))/4)*1.04</f>
+        <f t="shared" ref="Q542" si="613">((SUM(C542:F542))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R542">
-        <f t="shared" ref="R542" si="616">((SUM(C544:F544))/4)*1.04</f>
+        <f t="shared" ref="R542" si="614">((SUM(C544:F544))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S542">
-        <f t="shared" ref="S542" si="617">((SUM(C546:F546))/4)*1.04</f>
+        <f t="shared" ref="S542" si="615">((SUM(C546:F546))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T542">
-        <f t="shared" ref="T542" si="618">((SUM(C548:F548))/4)*1.04</f>
+        <f t="shared" ref="T542" si="616">((SUM(C548:F548))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U542">
-        <f t="shared" ref="U542" si="619">((SUM(C550:F550))/4)*1.04</f>
+        <f t="shared" ref="U542" si="617">((SUM(C550:F550))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V542">
-        <f t="shared" ref="V542" si="620">((SUM(C542:F550))/20)*1.04</f>
+        <f t="shared" ref="V542" si="618">((SUM(C542:F550))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W542">
-        <f t="shared" ref="W542" si="621">(SUM(G542:H550))/10</f>
+        <f t="shared" ref="W542" si="619">(SUM(G542:H550))/10</f>
         <v>35.5</v>
       </c>
       <c r="X542">
-        <f t="shared" ref="X542" si="622">(SUM(I542:I550))/5</f>
+        <f t="shared" ref="X542" si="620">(SUM(I542:I550))/5</f>
         <v>1.8</v>
       </c>
       <c r="Y542">
-        <f t="shared" ref="Y542" si="623">SUM(K542:K550)-Z542</f>
+        <f t="shared" ref="Y542" si="621">SUM(K542:K550)-Z542</f>
         <v>10</v>
       </c>
       <c r="Z542">
-        <f t="shared" ref="Z542" si="624">SUM(L542:L550)</f>
+        <f t="shared" ref="Z542" si="622">SUM(L542:L550)</f>
         <v>0</v>
       </c>
       <c r="AA542" t="s">
@@ -71615,47 +71614,47 @@
         <v>240</v>
       </c>
       <c r="P551">
-        <f t="shared" ref="P551" si="625">M551*10</f>
+        <f t="shared" ref="P551" si="623">M551*10</f>
         <v>50</v>
       </c>
       <c r="Q551">
-        <f t="shared" ref="Q551" si="626">((SUM(C551:F551))/4)*1.04</f>
+        <f t="shared" ref="Q551" si="624">((SUM(C551:F551))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R551">
-        <f t="shared" ref="R551" si="627">((SUM(C553:F553))/4)*1.04</f>
+        <f t="shared" ref="R551" si="625">((SUM(C553:F553))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S551">
-        <f t="shared" ref="S551" si="628">((SUM(C555:F555))/4)*1.04</f>
+        <f t="shared" ref="S551" si="626">((SUM(C555:F555))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T551">
-        <f t="shared" ref="T551" si="629">((SUM(C557:F557))/4)*1.04</f>
+        <f t="shared" ref="T551" si="627">((SUM(C557:F557))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U551">
-        <f t="shared" ref="U551" si="630">((SUM(C559:F559))/4)*1.04</f>
+        <f t="shared" ref="U551" si="628">((SUM(C559:F559))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V551">
-        <f t="shared" ref="V551" si="631">((SUM(C551:F559))/20)*1.04</f>
+        <f t="shared" ref="V551" si="629">((SUM(C551:F559))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W551">
-        <f t="shared" ref="W551" si="632">(SUM(G551:H559))/10</f>
+        <f t="shared" ref="W551" si="630">(SUM(G551:H559))/10</f>
         <v>49</v>
       </c>
       <c r="X551">
-        <f t="shared" ref="X551" si="633">(SUM(I551:I559))/5</f>
+        <f t="shared" ref="X551" si="631">(SUM(I551:I559))/5</f>
         <v>2.6</v>
       </c>
       <c r="Y551">
-        <f t="shared" ref="Y551" si="634">SUM(K551:K559)-Z551</f>
+        <f t="shared" ref="Y551" si="632">SUM(K551:K559)-Z551</f>
         <v>17</v>
       </c>
       <c r="Z551">
-        <f t="shared" ref="Z551" si="635">SUM(L551:L559)</f>
+        <f t="shared" ref="Z551" si="633">SUM(L551:L559)</f>
         <v>0</v>
       </c>
       <c r="AA551" t="s">
@@ -72109,47 +72108,47 @@
         <v>29</v>
       </c>
       <c r="P560">
-        <f t="shared" ref="P560" si="636">M560*10</f>
+        <f t="shared" ref="P560" si="634">M560*10</f>
         <v>70</v>
       </c>
       <c r="Q560">
-        <f t="shared" ref="Q560" si="637">((SUM(C560:F560))/4)*1.04</f>
+        <f t="shared" ref="Q560" si="635">((SUM(C560:F560))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R560">
-        <f t="shared" ref="R560" si="638">((SUM(C562:F562))/4)*1.04</f>
+        <f t="shared" ref="R560" si="636">((SUM(C562:F562))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S560">
-        <f t="shared" ref="S560" si="639">((SUM(C564:F564))/4)*1.04</f>
+        <f t="shared" ref="S560" si="637">((SUM(C564:F564))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T560">
-        <f t="shared" ref="T560" si="640">((SUM(C566:F566))/4)*1.04</f>
+        <f t="shared" ref="T560" si="638">((SUM(C566:F566))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U560">
-        <f t="shared" ref="U560" si="641">((SUM(C568:F568))/4)*1.04</f>
+        <f t="shared" ref="U560" si="639">((SUM(C568:F568))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V560">
-        <f t="shared" ref="V560" si="642">((SUM(C560:F568))/20)*1.04</f>
+        <f t="shared" ref="V560" si="640">((SUM(C560:F568))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W560">
-        <f t="shared" ref="W560" si="643">(SUM(G560:H568))/10</f>
+        <f t="shared" ref="W560" si="641">(SUM(G560:H568))/10</f>
         <v>11.8</v>
       </c>
       <c r="X560">
-        <f t="shared" ref="X560" si="644">(SUM(I560:I568))/5</f>
+        <f t="shared" ref="X560" si="642">(SUM(I560:I568))/5</f>
         <v>2</v>
       </c>
       <c r="Y560">
-        <f t="shared" ref="Y560" si="645">SUM(K560:K568)-Z560</f>
+        <f t="shared" ref="Y560" si="643">SUM(K560:K568)-Z560</f>
         <v>10</v>
       </c>
       <c r="Z560">
-        <f t="shared" ref="Z560" si="646">SUM(L560:L568)</f>
+        <f t="shared" ref="Z560" si="644">SUM(L560:L568)</f>
         <v>7</v>
       </c>
       <c r="AA560" t="s">
@@ -72603,47 +72602,47 @@
         <v>29</v>
       </c>
       <c r="P569" t="e">
-        <f t="shared" ref="P569" si="647">M569*10</f>
+        <f t="shared" ref="P569" si="645">M569*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q569">
-        <f t="shared" ref="Q569" si="648">((SUM(C569:F569))/4)*1.04</f>
+        <f t="shared" ref="Q569" si="646">((SUM(C569:F569))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R569">
-        <f t="shared" ref="R569" si="649">((SUM(C571:F571))/4)*1.04</f>
+        <f t="shared" ref="R569" si="647">((SUM(C571:F571))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S569">
-        <f t="shared" ref="S569" si="650">((SUM(C573:F573))/4)*1.04</f>
+        <f t="shared" ref="S569" si="648">((SUM(C573:F573))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T569">
-        <f t="shared" ref="T569" si="651">((SUM(C575:F575))/4)*1.04</f>
+        <f t="shared" ref="T569" si="649">((SUM(C575:F575))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U569">
-        <f t="shared" ref="U569" si="652">((SUM(C577:F577))/4)*1.04</f>
+        <f t="shared" ref="U569" si="650">((SUM(C577:F577))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V569">
-        <f t="shared" ref="V569" si="653">((SUM(C569:F577))/20)*1.04</f>
+        <f t="shared" ref="V569" si="651">((SUM(C569:F577))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W569">
-        <f t="shared" ref="W569" si="654">(SUM(G569:H577))/10</f>
+        <f t="shared" ref="W569" si="652">(SUM(G569:H577))/10</f>
         <v>3</v>
       </c>
       <c r="X569">
-        <f t="shared" ref="X569" si="655">(SUM(I569:I577))/5</f>
+        <f t="shared" ref="X569" si="653">(SUM(I569:I577))/5</f>
         <v>2.4</v>
       </c>
       <c r="Y569">
-        <f t="shared" ref="Y569" si="656">SUM(K569:K577)-Z569</f>
+        <f t="shared" ref="Y569" si="654">SUM(K569:K577)-Z569</f>
         <v>7</v>
       </c>
       <c r="Z569">
-        <f t="shared" ref="Z569" si="657">SUM(L569:L577)</f>
+        <f t="shared" ref="Z569" si="655">SUM(L569:L577)</f>
         <v>7</v>
       </c>
       <c r="AA569" t="s">
@@ -73097,47 +73096,47 @@
         <v>29</v>
       </c>
       <c r="P578">
-        <f t="shared" ref="P578" si="658">M578*10</f>
+        <f t="shared" ref="P578" si="656">M578*10</f>
         <v>120</v>
       </c>
       <c r="Q578">
-        <f t="shared" ref="Q578" si="659">((SUM(C578:F578))/4)*1.04</f>
+        <f t="shared" ref="Q578" si="657">((SUM(C578:F578))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R578">
-        <f t="shared" ref="R578" si="660">((SUM(C580:F580))/4)*1.04</f>
+        <f t="shared" ref="R578" si="658">((SUM(C580:F580))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S578">
-        <f t="shared" ref="S578" si="661">((SUM(C582:F582))/4)*1.04</f>
+        <f t="shared" ref="S578" si="659">((SUM(C582:F582))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T578">
-        <f t="shared" ref="T578" si="662">((SUM(C584:F584))/4)*1.04</f>
+        <f t="shared" ref="T578" si="660">((SUM(C584:F584))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U578">
-        <f t="shared" ref="U578" si="663">((SUM(C586:F586))/4)*1.04</f>
+        <f t="shared" ref="U578" si="661">((SUM(C586:F586))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V578">
-        <f t="shared" ref="V578" si="664">((SUM(C578:F586))/20)*1.04</f>
+        <f t="shared" ref="V578" si="662">((SUM(C578:F586))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W578">
-        <f t="shared" ref="W578" si="665">(SUM(G578:H586))/10</f>
+        <f t="shared" ref="W578" si="663">(SUM(G578:H586))/10</f>
         <v>0.3</v>
       </c>
       <c r="X578">
-        <f t="shared" ref="X578" si="666">(SUM(I578:I586))/5</f>
+        <f t="shared" ref="X578" si="664">(SUM(I578:I586))/5</f>
         <v>1.4</v>
       </c>
       <c r="Y578">
-        <f t="shared" ref="Y578" si="667">SUM(K578:K586)-Z578</f>
+        <f t="shared" ref="Y578" si="665">SUM(K578:K586)-Z578</f>
         <v>77</v>
       </c>
       <c r="Z578">
-        <f t="shared" ref="Z578" si="668">SUM(L578:L586)</f>
+        <f t="shared" ref="Z578" si="666">SUM(L578:L586)</f>
         <v>10</v>
       </c>
       <c r="AA578" t="s">
@@ -73591,47 +73590,47 @@
         <v>29</v>
       </c>
       <c r="P587">
-        <f t="shared" ref="P587" si="669">M587*10</f>
+        <f t="shared" ref="P587" si="667">M587*10</f>
         <v>160</v>
       </c>
       <c r="Q587">
-        <f t="shared" ref="Q587" si="670">((SUM(C587:F587))/4)*1.04</f>
+        <f t="shared" ref="Q587" si="668">((SUM(C587:F587))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R587">
-        <f t="shared" ref="R587" si="671">((SUM(C589:F589))/4)*1.04</f>
+        <f t="shared" ref="R587" si="669">((SUM(C589:F589))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S587">
-        <f t="shared" ref="S587" si="672">((SUM(C591:F591))/4)*1.04</f>
+        <f t="shared" ref="S587" si="670">((SUM(C591:F591))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T587">
-        <f t="shared" ref="T587" si="673">((SUM(C593:F593))/4)*1.04</f>
+        <f t="shared" ref="T587" si="671">((SUM(C593:F593))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U587">
-        <f t="shared" ref="U587" si="674">((SUM(C595:F595))/4)*1.04</f>
+        <f t="shared" ref="U587" si="672">((SUM(C595:F595))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V587">
-        <f t="shared" ref="V587" si="675">((SUM(C587:F595))/20)*1.04</f>
+        <f t="shared" ref="V587" si="673">((SUM(C587:F595))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W587">
-        <f t="shared" ref="W587" si="676">(SUM(G587:H595))/10</f>
+        <f t="shared" ref="W587" si="674">(SUM(G587:H595))/10</f>
         <v>0.5</v>
       </c>
       <c r="X587">
-        <f t="shared" ref="X587" si="677">(SUM(I587:I595))/5</f>
+        <f t="shared" ref="X587" si="675">(SUM(I587:I595))/5</f>
         <v>1.6</v>
       </c>
       <c r="Y587">
-        <f t="shared" ref="Y587" si="678">SUM(K587:K595)-Z587</f>
+        <f t="shared" ref="Y587" si="676">SUM(K587:K595)-Z587</f>
         <v>62</v>
       </c>
       <c r="Z587">
-        <f t="shared" ref="Z587" si="679">SUM(L587:L595)</f>
+        <f t="shared" ref="Z587" si="677">SUM(L587:L595)</f>
         <v>14</v>
       </c>
       <c r="AA587" t="s">
@@ -74085,47 +74084,47 @@
         <v>29</v>
       </c>
       <c r="P596">
-        <f t="shared" ref="P596" si="680">M596*10</f>
+        <f t="shared" ref="P596" si="678">M596*10</f>
         <v>150</v>
       </c>
       <c r="Q596">
-        <f t="shared" ref="Q596" si="681">((SUM(C596:F596))/4)*1.04</f>
+        <f t="shared" ref="Q596" si="679">((SUM(C596:F596))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R596">
-        <f t="shared" ref="R596" si="682">((SUM(C598:F598))/4)*1.04</f>
+        <f t="shared" ref="R596" si="680">((SUM(C598:F598))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S596">
-        <f t="shared" ref="S596" si="683">((SUM(C600:F600))/4)*1.04</f>
+        <f t="shared" ref="S596" si="681">((SUM(C600:F600))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T596">
-        <f t="shared" ref="T596" si="684">((SUM(C602:F602))/4)*1.04</f>
+        <f t="shared" ref="T596" si="682">((SUM(C602:F602))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U596">
-        <f t="shared" ref="U596" si="685">((SUM(C604:F604))/4)*1.04</f>
+        <f t="shared" ref="U596" si="683">((SUM(C604:F604))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V596">
-        <f t="shared" ref="V596" si="686">((SUM(C596:F604))/20)*1.04</f>
+        <f t="shared" ref="V596" si="684">((SUM(C596:F604))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W596">
-        <f t="shared" ref="W596" si="687">(SUM(G596:H604))/10</f>
+        <f t="shared" ref="W596" si="685">(SUM(G596:H604))/10</f>
         <v>9.8000000000000007</v>
       </c>
       <c r="X596">
-        <f t="shared" ref="X596" si="688">(SUM(I596:I604))/5</f>
+        <f t="shared" ref="X596" si="686">(SUM(I596:I604))/5</f>
         <v>2</v>
       </c>
       <c r="Y596">
-        <f t="shared" ref="Y596" si="689">SUM(K596:K604)-Z596</f>
+        <f t="shared" ref="Y596" si="687">SUM(K596:K604)-Z596</f>
         <v>29</v>
       </c>
       <c r="Z596">
-        <f t="shared" ref="Z596" si="690">SUM(L596:L604)</f>
+        <f t="shared" ref="Z596" si="688">SUM(L596:L604)</f>
         <v>8</v>
       </c>
       <c r="AA596" t="s">
@@ -74579,47 +74578,47 @@
         <v>29</v>
       </c>
       <c r="P605">
-        <f t="shared" ref="P605" si="691">M605*10</f>
+        <f t="shared" ref="P605" si="689">M605*10</f>
         <v>190</v>
       </c>
       <c r="Q605">
-        <f t="shared" ref="Q605" si="692">((SUM(C605:F605))/4)*1.04</f>
+        <f t="shared" ref="Q605" si="690">((SUM(C605:F605))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R605">
-        <f t="shared" ref="R605" si="693">((SUM(C607:F607))/4)*1.04</f>
+        <f t="shared" ref="R605" si="691">((SUM(C607:F607))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S605">
-        <f t="shared" ref="S605" si="694">((SUM(C609:F609))/4)*1.04</f>
+        <f t="shared" ref="S605" si="692">((SUM(C609:F609))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T605">
-        <f t="shared" ref="T605" si="695">((SUM(C611:F611))/4)*1.04</f>
+        <f t="shared" ref="T605" si="693">((SUM(C611:F611))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U605">
-        <f t="shared" ref="U605" si="696">((SUM(C613:F613))/4)*1.04</f>
+        <f t="shared" ref="U605" si="694">((SUM(C613:F613))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V605">
-        <f t="shared" ref="V605" si="697">((SUM(C605:F613))/20)*1.04</f>
+        <f t="shared" ref="V605" si="695">((SUM(C605:F613))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W605">
-        <f t="shared" ref="W605" si="698">(SUM(G605:H613))/10</f>
+        <f t="shared" ref="W605" si="696">(SUM(G605:H613))/10</f>
         <v>1.8</v>
       </c>
       <c r="X605">
-        <f t="shared" ref="X605" si="699">(SUM(I605:I613))/5</f>
+        <f t="shared" ref="X605" si="697">(SUM(I605:I613))/5</f>
         <v>3</v>
       </c>
       <c r="Y605">
-        <f t="shared" ref="Y605" si="700">SUM(K605:K613)-Z605</f>
+        <f t="shared" ref="Y605" si="698">SUM(K605:K613)-Z605</f>
         <v>93</v>
       </c>
       <c r="Z605">
-        <f t="shared" ref="Z605" si="701">SUM(L605:L613)</f>
+        <f t="shared" ref="Z605" si="699">SUM(L605:L613)</f>
         <v>2</v>
       </c>
       <c r="AA605" t="s">
@@ -75073,47 +75072,47 @@
         <v>29</v>
       </c>
       <c r="P614" t="e">
-        <f t="shared" ref="P614" si="702">M614*10</f>
+        <f t="shared" ref="P614" si="700">M614*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q614">
-        <f t="shared" ref="Q614" si="703">((SUM(C614:F614))/4)*1.04</f>
+        <f t="shared" ref="Q614" si="701">((SUM(C614:F614))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R614">
-        <f t="shared" ref="R614" si="704">((SUM(C616:F616))/4)*1.04</f>
+        <f t="shared" ref="R614" si="702">((SUM(C616:F616))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S614">
-        <f t="shared" ref="S614" si="705">((SUM(C618:F618))/4)*1.04</f>
+        <f t="shared" ref="S614" si="703">((SUM(C618:F618))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T614">
-        <f t="shared" ref="T614" si="706">((SUM(C620:F620))/4)*1.04</f>
+        <f t="shared" ref="T614" si="704">((SUM(C620:F620))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U614">
-        <f t="shared" ref="U614" si="707">((SUM(C622:F622))/4)*1.04</f>
+        <f t="shared" ref="U614" si="705">((SUM(C622:F622))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V614">
-        <f t="shared" ref="V614" si="708">((SUM(C614:F622))/20)*1.04</f>
+        <f t="shared" ref="V614" si="706">((SUM(C614:F622))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W614">
-        <f t="shared" ref="W614" si="709">(SUM(G614:H622))/10</f>
+        <f t="shared" ref="W614" si="707">(SUM(G614:H622))/10</f>
         <v>19.5</v>
       </c>
       <c r="X614">
-        <f t="shared" ref="X614" si="710">(SUM(I614:I622))/5</f>
+        <f t="shared" ref="X614" si="708">(SUM(I614:I622))/5</f>
         <v>2.8</v>
       </c>
       <c r="Y614">
-        <f t="shared" ref="Y614" si="711">SUM(K614:K622)-Z614</f>
+        <f t="shared" ref="Y614" si="709">SUM(K614:K622)-Z614</f>
         <v>2</v>
       </c>
       <c r="Z614">
-        <f t="shared" ref="Z614" si="712">SUM(L614:L622)</f>
+        <f t="shared" ref="Z614" si="710">SUM(L614:L622)</f>
         <v>9</v>
       </c>
       <c r="AA614" t="s">
@@ -75567,47 +75566,47 @@
         <v>29</v>
       </c>
       <c r="P623">
-        <f t="shared" ref="P623" si="713">M623*10</f>
+        <f t="shared" ref="P623" si="711">M623*10</f>
         <v>50</v>
       </c>
       <c r="Q623">
-        <f t="shared" ref="Q623" si="714">((SUM(C623:F623))/4)*1.04</f>
+        <f t="shared" ref="Q623" si="712">((SUM(C623:F623))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R623">
-        <f t="shared" ref="R623" si="715">((SUM(C625:F625))/4)*1.04</f>
+        <f t="shared" ref="R623" si="713">((SUM(C625:F625))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S623">
-        <f t="shared" ref="S623" si="716">((SUM(C627:F627))/4)*1.04</f>
+        <f t="shared" ref="S623" si="714">((SUM(C627:F627))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T623">
-        <f t="shared" ref="T623" si="717">((SUM(C629:F629))/4)*1.04</f>
+        <f t="shared" ref="T623" si="715">((SUM(C629:F629))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U623">
-        <f t="shared" ref="U623" si="718">((SUM(C631:F631))/4)*1.04</f>
+        <f t="shared" ref="U623" si="716">((SUM(C631:F631))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V623">
-        <f t="shared" ref="V623" si="719">((SUM(C623:F631))/20)*1.04</f>
+        <f t="shared" ref="V623" si="717">((SUM(C623:F631))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W623">
-        <f t="shared" ref="W623" si="720">(SUM(G623:H631))/10</f>
+        <f t="shared" ref="W623" si="718">(SUM(G623:H631))/10</f>
         <v>25.6</v>
       </c>
       <c r="X623">
-        <f t="shared" ref="X623" si="721">(SUM(I623:I631))/5</f>
+        <f t="shared" ref="X623" si="719">(SUM(I623:I631))/5</f>
         <v>1.6</v>
       </c>
       <c r="Y623">
-        <f t="shared" ref="Y623" si="722">SUM(K623:K631)-Z623</f>
+        <f t="shared" ref="Y623" si="720">SUM(K623:K631)-Z623</f>
         <v>12</v>
       </c>
       <c r="Z623">
-        <f t="shared" ref="Z623" si="723">SUM(L623:L631)</f>
+        <f t="shared" ref="Z623" si="721">SUM(L623:L631)</f>
         <v>4</v>
       </c>
       <c r="AA623" t="s">
@@ -76061,47 +76060,47 @@
         <v>29</v>
       </c>
       <c r="P632">
-        <f t="shared" ref="P632" si="724">M632*10</f>
+        <f t="shared" ref="P632" si="722">M632*10</f>
         <v>70</v>
       </c>
       <c r="Q632">
-        <f t="shared" ref="Q632" si="725">((SUM(C632:F632))/4)*1.04</f>
+        <f t="shared" ref="Q632" si="723">((SUM(C632:F632))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R632">
-        <f t="shared" ref="R632" si="726">((SUM(C634:F634))/4)*1.04</f>
+        <f t="shared" ref="R632" si="724">((SUM(C634:F634))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S632">
-        <f t="shared" ref="S632" si="727">((SUM(C636:F636))/4)*1.04</f>
+        <f t="shared" ref="S632" si="725">((SUM(C636:F636))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T632">
-        <f t="shared" ref="T632" si="728">((SUM(C638:F638))/4)*1.04</f>
+        <f t="shared" ref="T632" si="726">((SUM(C638:F638))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U632">
-        <f t="shared" ref="U632" si="729">((SUM(C640:F640))/4)*1.04</f>
+        <f t="shared" ref="U632" si="727">((SUM(C640:F640))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V632">
-        <f t="shared" ref="V632" si="730">((SUM(C632:F640))/20)*1.04</f>
+        <f t="shared" ref="V632" si="728">((SUM(C632:F640))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W632">
-        <f t="shared" ref="W632" si="731">(SUM(G632:H640))/10</f>
+        <f t="shared" ref="W632" si="729">(SUM(G632:H640))/10</f>
         <v>50</v>
       </c>
       <c r="X632">
-        <f t="shared" ref="X632" si="732">(SUM(I632:I640))/5</f>
+        <f t="shared" ref="X632" si="730">(SUM(I632:I640))/5</f>
         <v>1.4</v>
       </c>
       <c r="Y632">
-        <f t="shared" ref="Y632" si="733">SUM(K632:K640)-Z632</f>
+        <f t="shared" ref="Y632" si="731">SUM(K632:K640)-Z632</f>
         <v>-2</v>
       </c>
       <c r="Z632">
-        <f t="shared" ref="Z632" si="734">SUM(L632:L640)</f>
+        <f t="shared" ref="Z632" si="732">SUM(L632:L640)</f>
         <v>6</v>
       </c>
       <c r="AA632" t="s">
@@ -76555,35 +76554,35 @@
         <v>29</v>
       </c>
       <c r="P641">
-        <f t="shared" ref="P641" si="735">M641*10</f>
+        <f t="shared" ref="P641" si="733">M641*10</f>
         <v>40</v>
       </c>
       <c r="Q641">
-        <f t="shared" ref="Q641" si="736">((SUM(C641:F641))/4)*1.04</f>
+        <f t="shared" ref="Q641" si="734">((SUM(C641:F641))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="R641">
-        <f t="shared" ref="R641" si="737">((SUM(C643:F643))/4)*1.04</f>
+        <f t="shared" ref="R641" si="735">((SUM(C643:F643))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="S641">
-        <f t="shared" ref="S641" si="738">((SUM(C645:F645))/4)*1.04</f>
+        <f t="shared" ref="S641" si="736">((SUM(C645:F645))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="T641">
-        <f t="shared" ref="T641" si="739">((SUM(C647:F647))/4)*1.04</f>
+        <f t="shared" ref="T641" si="737">((SUM(C647:F647))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="U641">
-        <f t="shared" ref="U641" si="740">((SUM(C649:F649))/4)*1.04</f>
+        <f t="shared" ref="U641" si="738">((SUM(C649:F649))/4)*1.04</f>
         <v>0</v>
       </c>
       <c r="V641">
-        <f t="shared" ref="V641" si="741">((SUM(C641:F649))/20)*1.04</f>
+        <f t="shared" ref="V641" si="739">((SUM(C641:F649))/20)*1.04</f>
         <v>0</v>
       </c>
       <c r="W641">
-        <f t="shared" ref="W641" si="742">(SUM(G641:H649))/10</f>
+        <f t="shared" ref="W641" si="740">(SUM(G641:H649))/10</f>
         <v>10.5</v>
       </c>
       <c r="X641">
@@ -76591,11 +76590,11 @@
         <v>1.8</v>
       </c>
       <c r="Y641">
-        <f t="shared" ref="Y641" si="743">SUM(K641:K649)-Z641</f>
+        <f t="shared" ref="Y641" si="741">SUM(K641:K649)-Z641</f>
         <v>6</v>
       </c>
       <c r="Z641">
-        <f t="shared" ref="Z641" si="744">SUM(L641:L649)</f>
+        <f t="shared" ref="Z641" si="742">SUM(L641:L649)</f>
         <v>6</v>
       </c>
       <c r="AA641" t="s">
@@ -77011,7 +77010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>